<commit_message>
add ways to view best signal
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="24">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -90,6 +90,12 @@
   </si>
   <si>
     <t>relu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deepgo flat </t>
+  </si>
+  <si>
+    <t>BertAveLay12Govec</t>
   </si>
 </sst>
 </file>
@@ -506,14 +512,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:T20"/>
+  <dimension ref="A4:T22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
     <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
     <col min="19" max="20" width="0" hidden="1" customWidth="1"/>
@@ -631,603 +638,679 @@
         <v>0.51829999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="28"/>
-      <c r="J7" s="27">
-        <v>0.38469999999999999</v>
-      </c>
-      <c r="K7" s="27">
-        <v>0.77070000000000005</v>
-      </c>
-      <c r="L7" s="27">
-        <v>0.88870000000000005</v>
-      </c>
-      <c r="M7" s="27"/>
-      <c r="N7" s="27"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="27">
-        <v>0.60209999999999997</v>
-      </c>
-      <c r="Q7" s="27">
-        <v>0.75190000000000001</v>
-      </c>
-      <c r="R7" s="27">
-        <v>0.94389999999999996</v>
-      </c>
-      <c r="S7" s="27"/>
-      <c r="T7" s="27"/>
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="3">
+        <v>0.34649999999999997</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.64170000000000005</v>
+      </c>
+      <c r="F7" s="3">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="3">
+        <v>0.39579999999999999</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0.76959999999999995</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0.89039999999999997</v>
+      </c>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="3">
+        <v>0.57369999999999999</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>0.67589999999999995</v>
+      </c>
+      <c r="R7" s="3">
+        <v>0.92869999999999997</v>
+      </c>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
     </row>
     <row r="8" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="25" t="s">
         <v>20</v>
       </c>
       <c r="B8" s="25" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C8" s="26"/>
-      <c r="D8" s="27">
-        <v>0.37890000000000001</v>
-      </c>
-      <c r="E8" s="27">
-        <v>0.71919999999999995</v>
-      </c>
-      <c r="F8" s="27">
-        <v>0.8518</v>
-      </c>
+      <c r="D8" s="27"/>
+      <c r="E8" s="27"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="27"/>
       <c r="H8" s="27"/>
       <c r="I8" s="28"/>
       <c r="J8" s="27">
-        <v>0.38790000000000002</v>
+        <v>0.38469999999999999</v>
       </c>
       <c r="K8" s="27">
-        <v>0.77239999999999998</v>
+        <v>0.77070000000000005</v>
       </c>
       <c r="L8" s="27">
-        <v>0.88349999999999995</v>
+        <v>0.88870000000000005</v>
       </c>
       <c r="M8" s="27"/>
       <c r="N8" s="27"/>
       <c r="O8" s="28"/>
       <c r="P8" s="27">
-        <v>0.59709999999999996</v>
+        <v>0.60209999999999997</v>
       </c>
       <c r="Q8" s="27">
-        <v>0.74370000000000003</v>
+        <v>0.75190000000000001</v>
       </c>
       <c r="R8" s="27">
-        <v>0.93920000000000003</v>
+        <v>0.94389999999999996</v>
       </c>
       <c r="S8" s="27"/>
       <c r="T8" s="27"/>
     </row>
     <row r="9" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="25" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="27"/>
+      <c r="D9" s="27">
+        <v>0.37890000000000001</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0.71919999999999995</v>
+      </c>
+      <c r="F9" s="27">
+        <v>0.8518</v>
+      </c>
       <c r="G9" s="27"/>
       <c r="H9" s="27"/>
       <c r="I9" s="28"/>
       <c r="J9" s="27">
-        <v>0.40579999999999999</v>
+        <v>0.38790000000000002</v>
       </c>
       <c r="K9" s="27">
-        <v>0.79730000000000001</v>
+        <v>0.77239999999999998</v>
       </c>
       <c r="L9" s="27">
-        <v>0.89429999999999998</v>
+        <v>0.88349999999999995</v>
       </c>
       <c r="M9" s="27"/>
       <c r="N9" s="27"/>
       <c r="O9" s="28"/>
       <c r="P9" s="27">
-        <v>0.60599999999999998</v>
+        <v>0.59709999999999996</v>
       </c>
       <c r="Q9" s="27">
-        <v>0.75949999999999995</v>
+        <v>0.74370000000000003</v>
       </c>
       <c r="R9" s="27">
-        <v>0.94520000000000004</v>
+        <v>0.93920000000000003</v>
       </c>
       <c r="S9" s="27"/>
       <c r="T9" s="27"/>
     </row>
-    <row r="10" spans="1:20" s="29" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="6"/>
-      <c r="Q10" s="6"/>
-      <c r="R10" s="6"/>
-      <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C11" s="5" t="s">
+    <row r="10" spans="1:20" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="26"/>
+      <c r="D10" s="27"/>
+      <c r="E10" s="27"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="27"/>
+      <c r="H10" s="27"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="27">
+        <v>0.40579999999999999</v>
+      </c>
+      <c r="K10" s="27">
+        <v>0.79730000000000001</v>
+      </c>
+      <c r="L10" s="27">
+        <v>0.89429999999999998</v>
+      </c>
+      <c r="M10" s="27"/>
+      <c r="N10" s="27"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="27">
+        <v>0.60599999999999998</v>
+      </c>
+      <c r="Q10" s="27">
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="R10" s="27">
+        <v>0.94520000000000004</v>
+      </c>
+      <c r="S10" s="27"/>
+      <c r="T10" s="27"/>
+    </row>
+    <row r="11" spans="1:20" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="25" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11" s="25" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="26"/>
+      <c r="D11" s="27"/>
+      <c r="E11" s="27"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="27"/>
+      <c r="H11" s="27"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="27">
+        <v>0.40679999999999999</v>
+      </c>
+      <c r="K11" s="27">
+        <v>0.79210000000000003</v>
+      </c>
+      <c r="L11" s="27">
+        <v>0.8871</v>
+      </c>
+      <c r="M11" s="27"/>
+      <c r="N11" s="27"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+    </row>
+    <row r="12" spans="1:20" s="29" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="7"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="6"/>
+      <c r="Q12" s="6"/>
+      <c r="R12" s="6"/>
+      <c r="S12" s="6"/>
+      <c r="T12" s="6"/>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C13" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D11" s="6">
+      <c r="D13" s="6">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E13" s="6">
         <v>0.81869999999999998</v>
       </c>
-      <c r="F11" s="6">
+      <c r="F13" s="6">
         <v>0.89700000000000002</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6">
+      <c r="G13" s="6"/>
+      <c r="H13" s="6">
         <v>0.37009999999999998</v>
       </c>
-      <c r="I11" s="7"/>
-      <c r="J11" s="6">
+      <c r="I13" s="7"/>
+      <c r="J13" s="6">
         <v>0.4677</v>
       </c>
-      <c r="K11" s="6">
+      <c r="K13" s="6">
         <v>0.83730000000000004</v>
       </c>
-      <c r="L11" s="6">
+      <c r="L13" s="6">
         <v>0.90600000000000003</v>
       </c>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6">
+      <c r="M13" s="6"/>
+      <c r="N13" s="6">
         <v>0.3614</v>
       </c>
-      <c r="O11" s="7"/>
-      <c r="P11" s="6">
+      <c r="O13" s="7"/>
+      <c r="P13" s="6">
         <v>0.627</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q13" s="6">
         <v>0.878</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R13" s="6">
         <v>0.9647</v>
       </c>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3">
+      <c r="S13" s="3"/>
+      <c r="T13" s="3">
         <v>0.62470000000000003</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C12" s="8" t="s">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D14" s="9">
         <v>42.51</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E14" s="9">
         <v>82.97</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F14" s="9">
         <v>90.27</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="11">
+      <c r="G14" s="10"/>
+      <c r="H14" s="11">
         <v>0.37769999999999998</v>
       </c>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9">
+      <c r="I14" s="9"/>
+      <c r="J14" s="9">
         <v>48.62</v>
       </c>
-      <c r="K12" s="9">
+      <c r="K14" s="9">
         <v>87.25</v>
       </c>
-      <c r="L12" s="9">
+      <c r="L14" s="9">
         <v>93.14</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="11">
+      <c r="M14" s="9"/>
+      <c r="N14" s="11">
         <v>0.40760000000000002</v>
       </c>
-      <c r="O12" s="9"/>
-      <c r="P12" s="9">
+      <c r="O14" s="9"/>
+      <c r="P14" s="9">
         <v>63.77</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="Q14" s="9">
         <v>89.79</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R14" s="9">
         <v>97.1</v>
       </c>
-      <c r="S12" s="8"/>
-      <c r="T12" s="11">
+      <c r="S14" s="8"/>
+      <c r="T14" s="11">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C13" s="12" t="s">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C15" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="13">
+      <c r="D15" s="13">
         <v>0.4365</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E15" s="13">
         <v>0.83460000000000001</v>
       </c>
-      <c r="F13" s="13">
+      <c r="F15" s="13">
         <v>0.90629999999999999</v>
       </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="14">
+      <c r="G15" s="13"/>
+      <c r="H15" s="14">
         <v>0.39729999999999999</v>
       </c>
-      <c r="I13" s="15"/>
-      <c r="J13" s="13">
+      <c r="I15" s="15"/>
+      <c r="J15" s="13">
         <v>0.49740000000000001</v>
       </c>
-      <c r="K13" s="13">
+      <c r="K15" s="13">
         <v>0.87780000000000002</v>
       </c>
-      <c r="L13" s="13">
+      <c r="L15" s="13">
         <v>0.93500000000000005</v>
       </c>
-      <c r="M13" s="13"/>
-      <c r="N13" s="13">
+      <c r="M15" s="13"/>
+      <c r="N15" s="13">
         <v>0.41799999999999998</v>
       </c>
-      <c r="O13" s="15"/>
-      <c r="P13" s="13">
+      <c r="O15" s="15"/>
+      <c r="P15" s="13">
         <v>0.65200000000000002</v>
       </c>
-      <c r="Q13" s="13">
+      <c r="Q15" s="13">
         <v>0.90390000000000004</v>
       </c>
-      <c r="R13" s="13">
+      <c r="R15" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13">
+      <c r="S15" s="13"/>
+      <c r="T15" s="13">
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C14" s="6" t="s">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C16" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D16" s="6">
         <v>0.43480000000000002</v>
       </c>
-      <c r="E14" s="16">
+      <c r="E16" s="16">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F14" s="6">
+      <c r="F16" s="6">
         <v>0.9073</v>
       </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6">
+      <c r="G16" s="6"/>
+      <c r="H16" s="6">
         <v>0.39419999999999999</v>
       </c>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6">
+      <c r="I16" s="6"/>
+      <c r="J16" s="6">
         <v>0.502</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K16" s="6">
         <v>0.88019999999999998</v>
       </c>
-      <c r="L14" s="16">
+      <c r="L16" s="16">
         <v>0.93840000000000001</v>
       </c>
-      <c r="M14" s="6"/>
-      <c r="N14" s="16">
+      <c r="M16" s="6"/>
+      <c r="N16" s="16">
         <v>0.43809999999999999</v>
       </c>
-      <c r="O14" s="6"/>
-      <c r="P14" s="6">
+      <c r="O16" s="6"/>
+      <c r="P16" s="6">
         <v>0.65469999999999995</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q16" s="6">
         <v>0.90480000000000005</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R16" s="6">
         <v>0.97250000000000003</v>
       </c>
-      <c r="S14" s="6"/>
-      <c r="T14" s="6">
+      <c r="S16" s="6"/>
+      <c r="T16" s="6">
         <v>0.66139999999999999</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C15" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D15" s="3">
-        <v>0.43149999999999999</v>
-      </c>
-      <c r="E15" s="3">
-        <v>0.83409999999999995</v>
-      </c>
-      <c r="F15" s="3">
-        <v>0.90590000000000004</v>
-      </c>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3">
-        <v>0.39169999999999999</v>
-      </c>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3">
-        <v>0.49930000000000002</v>
-      </c>
-      <c r="K15" s="3">
-        <v>0.87290000000000001</v>
-      </c>
-      <c r="L15" s="3">
-        <v>0.93389999999999995</v>
-      </c>
-      <c r="M15" s="3"/>
-      <c r="N15" s="3">
-        <v>0.42930000000000001</v>
-      </c>
-      <c r="O15" s="4"/>
-      <c r="P15" s="3">
-        <v>0.65239999999999998</v>
-      </c>
-      <c r="Q15" s="17">
-        <v>0.90569999999999995</v>
-      </c>
-      <c r="R15" s="3">
-        <v>0.97260000000000002</v>
-      </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3">
-        <v>0.65810000000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" s="1">
-        <v>43.45</v>
-      </c>
-      <c r="E16" s="1">
-        <v>83.11</v>
-      </c>
-      <c r="F16" s="1">
-        <v>90.55</v>
-      </c>
-      <c r="G16" s="18"/>
-      <c r="H16" s="3">
-        <v>0.3896</v>
-      </c>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1">
-        <v>49.24</v>
-      </c>
-      <c r="K16" s="1">
-        <v>87.43</v>
-      </c>
-      <c r="L16" s="1">
-        <v>93.52</v>
-      </c>
-      <c r="M16" s="1"/>
-      <c r="N16" s="3">
-        <v>0.42209999999999998</v>
-      </c>
-      <c r="O16" s="1"/>
-      <c r="P16" s="4">
-        <v>65.39</v>
-      </c>
-      <c r="Q16" s="1">
-        <v>90.27</v>
-      </c>
-      <c r="R16" s="4">
-        <v>97.27</v>
-      </c>
-      <c r="S16" s="1"/>
-      <c r="T16" s="3">
-        <v>0.65659999999999996</v>
       </c>
     </row>
     <row r="17" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C17" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D17" s="3">
-        <v>0.42909999999999998</v>
+        <v>0.43149999999999999</v>
       </c>
       <c r="E17" s="3">
-        <v>0.83479999999999999</v>
+        <v>0.83409999999999995</v>
       </c>
       <c r="F17" s="3">
-        <v>0.90569999999999995</v>
+        <v>0.90590000000000004</v>
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3">
-        <v>0.38979999999999998</v>
+        <v>0.39169999999999999</v>
       </c>
       <c r="I17" s="3"/>
       <c r="J17" s="3">
-        <v>0.49349999999999999</v>
-      </c>
-      <c r="K17" s="17">
-        <v>0.87919999999999998</v>
+        <v>0.49930000000000002</v>
+      </c>
+      <c r="K17" s="3">
+        <v>0.87290000000000001</v>
       </c>
       <c r="L17" s="3">
-        <v>0.93830000000000002</v>
+        <v>0.93389999999999995</v>
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="3">
-        <v>0.43259999999999998</v>
-      </c>
-      <c r="O17" s="3"/>
+        <v>0.42930000000000001</v>
+      </c>
+      <c r="O17" s="4"/>
       <c r="P17" s="3">
-        <v>0.6482</v>
-      </c>
-      <c r="Q17" s="3">
-        <v>0.90500000000000003</v>
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="Q17" s="17">
+        <v>0.90569999999999995</v>
       </c>
       <c r="R17" s="3">
-        <v>0.97209999999999996</v>
+        <v>0.97260000000000002</v>
       </c>
       <c r="S17" s="3"/>
       <c r="T17" s="3">
-        <v>0.65500000000000003</v>
+        <v>0.65810000000000002</v>
       </c>
     </row>
     <row r="18" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D18" s="17">
-        <v>0.43919999999999998</v>
-      </c>
-      <c r="E18" s="17">
-        <v>0.83489999999999998</v>
-      </c>
-      <c r="F18" s="17">
-        <v>0.90769999999999995</v>
-      </c>
-      <c r="G18" s="19"/>
+        <v>13</v>
+      </c>
+      <c r="D18" s="1">
+        <v>43.45</v>
+      </c>
+      <c r="E18" s="1">
+        <v>83.11</v>
+      </c>
+      <c r="F18" s="1">
+        <v>90.55</v>
+      </c>
+      <c r="G18" s="18"/>
       <c r="H18" s="3">
-        <v>0.39300000000000002</v>
+        <v>0.3896</v>
       </c>
       <c r="I18" s="1"/>
-      <c r="J18" s="17">
-        <v>0.503</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.87680000000000002</v>
-      </c>
-      <c r="L18" s="3">
-        <v>0.93659999999999999</v>
-      </c>
-      <c r="M18" s="3"/>
+      <c r="J18" s="1">
+        <v>49.24</v>
+      </c>
+      <c r="K18" s="1">
+        <v>87.43</v>
+      </c>
+      <c r="L18" s="1">
+        <v>93.52</v>
+      </c>
+      <c r="M18" s="1"/>
       <c r="N18" s="3">
-        <v>0.43430000000000002</v>
+        <v>0.42209999999999998</v>
       </c>
       <c r="O18" s="1"/>
-      <c r="P18" s="17">
-        <v>0.6583</v>
-      </c>
-      <c r="Q18" s="3">
-        <v>0.90510000000000002</v>
-      </c>
-      <c r="R18" s="17">
-        <v>0.97299999999999998</v>
+      <c r="P18" s="4">
+        <v>65.39</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>90.27</v>
+      </c>
+      <c r="R18" s="4">
+        <v>97.27</v>
       </c>
       <c r="S18" s="1"/>
-      <c r="T18" s="17">
-        <v>0.66559999999999997</v>
+      <c r="T18" s="3">
+        <v>0.65659999999999996</v>
       </c>
     </row>
     <row r="19" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <v>42.83</v>
-      </c>
-      <c r="E19" s="4">
-        <v>83.36</v>
-      </c>
-      <c r="F19" s="4">
-        <v>90.7</v>
-      </c>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4">
-        <v>39.229999999999997</v>
-      </c>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4">
-        <v>49.84</v>
-      </c>
-      <c r="K19" s="4">
-        <v>87.5</v>
-      </c>
-      <c r="L19" s="4">
-        <v>93.41</v>
-      </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="4">
-        <v>42.63</v>
-      </c>
-      <c r="O19" s="4"/>
-      <c r="P19" s="4">
-        <v>65.8</v>
-      </c>
-      <c r="Q19" s="4">
-        <v>90.5</v>
-      </c>
-      <c r="R19" s="4">
-        <v>97.3</v>
-      </c>
-      <c r="S19" s="4"/>
-      <c r="T19" s="4">
-        <v>66.290000000000006</v>
+        <v>14</v>
+      </c>
+      <c r="D19" s="3">
+        <v>0.42909999999999998</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="F19" s="3">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="K19" s="17">
+        <v>0.87919999999999998</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0.93830000000000002</v>
+      </c>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3">
+        <v>0.43259999999999998</v>
+      </c>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3">
+        <v>0.6482</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="R19" s="3">
+        <v>0.97209999999999996</v>
+      </c>
+      <c r="S19" s="3"/>
+      <c r="T19" s="3">
+        <v>0.65500000000000003</v>
       </c>
     </row>
     <row r="20" spans="3:20" x14ac:dyDescent="0.25">
       <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="17">
+        <v>0.43919999999999998</v>
+      </c>
+      <c r="E20" s="17">
+        <v>0.83489999999999998</v>
+      </c>
+      <c r="F20" s="17">
+        <v>0.90769999999999995</v>
+      </c>
+      <c r="G20" s="19"/>
+      <c r="H20" s="3">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="J20" s="17">
+        <v>0.503</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0.93659999999999999</v>
+      </c>
+      <c r="M20" s="3"/>
+      <c r="N20" s="3">
+        <v>0.43430000000000002</v>
+      </c>
+      <c r="O20" s="1"/>
+      <c r="P20" s="17">
+        <v>0.6583</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>0.90510000000000002</v>
+      </c>
+      <c r="R20" s="17">
+        <v>0.97299999999999998</v>
+      </c>
+      <c r="S20" s="1"/>
+      <c r="T20" s="17">
+        <v>0.66559999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C21" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="4">
+        <v>42.83</v>
+      </c>
+      <c r="E21" s="4">
+        <v>83.36</v>
+      </c>
+      <c r="F21" s="4">
+        <v>90.7</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4">
+        <v>39.229999999999997</v>
+      </c>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4">
+        <v>49.84</v>
+      </c>
+      <c r="K21" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="L21" s="4">
+        <v>93.41</v>
+      </c>
+      <c r="M21" s="4"/>
+      <c r="N21" s="4">
+        <v>42.63</v>
+      </c>
+      <c r="O21" s="4"/>
+      <c r="P21" s="4">
+        <v>65.8</v>
+      </c>
+      <c r="Q21" s="4">
+        <v>90.5</v>
+      </c>
+      <c r="R21" s="4">
+        <v>97.3</v>
+      </c>
+      <c r="S21" s="4"/>
+      <c r="T21" s="4">
+        <v>66.290000000000006</v>
+      </c>
+    </row>
+    <row r="22" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D20" s="20">
+      <c r="D22" s="20">
         <v>0.4335</v>
       </c>
-      <c r="E20" s="20">
+      <c r="E22" s="20">
         <v>0.83350000000000002</v>
       </c>
-      <c r="F20" s="20">
+      <c r="F22" s="20">
         <v>0.90259999999999996</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="20">
+      <c r="G22" s="21"/>
+      <c r="H22" s="20">
         <v>0.38850000000000001</v>
       </c>
-      <c r="I20" s="22"/>
-      <c r="J20" s="20">
+      <c r="I22" s="22"/>
+      <c r="J22" s="20">
         <v>0.49130000000000001</v>
       </c>
-      <c r="K20" s="20">
+      <c r="K22" s="20">
         <v>0.87970000000000004</v>
       </c>
-      <c r="L20" s="20">
+      <c r="L22" s="20">
         <v>0.93069999999999997</v>
       </c>
-      <c r="M20" s="20"/>
-      <c r="N20" s="20">
+      <c r="M22" s="20"/>
+      <c r="N22" s="20">
         <v>0.41320000000000001</v>
       </c>
-      <c r="O20" s="22"/>
-      <c r="P20" s="20">
+      <c r="O22" s="22"/>
+      <c r="P22" s="20">
         <v>0.65659999999999996</v>
       </c>
-      <c r="Q20" s="20">
+      <c r="Q22" s="20">
         <v>0.90269999999999995</v>
       </c>
-      <c r="R20" s="20">
+      <c r="R22" s="20">
         <v>0.97240000000000004</v>
       </c>
-      <c r="S20" s="23"/>
-      <c r="T20" s="24">
+      <c r="S22" s="23"/>
+      <c r="T22" s="24">
         <v>0.66069999999999995</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add some examples on torch gather
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="38">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>58.13% *AsIsE768I768H6L8Drop0.1</t>
+  </si>
+  <si>
+    <t>2embMutPosPpiGeluH1L12BertLabDrop0.1</t>
+  </si>
+  <si>
+    <t>2embPpiGeluE768H1L12I768PretrainLabelDrop0.1</t>
+  </si>
+  <si>
+    <t>2embPpiGeluE768H6L8I768PretrainLabelDrop0.1</t>
   </si>
 </sst>
 </file>
@@ -576,10 +585,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:T40"/>
+  <dimension ref="A4:T48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1167,35 +1176,35 @@
       <c r="S20" s="26"/>
       <c r="T20" s="26"/>
     </row>
-    <row r="21" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
-        <v>32</v>
-      </c>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="7"/>
-      <c r="J21" s="6">
-        <v>0.50919999999999999</v>
-      </c>
-      <c r="K21" s="6">
-        <v>0.8871</v>
-      </c>
-      <c r="L21" s="6">
-        <v>0.93799999999999994</v>
-      </c>
-      <c r="M21" s="6"/>
-      <c r="N21" s="6"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="6"/>
-      <c r="Q21" s="6"/>
-      <c r="R21" s="6"/>
-      <c r="S21" s="6"/>
-      <c r="T21" s="6"/>
+        <v>37</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
+      <c r="I21" s="27"/>
+      <c r="J21" s="26">
+        <v>0.50470000000000004</v>
+      </c>
+      <c r="K21" s="26">
+        <v>0.88619999999999999</v>
+      </c>
+      <c r="L21" s="26">
+        <v>0.94006000000000001</v>
+      </c>
+      <c r="M21" s="26"/>
+      <c r="N21" s="26"/>
+      <c r="O21" s="27"/>
+      <c r="P21" s="26"/>
+      <c r="Q21" s="26"/>
+      <c r="R21" s="26"/>
+      <c r="S21" s="26"/>
+      <c r="T21" s="26"/>
     </row>
     <row r="22" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
@@ -1219,6 +1228,9 @@
       <c r="T22" s="6"/>
     </row>
     <row r="23" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
+        <v>32</v>
+      </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="6"/>
@@ -1227,9 +1239,15 @@
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
       <c r="I23" s="7"/>
-      <c r="J23" s="6"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="6"/>
+      <c r="J23" s="6">
+        <v>0.50919999999999999</v>
+      </c>
+      <c r="K23" s="6">
+        <v>0.8871</v>
+      </c>
+      <c r="L23" s="6">
+        <v>0.93799999999999994</v>
+      </c>
       <c r="M23" s="6"/>
       <c r="N23" s="6"/>
       <c r="O23" s="7"/>
@@ -1240,6 +1258,7 @@
       <c r="T23" s="6"/>
     </row>
     <row r="24" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="6"/>
       <c r="E24" s="6"/>
@@ -1259,478 +1278,669 @@
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C25" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="6">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="E25" s="6">
-        <v>0.81869999999999998</v>
-      </c>
-      <c r="F25" s="6">
-        <v>0.89700000000000002</v>
-      </c>
+    <row r="25" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="6"/>
-      <c r="H25" s="6">
-        <v>0.37009999999999998</v>
-      </c>
+      <c r="H25" s="6"/>
       <c r="I25" s="7"/>
       <c r="J25" s="6">
+        <v>0.49408999999999997</v>
+      </c>
+      <c r="K25" s="6">
+        <v>0.88570000000000004</v>
+      </c>
+      <c r="L25" s="6">
+        <v>0.93967000000000001</v>
+      </c>
+      <c r="M25" s="6"/>
+      <c r="N25" s="6"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="6"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+      <c r="T25" s="6"/>
+    </row>
+    <row r="26" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="6"/>
+      <c r="M26" s="6"/>
+      <c r="N26" s="6"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="6"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+      <c r="T26" s="6"/>
+    </row>
+    <row r="27" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="6"/>
+      <c r="M27" s="6"/>
+      <c r="N27" s="6"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="6"/>
+      <c r="Q27" s="6"/>
+      <c r="R27" s="6"/>
+      <c r="S27" s="6"/>
+      <c r="T27" s="6"/>
+    </row>
+    <row r="28" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" s="5"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="6">
+        <v>0.499</v>
+      </c>
+      <c r="K28" s="6">
+        <v>0.88307999999999998</v>
+      </c>
+      <c r="L28" s="6">
+        <v>0.93676999999999999</v>
+      </c>
+      <c r="M28" s="6"/>
+      <c r="N28" s="6"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="6"/>
+      <c r="Q28" s="6"/>
+      <c r="R28" s="6"/>
+      <c r="S28" s="6"/>
+      <c r="T28" s="6"/>
+    </row>
+    <row r="29" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B29" s="5"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="6"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="6"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+    </row>
+    <row r="30" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="6"/>
+      <c r="M30" s="6"/>
+      <c r="N30" s="6"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="6"/>
+      <c r="Q30" s="6"/>
+      <c r="R30" s="6"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+    </row>
+    <row r="31" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="5"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
+      <c r="M31" s="6"/>
+      <c r="N31" s="6"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="6"/>
+      <c r="T31" s="6"/>
+    </row>
+    <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="7"/>
+      <c r="J32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="6"/>
+      <c r="M32" s="6"/>
+      <c r="N32" s="6"/>
+      <c r="O32" s="7"/>
+      <c r="P32" s="6"/>
+      <c r="Q32" s="6"/>
+      <c r="R32" s="6"/>
+      <c r="S32" s="6"/>
+      <c r="T32" s="6"/>
+    </row>
+    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C33" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.81869999999999998</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6">
+        <v>0.37009999999999998</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="6">
         <v>0.4677</v>
       </c>
-      <c r="K25" s="6">
+      <c r="K33" s="6">
         <v>0.83730000000000004</v>
       </c>
-      <c r="L25" s="6">
+      <c r="L33" s="6">
         <v>0.90600000000000003</v>
       </c>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6">
+      <c r="M33" s="6"/>
+      <c r="N33" s="6">
         <v>0.3614</v>
       </c>
-      <c r="O25" s="7"/>
-      <c r="P25" s="6">
+      <c r="O33" s="7"/>
+      <c r="P33" s="6">
         <v>0.627</v>
       </c>
-      <c r="Q25" s="6">
+      <c r="Q33" s="6">
         <v>0.878</v>
       </c>
-      <c r="R25" s="6">
+      <c r="R33" s="6">
         <v>0.9647</v>
       </c>
-      <c r="S25" s="3"/>
-      <c r="T25" s="3">
+      <c r="S33" s="3"/>
+      <c r="T33" s="3">
         <v>0.62470000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C26" s="8" t="s">
+    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D34" s="9">
         <v>42.51</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E34" s="9">
         <v>82.97</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F34" s="9">
         <v>90.27</v>
       </c>
-      <c r="G26" s="10"/>
-      <c r="H26" s="11">
+      <c r="G34" s="10"/>
+      <c r="H34" s="11">
         <v>0.37769999999999998</v>
       </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9">
+      <c r="I34" s="9"/>
+      <c r="J34" s="9">
         <v>48.62</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K34" s="9">
         <v>87.25</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L34" s="9">
         <v>93.14</v>
       </c>
-      <c r="M26" s="9"/>
-      <c r="N26" s="11">
+      <c r="M34" s="9"/>
+      <c r="N34" s="11">
         <v>0.40760000000000002</v>
       </c>
-      <c r="O26" s="9"/>
-      <c r="P26" s="9">
+      <c r="O34" s="9"/>
+      <c r="P34" s="9">
         <v>63.77</v>
       </c>
-      <c r="Q26" s="9">
+      <c r="Q34" s="9">
         <v>89.79</v>
       </c>
-      <c r="R26" s="9">
+      <c r="R34" s="9">
         <v>97.1</v>
       </c>
-      <c r="S26" s="8"/>
-      <c r="T26" s="11">
+      <c r="S34" s="8"/>
+      <c r="T34" s="11">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C27" s="12" t="s">
+    <row r="35" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C35" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D27" s="13">
+      <c r="D35" s="13">
         <v>0.4365</v>
       </c>
-      <c r="E27" s="13">
+      <c r="E35" s="13">
         <v>0.83460000000000001</v>
       </c>
-      <c r="F27" s="13">
+      <c r="F35" s="13">
         <v>0.90629999999999999</v>
       </c>
-      <c r="G27" s="13"/>
-      <c r="H27" s="14">
+      <c r="G35" s="13"/>
+      <c r="H35" s="14">
         <v>0.39729999999999999</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="13">
+      <c r="I35" s="15"/>
+      <c r="J35" s="13">
         <v>0.49740000000000001</v>
       </c>
-      <c r="K27" s="13">
+      <c r="K35" s="13">
         <v>0.87780000000000002</v>
       </c>
-      <c r="L27" s="13">
+      <c r="L35" s="13">
         <v>0.93500000000000005</v>
       </c>
-      <c r="M27" s="13"/>
-      <c r="N27" s="13">
+      <c r="M35" s="13"/>
+      <c r="N35" s="13">
         <v>0.41799999999999998</v>
       </c>
-      <c r="O27" s="15"/>
-      <c r="P27" s="13">
+      <c r="O35" s="15"/>
+      <c r="P35" s="13">
         <v>0.65200000000000002</v>
       </c>
-      <c r="Q27" s="13">
+      <c r="Q35" s="13">
         <v>0.90390000000000004</v>
       </c>
-      <c r="R27" s="13">
+      <c r="R35" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13">
+      <c r="S35" s="13"/>
+      <c r="T35" s="13">
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C28" s="6" t="s">
+    <row r="36" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D36" s="6">
         <v>0.43480000000000002</v>
       </c>
-      <c r="E28" s="16">
+      <c r="E36" s="16">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F28" s="6">
+      <c r="F36" s="6">
         <v>0.9073</v>
       </c>
-      <c r="G28" s="6"/>
-      <c r="H28" s="6">
+      <c r="G36" s="6"/>
+      <c r="H36" s="6">
         <v>0.39419999999999999</v>
       </c>
-      <c r="I28" s="6"/>
-      <c r="J28" s="6">
+      <c r="I36" s="6"/>
+      <c r="J36" s="6">
         <v>0.502</v>
       </c>
-      <c r="K28" s="6">
+      <c r="K36" s="6">
         <v>0.88019999999999998</v>
       </c>
-      <c r="L28" s="16">
+      <c r="L36" s="16">
         <v>0.93840000000000001</v>
       </c>
-      <c r="M28" s="6"/>
-      <c r="N28" s="16">
+      <c r="M36" s="6"/>
+      <c r="N36" s="16">
         <v>0.43809999999999999</v>
       </c>
-      <c r="O28" s="6"/>
-      <c r="P28" s="6">
+      <c r="O36" s="6"/>
+      <c r="P36" s="6">
         <v>0.65469999999999995</v>
       </c>
-      <c r="Q28" s="6">
+      <c r="Q36" s="6">
         <v>0.90480000000000005</v>
       </c>
-      <c r="R28" s="6">
+      <c r="R36" s="6">
         <v>0.97250000000000003</v>
       </c>
-      <c r="S28" s="6"/>
-      <c r="T28" s="6">
+      <c r="S36" s="6"/>
+      <c r="T36" s="6">
         <v>0.66139999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C29" s="1" t="s">
+    <row r="37" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C37" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="3">
+      <c r="D37" s="3">
         <v>0.43149999999999999</v>
       </c>
-      <c r="E29" s="3">
+      <c r="E37" s="3">
         <v>0.83409999999999995</v>
       </c>
-      <c r="F29" s="3">
+      <c r="F37" s="3">
         <v>0.90590000000000004</v>
       </c>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3">
+      <c r="G37" s="3"/>
+      <c r="H37" s="3">
         <v>0.39169999999999999</v>
       </c>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3">
+      <c r="I37" s="3"/>
+      <c r="J37" s="3">
         <v>0.49930000000000002</v>
       </c>
-      <c r="K29" s="3">
+      <c r="K37" s="3">
         <v>0.87290000000000001</v>
       </c>
-      <c r="L29" s="3">
+      <c r="L37" s="3">
         <v>0.93389999999999995</v>
       </c>
-      <c r="M29" s="3"/>
-      <c r="N29" s="3">
+      <c r="M37" s="3"/>
+      <c r="N37" s="3">
         <v>0.42930000000000001</v>
       </c>
-      <c r="O29" s="4"/>
-      <c r="P29" s="3">
+      <c r="O37" s="4"/>
+      <c r="P37" s="3">
         <v>0.65239999999999998</v>
       </c>
-      <c r="Q29" s="17">
+      <c r="Q37" s="17">
         <v>0.90569999999999995</v>
       </c>
-      <c r="R29" s="3">
+      <c r="R37" s="3">
         <v>0.97260000000000002</v>
       </c>
-      <c r="S29" s="3"/>
-      <c r="T29" s="3">
+      <c r="S37" s="3"/>
+      <c r="T37" s="3">
         <v>0.65810000000000002</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C30" s="1" t="s">
+    <row r="38" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C38" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D38" s="1">
         <v>43.45</v>
       </c>
-      <c r="E30" s="1">
+      <c r="E38" s="1">
         <v>83.11</v>
       </c>
-      <c r="F30" s="1">
+      <c r="F38" s="1">
         <v>90.55</v>
       </c>
-      <c r="G30" s="18"/>
-      <c r="H30" s="3">
+      <c r="G38" s="18"/>
+      <c r="H38" s="3">
         <v>0.3896</v>
       </c>
-      <c r="I30" s="1"/>
-      <c r="J30" s="1">
+      <c r="I38" s="1"/>
+      <c r="J38" s="1">
         <v>49.24</v>
       </c>
-      <c r="K30" s="1">
+      <c r="K38" s="1">
         <v>87.43</v>
       </c>
-      <c r="L30" s="1">
+      <c r="L38" s="1">
         <v>93.52</v>
       </c>
-      <c r="M30" s="1"/>
-      <c r="N30" s="3">
+      <c r="M38" s="1"/>
+      <c r="N38" s="3">
         <v>0.42209999999999998</v>
       </c>
-      <c r="O30" s="1"/>
-      <c r="P30" s="4">
+      <c r="O38" s="1"/>
+      <c r="P38" s="4">
         <v>65.39</v>
       </c>
-      <c r="Q30" s="1">
+      <c r="Q38" s="1">
         <v>90.27</v>
       </c>
-      <c r="R30" s="4">
+      <c r="R38" s="4">
         <v>97.27</v>
       </c>
-      <c r="S30" s="1"/>
-      <c r="T30" s="3">
+      <c r="S38" s="1"/>
+      <c r="T38" s="3">
         <v>0.65659999999999996</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C31" s="1" t="s">
+    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="3">
+      <c r="D39" s="3">
         <v>0.42909999999999998</v>
       </c>
-      <c r="E31" s="3">
+      <c r="E39" s="3">
         <v>0.83479999999999999</v>
       </c>
-      <c r="F31" s="3">
+      <c r="F39" s="3">
         <v>0.90569999999999995</v>
       </c>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3">
+      <c r="G39" s="3"/>
+      <c r="H39" s="3">
         <v>0.38979999999999998</v>
       </c>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3">
+      <c r="I39" s="3"/>
+      <c r="J39" s="3">
         <v>0.49349999999999999</v>
       </c>
-      <c r="K31" s="17">
+      <c r="K39" s="17">
         <v>0.87919999999999998</v>
       </c>
-      <c r="L31" s="3">
+      <c r="L39" s="3">
         <v>0.93830000000000002</v>
       </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3">
+      <c r="M39" s="3"/>
+      <c r="N39" s="3">
         <v>0.43259999999999998</v>
       </c>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3">
+      <c r="O39" s="3"/>
+      <c r="P39" s="3">
         <v>0.6482</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q39" s="3">
         <v>0.90500000000000003</v>
       </c>
-      <c r="R31" s="3">
+      <c r="R39" s="3">
         <v>0.97209999999999996</v>
       </c>
-      <c r="S31" s="3"/>
-      <c r="T31" s="3">
+      <c r="S39" s="3"/>
+      <c r="T39" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C32" s="32" t="s">
+    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C40" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D32" s="33">
+      <c r="D40" s="33">
         <v>0.43919999999999998</v>
       </c>
-      <c r="E32" s="33">
+      <c r="E40" s="33">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F32" s="33">
+      <c r="F40" s="33">
         <v>0.90769999999999995</v>
       </c>
-      <c r="G32" s="34"/>
-      <c r="H32" s="35">
+      <c r="G40" s="34"/>
+      <c r="H40" s="35">
         <v>0.39300000000000002</v>
       </c>
-      <c r="I32" s="32"/>
-      <c r="J32" s="33">
+      <c r="I40" s="32"/>
+      <c r="J40" s="33">
         <v>0.503</v>
       </c>
-      <c r="K32" s="35">
+      <c r="K40" s="35">
         <v>0.87680000000000002</v>
       </c>
-      <c r="L32" s="35">
+      <c r="L40" s="35">
         <v>0.93659999999999999</v>
       </c>
-      <c r="M32" s="35"/>
-      <c r="N32" s="35">
+      <c r="M40" s="35"/>
+      <c r="N40" s="35">
         <v>0.43430000000000002</v>
       </c>
-      <c r="O32" s="32"/>
-      <c r="P32" s="33">
+      <c r="O40" s="32"/>
+      <c r="P40" s="33">
         <v>0.6583</v>
       </c>
-      <c r="Q32" s="35">
+      <c r="Q40" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="R32" s="33">
+      <c r="R40" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="S32" s="1"/>
-      <c r="T32" s="17">
+      <c r="S40" s="1"/>
+      <c r="T40" s="17">
         <v>0.66559999999999997</v>
       </c>
     </row>
-    <row r="33" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C33" s="1" t="s">
+    <row r="41" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C41" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D41" s="4">
         <v>42.83</v>
       </c>
-      <c r="E33" s="4">
+      <c r="E41" s="4">
         <v>83.36</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F41" s="4">
         <v>90.7</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4">
+      <c r="G41" s="4"/>
+      <c r="H41" s="4">
         <v>39.229999999999997</v>
       </c>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4">
+      <c r="I41" s="4"/>
+      <c r="J41" s="4">
         <v>49.84</v>
       </c>
-      <c r="K33" s="4">
+      <c r="K41" s="4">
         <v>87.5</v>
       </c>
-      <c r="L33" s="4">
+      <c r="L41" s="4">
         <v>93.41</v>
       </c>
-      <c r="M33" s="4"/>
-      <c r="N33" s="4">
+      <c r="M41" s="4"/>
+      <c r="N41" s="4">
         <v>42.63</v>
       </c>
-      <c r="O33" s="4"/>
-      <c r="P33" s="4">
+      <c r="O41" s="4"/>
+      <c r="P41" s="4">
         <v>65.8</v>
       </c>
-      <c r="Q33" s="4">
+      <c r="Q41" s="4">
         <v>90.5</v>
       </c>
-      <c r="R33" s="4">
+      <c r="R41" s="4">
         <v>97.3</v>
       </c>
-      <c r="S33" s="4"/>
-      <c r="T33" s="4">
+      <c r="S41" s="4"/>
+      <c r="T41" s="4">
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="34" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C34" s="1" t="s">
+    <row r="42" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C42" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D42" s="19">
         <v>0.4335</v>
       </c>
-      <c r="E34" s="19">
+      <c r="E42" s="19">
         <v>0.83350000000000002</v>
       </c>
-      <c r="F34" s="19">
+      <c r="F42" s="19">
         <v>0.90259999999999996</v>
       </c>
-      <c r="G34" s="20"/>
-      <c r="H34" s="19">
+      <c r="G42" s="20"/>
+      <c r="H42" s="19">
         <v>0.38850000000000001</v>
       </c>
-      <c r="I34" s="21"/>
-      <c r="J34" s="19">
+      <c r="I42" s="21"/>
+      <c r="J42" s="19">
         <v>0.49130000000000001</v>
       </c>
-      <c r="K34" s="19">
+      <c r="K42" s="19">
         <v>0.87970000000000004</v>
       </c>
-      <c r="L34" s="19">
+      <c r="L42" s="19">
         <v>0.93069999999999997</v>
       </c>
-      <c r="M34" s="19"/>
-      <c r="N34" s="19">
+      <c r="M42" s="19"/>
+      <c r="N42" s="19">
         <v>0.41320000000000001</v>
       </c>
-      <c r="O34" s="21"/>
-      <c r="P34" s="19">
+      <c r="O42" s="21"/>
+      <c r="P42" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="Q34" s="19">
+      <c r="Q42" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="R34" s="19">
+      <c r="R42" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="S34" s="22"/>
-      <c r="T34" s="23">
+      <c r="S42" s="22"/>
+      <c r="T42" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="39" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C39" t="s">
+    <row r="47" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C47" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C40" t="s">
+    <row r="48" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C48" t="s">
         <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
check aa len and input prot label
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dat\Documents\GitHub\BertGOAnnotation\SeeAttention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\BertGOAnnotation\SeeAttention\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9045" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="9045"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="99">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -314,12 +314,21 @@
   </si>
   <si>
     <t>Q08873</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE768H1L12I768PreLabSet0_1stRun</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE768H1L12I768PreLabSet0_1stRunDrop0.2</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE768H4L12I768PreLabSet0_1stRun</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
@@ -776,10 +785,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:T50"/>
+  <dimension ref="A4:T55"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,6 +1581,9 @@
       <c r="T28" s="6"/>
     </row>
     <row r="29" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="28" t="s">
+        <v>96</v>
+      </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="6"/>
@@ -1580,9 +1592,15 @@
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
       <c r="I29" s="7"/>
-      <c r="J29" s="6"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="6"/>
+      <c r="J29" s="6">
+        <v>0.51929999999999998</v>
+      </c>
+      <c r="K29" s="6">
+        <v>0.89648000000000005</v>
+      </c>
+      <c r="L29" s="6">
+        <v>0.94398000000000004</v>
+      </c>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
       <c r="O29" s="7"/>
@@ -1594,7 +1612,7 @@
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>35</v>
+        <v>97</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
@@ -1604,9 +1622,15 @@
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="7"/>
-      <c r="J30" s="6"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="6"/>
+      <c r="J30" s="6">
+        <v>0.52579759999999998</v>
+      </c>
+      <c r="K30" s="6">
+        <v>0.8861</v>
+      </c>
+      <c r="L30" s="6">
+        <v>0.93849190000000005</v>
+      </c>
       <c r="M30" s="6"/>
       <c r="N30" s="6"/>
       <c r="O30" s="7"/>
@@ -1618,7 +1642,7 @@
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>35</v>
+        <v>98</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1628,9 +1652,15 @@
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="7"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
+      <c r="J31" s="6">
+        <v>0.51198109999999997</v>
+      </c>
+      <c r="K31" s="6">
+        <v>0.89452399999999999</v>
+      </c>
+      <c r="L31" s="6">
+        <v>0.94331580000000004</v>
+      </c>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
       <c r="O31" s="7"/>
@@ -1641,9 +1671,6 @@
       <c r="T31" s="6"/>
     </row>
     <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
       <c r="D32" s="6"/>
@@ -1664,7 +1691,7 @@
       <c r="S32" s="6"/>
       <c r="T32" s="6"/>
     </row>
-    <row r="33" spans="2:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -1685,7 +1712,8 @@
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
     </row>
-    <row r="34" spans="2:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
@@ -1705,473 +1733,586 @@
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
     </row>
-    <row r="35" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C35" s="5" t="s">
+    <row r="35" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="6"/>
+      <c r="K35" s="6"/>
+      <c r="L35" s="6"/>
+      <c r="M35" s="6"/>
+      <c r="N35" s="6"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="6"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="6"/>
+      <c r="T35" s="6"/>
+    </row>
+    <row r="36" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
+      <c r="L36" s="6"/>
+      <c r="M36" s="6"/>
+      <c r="N36" s="6"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="6"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+      <c r="S36" s="6"/>
+      <c r="T36" s="6"/>
+    </row>
+    <row r="37" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="7"/>
+      <c r="J37" s="6"/>
+      <c r="K37" s="6"/>
+      <c r="L37" s="6"/>
+      <c r="M37" s="6"/>
+      <c r="N37" s="6"/>
+      <c r="O37" s="7"/>
+      <c r="P37" s="6"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+      <c r="S37" s="6"/>
+      <c r="T37" s="6"/>
+    </row>
+    <row r="38" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="7"/>
+      <c r="J38" s="6"/>
+      <c r="K38" s="6"/>
+      <c r="L38" s="6"/>
+      <c r="M38" s="6"/>
+      <c r="N38" s="6"/>
+      <c r="O38" s="7"/>
+      <c r="P38" s="6"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+      <c r="S38" s="6"/>
+      <c r="T38" s="6"/>
+    </row>
+    <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="7"/>
+      <c r="J39" s="6"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
+      <c r="M39" s="6"/>
+      <c r="N39" s="6"/>
+      <c r="O39" s="7"/>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+      <c r="S39" s="6"/>
+      <c r="T39" s="6"/>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C40" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D40" s="6">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E35" s="6">
+      <c r="E40" s="6">
         <v>0.81869999999999998</v>
       </c>
-      <c r="F35" s="6">
+      <c r="F40" s="6">
         <v>0.89700000000000002</v>
       </c>
-      <c r="G35" s="6"/>
-      <c r="H35" s="6">
+      <c r="G40" s="6"/>
+      <c r="H40" s="6">
         <v>0.37009999999999998</v>
       </c>
-      <c r="I35" s="7"/>
-      <c r="J35" s="6">
+      <c r="I40" s="7"/>
+      <c r="J40" s="6">
         <v>0.4677</v>
       </c>
-      <c r="K35" s="6">
+      <c r="K40" s="6">
         <v>0.83730000000000004</v>
       </c>
-      <c r="L35" s="6">
+      <c r="L40" s="6">
         <v>0.90600000000000003</v>
       </c>
-      <c r="M35" s="6"/>
-      <c r="N35" s="6">
+      <c r="M40" s="6"/>
+      <c r="N40" s="6">
         <v>0.3614</v>
       </c>
-      <c r="O35" s="7"/>
-      <c r="P35" s="6">
+      <c r="O40" s="7"/>
+      <c r="P40" s="6">
         <v>0.627</v>
       </c>
-      <c r="Q35" s="6">
+      <c r="Q40" s="6">
         <v>0.878</v>
       </c>
-      <c r="R35" s="6">
+      <c r="R40" s="6">
         <v>0.9647</v>
       </c>
-      <c r="S35" s="3"/>
-      <c r="T35" s="3">
+      <c r="S40" s="3"/>
+      <c r="T40" s="3">
         <v>0.62470000000000003</v>
       </c>
     </row>
-    <row r="36" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C36" s="8" t="s">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C41" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D36" s="9">
+      <c r="D41" s="9">
         <v>42.51</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E41" s="9">
         <v>82.97</v>
       </c>
-      <c r="F36" s="9">
+      <c r="F41" s="9">
         <v>90.27</v>
       </c>
-      <c r="G36" s="10"/>
-      <c r="H36" s="11">
+      <c r="G41" s="10"/>
+      <c r="H41" s="11">
         <v>0.37769999999999998</v>
       </c>
-      <c r="I36" s="9"/>
-      <c r="J36" s="9">
+      <c r="I41" s="9"/>
+      <c r="J41" s="9">
         <v>48.62</v>
       </c>
-      <c r="K36" s="9">
+      <c r="K41" s="9">
         <v>87.25</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L41" s="9">
         <v>93.14</v>
       </c>
-      <c r="M36" s="9"/>
-      <c r="N36" s="11">
+      <c r="M41" s="9"/>
+      <c r="N41" s="11">
         <v>0.40760000000000002</v>
       </c>
-      <c r="O36" s="9"/>
-      <c r="P36" s="9">
+      <c r="O41" s="9"/>
+      <c r="P41" s="9">
         <v>63.77</v>
       </c>
-      <c r="Q36" s="9">
+      <c r="Q41" s="9">
         <v>89.79</v>
       </c>
-      <c r="R36" s="9">
+      <c r="R41" s="9">
         <v>97.1</v>
       </c>
-      <c r="S36" s="8"/>
-      <c r="T36" s="11">
+      <c r="S41" s="8"/>
+      <c r="T41" s="11">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="37" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C37" s="12" t="s">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C42" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D37" s="13">
+      <c r="D42" s="13">
         <v>0.4365</v>
       </c>
-      <c r="E37" s="13">
+      <c r="E42" s="13">
         <v>0.83460000000000001</v>
       </c>
-      <c r="F37" s="13">
+      <c r="F42" s="13">
         <v>0.90629999999999999</v>
       </c>
-      <c r="G37" s="13"/>
-      <c r="H37" s="14">
+      <c r="G42" s="13"/>
+      <c r="H42" s="14">
         <v>0.39729999999999999</v>
       </c>
-      <c r="I37" s="15"/>
-      <c r="J37" s="13">
+      <c r="I42" s="15"/>
+      <c r="J42" s="13">
         <v>0.49740000000000001</v>
       </c>
-      <c r="K37" s="13">
+      <c r="K42" s="13">
         <v>0.87780000000000002</v>
       </c>
-      <c r="L37" s="13">
+      <c r="L42" s="13">
         <v>0.93500000000000005</v>
       </c>
-      <c r="M37" s="13"/>
-      <c r="N37" s="13">
+      <c r="M42" s="13"/>
+      <c r="N42" s="13">
         <v>0.41799999999999998</v>
       </c>
-      <c r="O37" s="15"/>
-      <c r="P37" s="13">
+      <c r="O42" s="15"/>
+      <c r="P42" s="13">
         <v>0.65200000000000002</v>
       </c>
-      <c r="Q37" s="13">
+      <c r="Q42" s="13">
         <v>0.90390000000000004</v>
       </c>
-      <c r="R37" s="13">
+      <c r="R42" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13">
+      <c r="S42" s="13"/>
+      <c r="T42" s="13">
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="38" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C38" s="6" t="s">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C43" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D43" s="6">
         <v>0.43480000000000002</v>
       </c>
-      <c r="E38" s="16">
+      <c r="E43" s="16">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F38" s="6">
+      <c r="F43" s="6">
         <v>0.9073</v>
       </c>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6">
+      <c r="G43" s="6"/>
+      <c r="H43" s="6">
         <v>0.39419999999999999</v>
       </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6">
+      <c r="I43" s="6"/>
+      <c r="J43" s="6">
         <v>0.502</v>
       </c>
-      <c r="K38" s="6">
+      <c r="K43" s="6">
         <v>0.88019999999999998</v>
       </c>
-      <c r="L38" s="16">
+      <c r="L43" s="16">
         <v>0.93840000000000001</v>
       </c>
-      <c r="M38" s="6"/>
-      <c r="N38" s="16">
+      <c r="M43" s="6"/>
+      <c r="N43" s="16">
         <v>0.43809999999999999</v>
       </c>
-      <c r="O38" s="6"/>
-      <c r="P38" s="6">
+      <c r="O43" s="6"/>
+      <c r="P43" s="6">
         <v>0.65469999999999995</v>
       </c>
-      <c r="Q38" s="6">
+      <c r="Q43" s="6">
         <v>0.90480000000000005</v>
       </c>
-      <c r="R38" s="6">
+      <c r="R43" s="6">
         <v>0.97250000000000003</v>
       </c>
-      <c r="S38" s="6"/>
-      <c r="T38" s="6">
+      <c r="S43" s="6"/>
+      <c r="T43" s="6">
         <v>0.66139999999999999</v>
       </c>
     </row>
-    <row r="39" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C39" s="1" t="s">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C44" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D39" s="3">
+      <c r="D44" s="3">
         <v>0.43149999999999999</v>
       </c>
-      <c r="E39" s="3">
+      <c r="E44" s="3">
         <v>0.83409999999999995</v>
       </c>
-      <c r="F39" s="3">
+      <c r="F44" s="3">
         <v>0.90590000000000004</v>
       </c>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3">
+      <c r="G44" s="3"/>
+      <c r="H44" s="3">
         <v>0.39169999999999999</v>
       </c>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3">
+      <c r="I44" s="3"/>
+      <c r="J44" s="3">
         <v>0.49930000000000002</v>
       </c>
-      <c r="K39" s="3">
+      <c r="K44" s="3">
         <v>0.87290000000000001</v>
       </c>
-      <c r="L39" s="3">
+      <c r="L44" s="3">
         <v>0.93389999999999995</v>
       </c>
-      <c r="M39" s="3"/>
-      <c r="N39" s="3">
+      <c r="M44" s="3"/>
+      <c r="N44" s="3">
         <v>0.42930000000000001</v>
       </c>
-      <c r="O39" s="4"/>
-      <c r="P39" s="3">
+      <c r="O44" s="4"/>
+      <c r="P44" s="3">
         <v>0.65239999999999998</v>
       </c>
-      <c r="Q39" s="17">
+      <c r="Q44" s="17">
         <v>0.90569999999999995</v>
       </c>
-      <c r="R39" s="3">
+      <c r="R44" s="3">
         <v>0.97260000000000002</v>
       </c>
-      <c r="S39" s="3"/>
-      <c r="T39" s="3">
+      <c r="S44" s="3"/>
+      <c r="T44" s="3">
         <v>0.65810000000000002</v>
       </c>
     </row>
-    <row r="40" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C40" s="1" t="s">
+    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D45" s="1">
         <v>43.45</v>
       </c>
-      <c r="E40" s="1">
+      <c r="E45" s="1">
         <v>83.11</v>
       </c>
-      <c r="F40" s="1">
+      <c r="F45" s="1">
         <v>90.55</v>
       </c>
-      <c r="G40" s="18"/>
-      <c r="H40" s="3">
+      <c r="G45" s="18"/>
+      <c r="H45" s="3">
         <v>0.3896</v>
       </c>
-      <c r="I40" s="1"/>
-      <c r="J40" s="1">
+      <c r="I45" s="1"/>
+      <c r="J45" s="1">
         <v>49.24</v>
       </c>
-      <c r="K40" s="1">
+      <c r="K45" s="1">
         <v>87.43</v>
       </c>
-      <c r="L40" s="1">
+      <c r="L45" s="1">
         <v>93.52</v>
       </c>
-      <c r="M40" s="1"/>
-      <c r="N40" s="3">
+      <c r="M45" s="1"/>
+      <c r="N45" s="3">
         <v>0.42209999999999998</v>
       </c>
-      <c r="O40" s="1"/>
-      <c r="P40" s="4">
+      <c r="O45" s="1"/>
+      <c r="P45" s="4">
         <v>65.39</v>
       </c>
-      <c r="Q40" s="1">
+      <c r="Q45" s="1">
         <v>90.27</v>
       </c>
-      <c r="R40" s="4">
+      <c r="R45" s="4">
         <v>97.27</v>
       </c>
-      <c r="S40" s="1"/>
-      <c r="T40" s="3">
+      <c r="S45" s="1"/>
+      <c r="T45" s="3">
         <v>0.65659999999999996</v>
       </c>
     </row>
-    <row r="41" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C41" s="1" t="s">
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C46" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D46" s="3">
         <v>0.42909999999999998</v>
       </c>
-      <c r="E41" s="3">
+      <c r="E46" s="3">
         <v>0.83479999999999999</v>
       </c>
-      <c r="F41" s="3">
+      <c r="F46" s="3">
         <v>0.90569999999999995</v>
       </c>
-      <c r="G41" s="3"/>
-      <c r="H41" s="3">
+      <c r="G46" s="3"/>
+      <c r="H46" s="3">
         <v>0.38979999999999998</v>
       </c>
-      <c r="I41" s="3"/>
-      <c r="J41" s="3">
+      <c r="I46" s="3"/>
+      <c r="J46" s="3">
         <v>0.49349999999999999</v>
       </c>
-      <c r="K41" s="17">
+      <c r="K46" s="17">
         <v>0.87919999999999998</v>
       </c>
-      <c r="L41" s="3">
+      <c r="L46" s="3">
         <v>0.93830000000000002</v>
       </c>
-      <c r="M41" s="3"/>
-      <c r="N41" s="3">
+      <c r="M46" s="3"/>
+      <c r="N46" s="3">
         <v>0.43259999999999998</v>
       </c>
-      <c r="O41" s="3"/>
-      <c r="P41" s="3">
+      <c r="O46" s="3"/>
+      <c r="P46" s="3">
         <v>0.6482</v>
       </c>
-      <c r="Q41" s="3">
+      <c r="Q46" s="3">
         <v>0.90500000000000003</v>
       </c>
-      <c r="R41" s="3">
+      <c r="R46" s="3">
         <v>0.97209999999999996</v>
       </c>
-      <c r="S41" s="3"/>
-      <c r="T41" s="3">
+      <c r="S46" s="3"/>
+      <c r="T46" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="42" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C42" s="32" t="s">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C47" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D42" s="33">
+      <c r="D47" s="33">
         <v>0.43919999999999998</v>
       </c>
-      <c r="E42" s="33">
+      <c r="E47" s="33">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F42" s="33">
+      <c r="F47" s="33">
         <v>0.90769999999999995</v>
       </c>
-      <c r="G42" s="34"/>
-      <c r="H42" s="35">
+      <c r="G47" s="34"/>
+      <c r="H47" s="35">
         <v>0.39300000000000002</v>
       </c>
-      <c r="I42" s="32"/>
-      <c r="J42" s="33">
+      <c r="I47" s="32"/>
+      <c r="J47" s="33">
         <v>0.503</v>
       </c>
-      <c r="K42" s="35">
+      <c r="K47" s="35">
         <v>0.87680000000000002</v>
       </c>
-      <c r="L42" s="35">
+      <c r="L47" s="35">
         <v>0.93659999999999999</v>
       </c>
-      <c r="M42" s="35"/>
-      <c r="N42" s="35">
+      <c r="M47" s="35"/>
+      <c r="N47" s="35">
         <v>0.43430000000000002</v>
       </c>
-      <c r="O42" s="32"/>
-      <c r="P42" s="33">
+      <c r="O47" s="32"/>
+      <c r="P47" s="33">
         <v>0.6583</v>
       </c>
-      <c r="Q42" s="35">
+      <c r="Q47" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="R42" s="33">
+      <c r="R47" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="S42" s="1"/>
-      <c r="T42" s="17">
+      <c r="S47" s="1"/>
+      <c r="T47" s="17">
         <v>0.66559999999999997</v>
       </c>
     </row>
-    <row r="43" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C43" s="1" t="s">
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C48" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D43" s="4">
+      <c r="D48" s="4">
         <v>42.83</v>
       </c>
-      <c r="E43" s="4">
+      <c r="E48" s="4">
         <v>83.36</v>
       </c>
-      <c r="F43" s="4">
+      <c r="F48" s="4">
         <v>90.7</v>
       </c>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4">
+      <c r="G48" s="4"/>
+      <c r="H48" s="4">
         <v>39.229999999999997</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4">
+      <c r="I48" s="4"/>
+      <c r="J48" s="4">
         <v>49.84</v>
       </c>
-      <c r="K43" s="4">
+      <c r="K48" s="4">
         <v>87.5</v>
       </c>
-      <c r="L43" s="4">
+      <c r="L48" s="4">
         <v>93.41</v>
       </c>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4">
+      <c r="M48" s="4"/>
+      <c r="N48" s="4">
         <v>42.63</v>
       </c>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4">
+      <c r="O48" s="4"/>
+      <c r="P48" s="4">
         <v>65.8</v>
       </c>
-      <c r="Q43" s="4">
+      <c r="Q48" s="4">
         <v>90.5</v>
       </c>
-      <c r="R43" s="4">
+      <c r="R48" s="4">
         <v>97.3</v>
       </c>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4">
+      <c r="S48" s="4"/>
+      <c r="T48" s="4">
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="44" spans="2:20" x14ac:dyDescent="0.25">
-      <c r="C44" s="1" t="s">
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C49" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D44" s="19">
+      <c r="D49" s="19">
         <v>0.4335</v>
       </c>
-      <c r="E44" s="19">
+      <c r="E49" s="19">
         <v>0.83350000000000002</v>
       </c>
-      <c r="F44" s="19">
+      <c r="F49" s="19">
         <v>0.90259999999999996</v>
       </c>
-      <c r="G44" s="20"/>
-      <c r="H44" s="19">
+      <c r="G49" s="20"/>
+      <c r="H49" s="19">
         <v>0.38850000000000001</v>
       </c>
-      <c r="I44" s="21"/>
-      <c r="J44" s="19">
+      <c r="I49" s="21"/>
+      <c r="J49" s="19">
         <v>0.49130000000000001</v>
       </c>
-      <c r="K44" s="19">
+      <c r="K49" s="19">
         <v>0.87970000000000004</v>
       </c>
-      <c r="L44" s="19">
+      <c r="L49" s="19">
         <v>0.93069999999999997</v>
       </c>
-      <c r="M44" s="19"/>
-      <c r="N44" s="19">
+      <c r="M49" s="19"/>
+      <c r="N49" s="19">
         <v>0.41320000000000001</v>
       </c>
-      <c r="O44" s="21"/>
-      <c r="P44" s="19">
+      <c r="O49" s="21"/>
+      <c r="P49" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="Q44" s="19">
+      <c r="Q49" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="R44" s="19">
+      <c r="R49" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="S44" s="22"/>
-      <c r="T44" s="23">
+      <c r="S49" s="22"/>
+      <c r="T49" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C50" t="s">
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C55" t="s">
         <v>31</v>
       </c>
     </row>
@@ -2185,7 +2326,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L20" sqref="L20:M20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix to random read test data
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="100">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -323,6 +323,9 @@
   </si>
   <si>
     <t>2embPpiAnnotE768H4L12I768PreLabSet0_1stRun</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE768H4L12I768PreLabSet0Drop0.2</t>
   </si>
 </sst>
 </file>
@@ -787,8 +790,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:T55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1692,6 +1695,9 @@
       <c r="T32" s="6"/>
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="28" t="s">
+        <v>99</v>
+      </c>
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="6"/>
@@ -1706,9 +1712,15 @@
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="7"/>
-      <c r="P33" s="6"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
+      <c r="P33" s="6">
+        <v>0.66569299999999998</v>
+      </c>
+      <c r="Q33" s="6">
+        <v>0.90422999999999998</v>
+      </c>
+      <c r="R33" s="6">
+        <v>0.97198600000000002</v>
+      </c>
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
     </row>
@@ -1734,9 +1746,6 @@
       <c r="T34" s="6"/>
     </row>
     <row r="35" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="6"/>
@@ -1758,9 +1767,6 @@
       <c r="T35" s="6"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
       <c r="D36" s="6"/>
@@ -1782,9 +1788,6 @@
       <c r="T36" s="6"/>
     </row>
     <row r="37" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
       <c r="D37" s="6"/>
@@ -1806,6 +1809,9 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -1827,6 +1833,9 @@
       <c r="T38" s="6"/>
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1847,6 +1856,9 @@
       <c r="T39" s="6"/>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>35</v>
+      </c>
       <c r="C40" s="5" t="s">
         <v>8</v>
       </c>
@@ -1893,6 +1905,7 @@
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A41" s="28"/>
       <c r="C41" s="8" t="s">
         <v>9</v>
       </c>
@@ -1939,6 +1952,7 @@
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A42" s="28"/>
       <c r="C42" s="12" t="s">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
some scaling init weight not work right
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="351" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="104">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -316,16 +316,28 @@
     <t>Q08873</t>
   </si>
   <si>
-    <t>2embPpiAnnotE768H1L12I768PreLabSet0_1stRun</t>
-  </si>
-  <si>
-    <t>2embPpiAnnotE768H1L12I768PreLabSet0_1stRunDrop0.2</t>
-  </si>
-  <si>
-    <t>2embPpiAnnotE768H4L12I768PreLabSet0_1stRun</t>
-  </si>
-  <si>
     <t>2embPpiAnnotE768H4L12I768PreLabSet0Drop0.2</t>
+  </si>
+  <si>
+    <t>drop0.1 in256 ep10e10</t>
+  </si>
+  <si>
+    <t>drop0.1 in256 ep10e12</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I768Set0_1stRun</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I768Set0_1stRunDrop0.2</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H4L12I768Set0_1stRun</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I768Set0</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H4L12I768Set0</t>
   </si>
 </sst>
 </file>
@@ -788,10 +800,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:T55"/>
+  <dimension ref="A4:T61"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1585,7 +1597,7 @@
     </row>
     <row r="29" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="28" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
@@ -1615,13 +1627,19 @@
     </row>
     <row r="30" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
+      <c r="D30" s="6">
+        <v>0.43213083677139902</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.83454316071685597</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.90633091683560396</v>
+      </c>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
       <c r="I30" s="7"/>
@@ -1645,7 +1663,7 @@
     </row>
     <row r="31" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="28" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1696,37 +1714,56 @@
     </row>
     <row r="33" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="28" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="6"/>
-      <c r="F33" s="6"/>
+      <c r="C33" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" s="6">
+        <v>0.43916617238933098</v>
+      </c>
+      <c r="E33" s="6">
+        <v>0.835605451873769</v>
+      </c>
+      <c r="F33" s="6">
+        <v>0.90752296578104596</v>
+      </c>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="6"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="6"/>
+      <c r="J33" s="6">
+        <v>0.5309239</v>
+      </c>
+      <c r="K33" s="6">
+        <v>0.892953</v>
+      </c>
+      <c r="L33" s="6">
+        <v>0.94298300000000002</v>
+      </c>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
       <c r="O33" s="7"/>
       <c r="P33" s="6">
-        <v>0.66569299999999998</v>
+        <v>0.66610357651026797</v>
       </c>
       <c r="Q33" s="6">
-        <v>0.90422999999999998</v>
+        <v>0.90778748640305595</v>
       </c>
       <c r="R33" s="6">
-        <v>0.97198600000000002</v>
+        <v>0.97222662155700101</v>
       </c>
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
     </row>
     <row r="34" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="B34" s="5"/>
-      <c r="C34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>98</v>
+      </c>
       <c r="D34" s="6"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
@@ -1739,9 +1776,15 @@
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
       <c r="O34" s="7"/>
-      <c r="P34" s="6"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
+      <c r="P34" s="6">
+        <v>0.66219899999999998</v>
+      </c>
+      <c r="Q34" s="6">
+        <v>0.90361093533127401</v>
+      </c>
+      <c r="R34" s="6">
+        <v>0.97134283099715801</v>
+      </c>
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
     </row>
@@ -1767,17 +1810,28 @@
       <c r="T35" s="6"/>
     </row>
     <row r="36" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="D36" s="6"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
       <c r="I36" s="7"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
-      <c r="L36" s="6"/>
+      <c r="J36" s="6">
+        <v>0.520983673424954</v>
+      </c>
+      <c r="K36" s="6">
+        <v>0.89486151979039896</v>
+      </c>
+      <c r="L36" s="6">
+        <v>0.93774798228002598</v>
+      </c>
       <c r="M36" s="6"/>
       <c r="N36" s="6"/>
       <c r="O36" s="7"/>
@@ -1809,9 +1863,6 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="28" t="s">
-        <v>35</v>
-      </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -1834,8 +1885,9 @@
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="28" t="s">
-        <v>35</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
@@ -1849,484 +1901,621 @@
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
       <c r="O39" s="7"/>
-      <c r="P39" s="6"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
+      <c r="P39" s="6">
+        <v>0.66569299999999998</v>
+      </c>
+      <c r="Q39" s="6">
+        <v>0.90422999999999998</v>
+      </c>
+      <c r="R39" s="6">
+        <v>0.97198600000000002</v>
+      </c>
       <c r="S39" s="6"/>
       <c r="T39" s="6"/>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A40" s="28" t="s">
+    <row r="40" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="7"/>
+      <c r="J40" s="6"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="6"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="6"/>
+      <c r="O40" s="7"/>
+      <c r="P40" s="6"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="6"/>
+      <c r="S40" s="6"/>
+      <c r="T40" s="6"/>
+    </row>
+    <row r="41" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="7"/>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
+      <c r="M41" s="6"/>
+      <c r="N41" s="6"/>
+      <c r="O41" s="7"/>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
+      <c r="S41" s="6"/>
+      <c r="T41" s="6"/>
+    </row>
+    <row r="42" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="5"/>
+      <c r="C42" s="5"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="7"/>
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
+      <c r="L42" s="6"/>
+      <c r="M42" s="6"/>
+      <c r="N42" s="6"/>
+      <c r="O42" s="7"/>
+      <c r="P42" s="6"/>
+      <c r="Q42" s="6"/>
+      <c r="R42" s="6"/>
+      <c r="S42" s="6"/>
+      <c r="T42" s="6"/>
+    </row>
+    <row r="43" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="7"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
+      <c r="L43" s="6"/>
+      <c r="M43" s="6"/>
+      <c r="N43" s="6"/>
+      <c r="O43" s="7"/>
+      <c r="P43" s="6"/>
+      <c r="Q43" s="6"/>
+      <c r="R43" s="6"/>
+      <c r="S43" s="6"/>
+      <c r="T43" s="6"/>
+    </row>
+    <row r="44" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="7"/>
+      <c r="J44" s="6"/>
+      <c r="K44" s="6"/>
+      <c r="L44" s="6"/>
+      <c r="M44" s="6"/>
+      <c r="N44" s="6"/>
+      <c r="O44" s="7"/>
+      <c r="P44" s="6"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
+      <c r="S44" s="6"/>
+      <c r="T44" s="6"/>
+    </row>
+    <row r="45" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="7"/>
+      <c r="J45" s="6"/>
+      <c r="K45" s="6"/>
+      <c r="L45" s="6"/>
+      <c r="M45" s="6"/>
+      <c r="N45" s="6"/>
+      <c r="O45" s="7"/>
+      <c r="P45" s="6"/>
+      <c r="Q45" s="6"/>
+      <c r="R45" s="6"/>
+      <c r="S45" s="6"/>
+      <c r="T45" s="6"/>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A46" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C46" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D46" s="6">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E40" s="6">
+      <c r="E46" s="6">
         <v>0.81869999999999998</v>
       </c>
-      <c r="F40" s="6">
+      <c r="F46" s="6">
         <v>0.89700000000000002</v>
       </c>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6">
+      <c r="G46" s="6"/>
+      <c r="H46" s="6">
         <v>0.37009999999999998</v>
       </c>
-      <c r="I40" s="7"/>
-      <c r="J40" s="6">
+      <c r="I46" s="7"/>
+      <c r="J46" s="6">
         <v>0.4677</v>
       </c>
-      <c r="K40" s="6">
+      <c r="K46" s="6">
         <v>0.83730000000000004</v>
       </c>
-      <c r="L40" s="6">
+      <c r="L46" s="6">
         <v>0.90600000000000003</v>
       </c>
-      <c r="M40" s="6"/>
-      <c r="N40" s="6">
+      <c r="M46" s="6"/>
+      <c r="N46" s="6">
         <v>0.3614</v>
       </c>
-      <c r="O40" s="7"/>
-      <c r="P40" s="6">
+      <c r="O46" s="7"/>
+      <c r="P46" s="6">
         <v>0.627</v>
       </c>
-      <c r="Q40" s="6">
+      <c r="Q46" s="6">
         <v>0.878</v>
       </c>
-      <c r="R40" s="6">
+      <c r="R46" s="6">
         <v>0.9647</v>
-      </c>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3">
-        <v>0.62470000000000003</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A41" s="28"/>
-      <c r="C41" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="9">
-        <v>42.51</v>
-      </c>
-      <c r="E41" s="9">
-        <v>82.97</v>
-      </c>
-      <c r="F41" s="9">
-        <v>90.27</v>
-      </c>
-      <c r="G41" s="10"/>
-      <c r="H41" s="11">
-        <v>0.37769999999999998</v>
-      </c>
-      <c r="I41" s="9"/>
-      <c r="J41" s="9">
-        <v>48.62</v>
-      </c>
-      <c r="K41" s="9">
-        <v>87.25</v>
-      </c>
-      <c r="L41" s="9">
-        <v>93.14</v>
-      </c>
-      <c r="M41" s="9"/>
-      <c r="N41" s="11">
-        <v>0.40760000000000002</v>
-      </c>
-      <c r="O41" s="9"/>
-      <c r="P41" s="9">
-        <v>63.77</v>
-      </c>
-      <c r="Q41" s="9">
-        <v>89.79</v>
-      </c>
-      <c r="R41" s="9">
-        <v>97.1</v>
-      </c>
-      <c r="S41" s="8"/>
-      <c r="T41" s="11">
-        <v>0.64100000000000001</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A42" s="28"/>
-      <c r="C42" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="D42" s="13">
-        <v>0.4365</v>
-      </c>
-      <c r="E42" s="13">
-        <v>0.83460000000000001</v>
-      </c>
-      <c r="F42" s="13">
-        <v>0.90629999999999999</v>
-      </c>
-      <c r="G42" s="13"/>
-      <c r="H42" s="14">
-        <v>0.39729999999999999</v>
-      </c>
-      <c r="I42" s="15"/>
-      <c r="J42" s="13">
-        <v>0.49740000000000001</v>
-      </c>
-      <c r="K42" s="13">
-        <v>0.87780000000000002</v>
-      </c>
-      <c r="L42" s="13">
-        <v>0.93500000000000005</v>
-      </c>
-      <c r="M42" s="13"/>
-      <c r="N42" s="13">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="O42" s="15"/>
-      <c r="P42" s="13">
-        <v>0.65200000000000002</v>
-      </c>
-      <c r="Q42" s="13">
-        <v>0.90390000000000004</v>
-      </c>
-      <c r="R42" s="13">
-        <v>0.97199999999999998</v>
-      </c>
-      <c r="S42" s="13"/>
-      <c r="T42" s="13">
-        <v>0.65949999999999998</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C43" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="D43" s="6">
-        <v>0.43480000000000002</v>
-      </c>
-      <c r="E43" s="16">
-        <v>0.83489999999999998</v>
-      </c>
-      <c r="F43" s="6">
-        <v>0.9073</v>
-      </c>
-      <c r="G43" s="6"/>
-      <c r="H43" s="6">
-        <v>0.39419999999999999</v>
-      </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6">
-        <v>0.502</v>
-      </c>
-      <c r="K43" s="6">
-        <v>0.88019999999999998</v>
-      </c>
-      <c r="L43" s="16">
-        <v>0.93840000000000001</v>
-      </c>
-      <c r="M43" s="6"/>
-      <c r="N43" s="16">
-        <v>0.43809999999999999</v>
-      </c>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6">
-        <v>0.65469999999999995</v>
-      </c>
-      <c r="Q43" s="6">
-        <v>0.90480000000000005</v>
-      </c>
-      <c r="R43" s="6">
-        <v>0.97250000000000003</v>
-      </c>
-      <c r="S43" s="6"/>
-      <c r="T43" s="6">
-        <v>0.66139999999999999</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C44" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D44" s="3">
-        <v>0.43149999999999999</v>
-      </c>
-      <c r="E44" s="3">
-        <v>0.83409999999999995</v>
-      </c>
-      <c r="F44" s="3">
-        <v>0.90590000000000004</v>
-      </c>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3">
-        <v>0.39169999999999999</v>
-      </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3">
-        <v>0.49930000000000002</v>
-      </c>
-      <c r="K44" s="3">
-        <v>0.87290000000000001</v>
-      </c>
-      <c r="L44" s="3">
-        <v>0.93389999999999995</v>
-      </c>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3">
-        <v>0.42930000000000001</v>
-      </c>
-      <c r="O44" s="4"/>
-      <c r="P44" s="3">
-        <v>0.65239999999999998</v>
-      </c>
-      <c r="Q44" s="17">
-        <v>0.90569999999999995</v>
-      </c>
-      <c r="R44" s="3">
-        <v>0.97260000000000002</v>
-      </c>
-      <c r="S44" s="3"/>
-      <c r="T44" s="3">
-        <v>0.65810000000000002</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C45" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D45" s="1">
-        <v>43.45</v>
-      </c>
-      <c r="E45" s="1">
-        <v>83.11</v>
-      </c>
-      <c r="F45" s="1">
-        <v>90.55</v>
-      </c>
-      <c r="G45" s="18"/>
-      <c r="H45" s="3">
-        <v>0.3896</v>
-      </c>
-      <c r="I45" s="1"/>
-      <c r="J45" s="1">
-        <v>49.24</v>
-      </c>
-      <c r="K45" s="1">
-        <v>87.43</v>
-      </c>
-      <c r="L45" s="1">
-        <v>93.52</v>
-      </c>
-      <c r="M45" s="1"/>
-      <c r="N45" s="3">
-        <v>0.42209999999999998</v>
-      </c>
-      <c r="O45" s="1"/>
-      <c r="P45" s="4">
-        <v>65.39</v>
-      </c>
-      <c r="Q45" s="1">
-        <v>90.27</v>
-      </c>
-      <c r="R45" s="4">
-        <v>97.27</v>
-      </c>
-      <c r="S45" s="1"/>
-      <c r="T45" s="3">
-        <v>0.65659999999999996</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D46" s="3">
-        <v>0.42909999999999998</v>
-      </c>
-      <c r="E46" s="3">
-        <v>0.83479999999999999</v>
-      </c>
-      <c r="F46" s="3">
-        <v>0.90569999999999995</v>
-      </c>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3">
-        <v>0.38979999999999998</v>
-      </c>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3">
-        <v>0.49349999999999999</v>
-      </c>
-      <c r="K46" s="17">
-        <v>0.87919999999999998</v>
-      </c>
-      <c r="L46" s="3">
-        <v>0.93830000000000002</v>
-      </c>
-      <c r="M46" s="3"/>
-      <c r="N46" s="3">
-        <v>0.43259999999999998</v>
-      </c>
-      <c r="O46" s="3"/>
-      <c r="P46" s="3">
-        <v>0.6482</v>
-      </c>
-      <c r="Q46" s="3">
-        <v>0.90500000000000003</v>
-      </c>
-      <c r="R46" s="3">
-        <v>0.97209999999999996</v>
       </c>
       <c r="S46" s="3"/>
       <c r="T46" s="3">
+        <v>0.62470000000000003</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A47" s="28"/>
+      <c r="C47" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="9">
+        <v>42.51</v>
+      </c>
+      <c r="E47" s="9">
+        <v>82.97</v>
+      </c>
+      <c r="F47" s="9">
+        <v>90.27</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="11">
+        <v>0.37769999999999998</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9">
+        <v>48.62</v>
+      </c>
+      <c r="K47" s="9">
+        <v>87.25</v>
+      </c>
+      <c r="L47" s="9">
+        <v>93.14</v>
+      </c>
+      <c r="M47" s="9"/>
+      <c r="N47" s="11">
+        <v>0.40760000000000002</v>
+      </c>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9">
+        <v>63.77</v>
+      </c>
+      <c r="Q47" s="9">
+        <v>89.79</v>
+      </c>
+      <c r="R47" s="9">
+        <v>97.1</v>
+      </c>
+      <c r="S47" s="8"/>
+      <c r="T47" s="11">
+        <v>0.64100000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A48" s="28"/>
+      <c r="C48" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48" s="13">
+        <v>0.4365</v>
+      </c>
+      <c r="E48" s="13">
+        <v>0.83460000000000001</v>
+      </c>
+      <c r="F48" s="13">
+        <v>0.90629999999999999</v>
+      </c>
+      <c r="G48" s="13"/>
+      <c r="H48" s="14">
+        <v>0.39729999999999999</v>
+      </c>
+      <c r="I48" s="15"/>
+      <c r="J48" s="13">
+        <v>0.49740000000000001</v>
+      </c>
+      <c r="K48" s="13">
+        <v>0.87780000000000002</v>
+      </c>
+      <c r="L48" s="13">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="M48" s="13"/>
+      <c r="N48" s="13">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="O48" s="15"/>
+      <c r="P48" s="13">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="Q48" s="13">
+        <v>0.90390000000000004</v>
+      </c>
+      <c r="R48" s="13">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="S48" s="13"/>
+      <c r="T48" s="13">
+        <v>0.65949999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C49" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D49" s="6">
+        <v>0.43480000000000002</v>
+      </c>
+      <c r="E49" s="16">
+        <v>0.83489999999999998</v>
+      </c>
+      <c r="F49" s="6">
+        <v>0.9073</v>
+      </c>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6">
+        <v>0.39419999999999999</v>
+      </c>
+      <c r="I49" s="6"/>
+      <c r="J49" s="6">
+        <v>0.502</v>
+      </c>
+      <c r="K49" s="6">
+        <v>0.88019999999999998</v>
+      </c>
+      <c r="L49" s="16">
+        <v>0.93840000000000001</v>
+      </c>
+      <c r="M49" s="6"/>
+      <c r="N49" s="16">
+        <v>0.43809999999999999</v>
+      </c>
+      <c r="O49" s="6"/>
+      <c r="P49" s="6">
+        <v>0.65469999999999995</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>0.90480000000000005</v>
+      </c>
+      <c r="R49" s="6">
+        <v>0.97250000000000003</v>
+      </c>
+      <c r="S49" s="6"/>
+      <c r="T49" s="6">
+        <v>0.66139999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C50" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" s="3">
+        <v>0.43149999999999999</v>
+      </c>
+      <c r="E50" s="3">
+        <v>0.83409999999999995</v>
+      </c>
+      <c r="F50" s="3">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3">
+        <v>0.39169999999999999</v>
+      </c>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3">
+        <v>0.49930000000000002</v>
+      </c>
+      <c r="K50" s="3">
+        <v>0.87290000000000001</v>
+      </c>
+      <c r="L50" s="3">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="M50" s="3"/>
+      <c r="N50" s="3">
+        <v>0.42930000000000001</v>
+      </c>
+      <c r="O50" s="4"/>
+      <c r="P50" s="3">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="Q50" s="17">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="R50" s="3">
+        <v>0.97260000000000002</v>
+      </c>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3">
+        <v>0.65810000000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D51" s="1">
+        <v>43.45</v>
+      </c>
+      <c r="E51" s="1">
+        <v>83.11</v>
+      </c>
+      <c r="F51" s="1">
+        <v>90.55</v>
+      </c>
+      <c r="G51" s="18"/>
+      <c r="H51" s="3">
+        <v>0.3896</v>
+      </c>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1">
+        <v>49.24</v>
+      </c>
+      <c r="K51" s="1">
+        <v>87.43</v>
+      </c>
+      <c r="L51" s="1">
+        <v>93.52</v>
+      </c>
+      <c r="M51" s="1"/>
+      <c r="N51" s="3">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="O51" s="1"/>
+      <c r="P51" s="4">
+        <v>65.39</v>
+      </c>
+      <c r="Q51" s="1">
+        <v>90.27</v>
+      </c>
+      <c r="R51" s="4">
+        <v>97.27</v>
+      </c>
+      <c r="S51" s="1"/>
+      <c r="T51" s="3">
+        <v>0.65659999999999996</v>
+      </c>
+    </row>
+    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D52" s="3">
+        <v>0.42909999999999998</v>
+      </c>
+      <c r="E52" s="3">
+        <v>0.83479999999999999</v>
+      </c>
+      <c r="F52" s="3">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="G52" s="3"/>
+      <c r="H52" s="3">
+        <v>0.38979999999999998</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3">
+        <v>0.49349999999999999</v>
+      </c>
+      <c r="K52" s="17">
+        <v>0.87919999999999998</v>
+      </c>
+      <c r="L52" s="3">
+        <v>0.93830000000000002</v>
+      </c>
+      <c r="M52" s="3"/>
+      <c r="N52" s="3">
+        <v>0.43259999999999998</v>
+      </c>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3">
+        <v>0.6482</v>
+      </c>
+      <c r="Q52" s="3">
+        <v>0.90500000000000003</v>
+      </c>
+      <c r="R52" s="3">
+        <v>0.97209999999999996</v>
+      </c>
+      <c r="S52" s="3"/>
+      <c r="T52" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C47" s="32" t="s">
+    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C53" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="33">
+      <c r="D53" s="33">
         <v>0.43919999999999998</v>
       </c>
-      <c r="E47" s="33">
+      <c r="E53" s="33">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F47" s="33">
+      <c r="F53" s="33">
         <v>0.90769999999999995</v>
       </c>
-      <c r="G47" s="34"/>
-      <c r="H47" s="35">
+      <c r="G53" s="34"/>
+      <c r="H53" s="35">
         <v>0.39300000000000002</v>
       </c>
-      <c r="I47" s="32"/>
-      <c r="J47" s="33">
+      <c r="I53" s="32"/>
+      <c r="J53" s="33">
         <v>0.503</v>
       </c>
-      <c r="K47" s="35">
+      <c r="K53" s="35">
         <v>0.87680000000000002</v>
       </c>
-      <c r="L47" s="35">
+      <c r="L53" s="35">
         <v>0.93659999999999999</v>
       </c>
-      <c r="M47" s="35"/>
-      <c r="N47" s="35">
+      <c r="M53" s="35"/>
+      <c r="N53" s="35">
         <v>0.43430000000000002</v>
       </c>
-      <c r="O47" s="32"/>
-      <c r="P47" s="33">
+      <c r="O53" s="32"/>
+      <c r="P53" s="33">
         <v>0.6583</v>
       </c>
-      <c r="Q47" s="35">
+      <c r="Q53" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="R47" s="33">
+      <c r="R53" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="S47" s="1"/>
-      <c r="T47" s="17">
+      <c r="S53" s="1"/>
+      <c r="T53" s="17">
         <v>0.66559999999999997</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C48" s="1" t="s">
+    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C54" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="4">
+      <c r="D54" s="4">
         <v>42.83</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E54" s="4">
         <v>83.36</v>
       </c>
-      <c r="F48" s="4">
+      <c r="F54" s="4">
         <v>90.7</v>
       </c>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4">
+      <c r="G54" s="4"/>
+      <c r="H54" s="4">
         <v>39.229999999999997</v>
       </c>
-      <c r="I48" s="4"/>
-      <c r="J48" s="4">
+      <c r="I54" s="4"/>
+      <c r="J54" s="4">
         <v>49.84</v>
       </c>
-      <c r="K48" s="4">
+      <c r="K54" s="4">
         <v>87.5</v>
       </c>
-      <c r="L48" s="4">
+      <c r="L54" s="4">
         <v>93.41</v>
       </c>
-      <c r="M48" s="4"/>
-      <c r="N48" s="4">
+      <c r="M54" s="4"/>
+      <c r="N54" s="4">
         <v>42.63</v>
       </c>
-      <c r="O48" s="4"/>
-      <c r="P48" s="4">
+      <c r="O54" s="4"/>
+      <c r="P54" s="4">
         <v>65.8</v>
       </c>
-      <c r="Q48" s="4">
+      <c r="Q54" s="4">
         <v>90.5</v>
       </c>
-      <c r="R48" s="4">
+      <c r="R54" s="4">
         <v>97.3</v>
       </c>
-      <c r="S48" s="4"/>
-      <c r="T48" s="4">
+      <c r="S54" s="4"/>
+      <c r="T54" s="4">
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C49" s="1" t="s">
+    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C55" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="19">
+      <c r="D55" s="19">
         <v>0.4335</v>
       </c>
-      <c r="E49" s="19">
+      <c r="E55" s="19">
         <v>0.83350000000000002</v>
       </c>
-      <c r="F49" s="19">
+      <c r="F55" s="19">
         <v>0.90259999999999996</v>
       </c>
-      <c r="G49" s="20"/>
-      <c r="H49" s="19">
+      <c r="G55" s="20"/>
+      <c r="H55" s="19">
         <v>0.38850000000000001</v>
       </c>
-      <c r="I49" s="21"/>
-      <c r="J49" s="19">
+      <c r="I55" s="21"/>
+      <c r="J55" s="19">
         <v>0.49130000000000001</v>
       </c>
-      <c r="K49" s="19">
+      <c r="K55" s="19">
         <v>0.87970000000000004</v>
       </c>
-      <c r="L49" s="19">
+      <c r="L55" s="19">
         <v>0.93069999999999997</v>
       </c>
-      <c r="M49" s="19"/>
-      <c r="N49" s="19">
+      <c r="M55" s="19"/>
+      <c r="N55" s="19">
         <v>0.41320000000000001</v>
       </c>
-      <c r="O49" s="21"/>
-      <c r="P49" s="19">
+      <c r="O55" s="21"/>
+      <c r="P55" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="Q49" s="19">
+      <c r="Q55" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="R49" s="19">
+      <c r="R55" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="S49" s="22"/>
-      <c r="T49" s="23">
+      <c r="S55" s="22"/>
+      <c r="T55" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C54" t="s">
+    <row r="60" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C55" t="s">
+    <row r="61" spans="3:20" x14ac:dyDescent="0.25">
+      <c r="C61" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fix some stupid path
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="106">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -341,14 +341,18 @@
   </si>
   <si>
     <t>NoPpiEp10e10Drop0.1</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I768Set0/BertAve12Ep10e12Drop0.1Lr5e5None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -481,7 +485,7 @@
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
@@ -521,6 +525,8 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
@@ -803,10 +809,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:T61"/>
+  <dimension ref="A4:T66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R41" sqref="P41:R41"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1735,18 +1741,20 @@
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
       <c r="I33" s="7"/>
-      <c r="J33" s="6">
+      <c r="J33" s="40">
         <v>0.5309239</v>
       </c>
-      <c r="K33" s="6">
+      <c r="K33" s="40">
         <v>0.892953</v>
       </c>
-      <c r="L33" s="6">
+      <c r="L33" s="40">
         <v>0.94298300000000002</v>
       </c>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
-      <c r="O33" s="7"/>
+      <c r="O33" s="39">
+        <v>4.1920459275095398E-2</v>
+      </c>
       <c r="P33" s="6">
         <v>0.66610357651026797</v>
       </c>
@@ -1866,6 +1874,9 @@
       <c r="T37" s="6"/>
     </row>
     <row r="38" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
       <c r="D38" s="6"/>
@@ -1874,9 +1885,15 @@
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
       <c r="I38" s="7"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
-      <c r="L38" s="6"/>
+      <c r="J38" s="6">
+        <v>0.51423909004761503</v>
+      </c>
+      <c r="K38" s="6">
+        <v>0.88734048870237103</v>
+      </c>
+      <c r="L38" s="6">
+        <v>0.93880771591373202</v>
+      </c>
       <c r="M38" s="6"/>
       <c r="N38" s="6"/>
       <c r="O38" s="7"/>
@@ -1887,9 +1904,6 @@
       <c r="T38" s="6"/>
     </row>
     <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="28" t="s">
-        <v>96</v>
-      </c>
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="6"/>
@@ -1898,21 +1912,23 @@
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
       <c r="I39" s="7"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
-      <c r="L39" s="6"/>
+      <c r="J39" s="6">
+        <v>0.51169393197777102</v>
+      </c>
+      <c r="K39" s="6">
+        <v>0.89076338804911404</v>
+      </c>
+      <c r="L39" s="6">
+        <v>0.94032778400047801</v>
+      </c>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
-      <c r="O39" s="7"/>
-      <c r="P39" s="6">
-        <v>0.66569299999999998</v>
-      </c>
-      <c r="Q39" s="6">
-        <v>0.90422999999999998</v>
-      </c>
-      <c r="R39" s="6">
-        <v>0.97198600000000002</v>
-      </c>
+      <c r="O39" s="39">
+        <v>4.2612862119596799E-2</v>
+      </c>
+      <c r="P39" s="6"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
       <c r="S39" s="6"/>
       <c r="T39" s="6"/>
     </row>
@@ -1938,9 +1954,6 @@
       <c r="T40" s="6"/>
     </row>
     <row r="41" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="28" t="s">
-        <v>104</v>
-      </c>
       <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="6"/>
@@ -1949,27 +1962,15 @@
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
       <c r="I41" s="7"/>
-      <c r="J41" s="6">
-        <v>0.40104148966138098</v>
-      </c>
-      <c r="K41" s="6">
-        <v>0.78469118831988205</v>
-      </c>
-      <c r="L41" s="6">
-        <v>0.89141190674054405</v>
-      </c>
+      <c r="J41" s="6"/>
+      <c r="K41" s="6"/>
+      <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
       <c r="O41" s="7"/>
-      <c r="P41" s="6">
-        <v>0.59847806990903096</v>
-      </c>
-      <c r="Q41" s="6">
-        <v>0.74540495542180496</v>
-      </c>
-      <c r="R41" s="6">
-        <v>0.94279293529049801</v>
-      </c>
+      <c r="P41" s="6"/>
+      <c r="Q41" s="6"/>
+      <c r="R41" s="6"/>
       <c r="S41" s="6"/>
       <c r="T41" s="6"/>
     </row>
@@ -2017,7 +2018,7 @@
     </row>
     <row r="44" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="28" t="s">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
@@ -2033,16 +2034,20 @@
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
       <c r="O44" s="7"/>
-      <c r="P44" s="6"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
+      <c r="P44" s="6">
+        <v>0.66569299999999998</v>
+      </c>
+      <c r="Q44" s="6">
+        <v>0.90422999999999998</v>
+      </c>
+      <c r="R44" s="6">
+        <v>0.97198600000000002</v>
+      </c>
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
     </row>
     <row r="45" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="28" t="s">
-        <v>35</v>
-      </c>
+      <c r="B45" s="5"/>
       <c r="C45" s="5"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
@@ -2062,478 +2067,603 @@
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C46" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D46" s="6">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="E46" s="6">
-        <v>0.81869999999999998</v>
-      </c>
-      <c r="F46" s="6">
-        <v>0.89700000000000002</v>
-      </c>
+        <v>104</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="6">
-        <v>0.37009999999999998</v>
-      </c>
+      <c r="H46" s="6"/>
       <c r="I46" s="7"/>
       <c r="J46" s="6">
-        <v>0.4677</v>
+        <v>0.40104148966138098</v>
       </c>
       <c r="K46" s="6">
-        <v>0.83730000000000004</v>
+        <v>0.78469118831988205</v>
       </c>
       <c r="L46" s="6">
-        <v>0.90600000000000003</v>
+        <v>0.89141190674054405</v>
       </c>
       <c r="M46" s="6"/>
-      <c r="N46" s="6">
-        <v>0.3614</v>
-      </c>
+      <c r="N46" s="6"/>
       <c r="O46" s="7"/>
       <c r="P46" s="6">
+        <v>0.59847806990903096</v>
+      </c>
+      <c r="Q46" s="6">
+        <v>0.74540495542180496</v>
+      </c>
+      <c r="R46" s="6">
+        <v>0.94279293529049801</v>
+      </c>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
+    </row>
+    <row r="47" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="7"/>
+      <c r="J47" s="6"/>
+      <c r="K47" s="6"/>
+      <c r="L47" s="6"/>
+      <c r="M47" s="6"/>
+      <c r="N47" s="6"/>
+      <c r="O47" s="7"/>
+      <c r="P47" s="6"/>
+      <c r="Q47" s="6"/>
+      <c r="R47" s="6"/>
+      <c r="S47" s="6"/>
+      <c r="T47" s="6"/>
+    </row>
+    <row r="48" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="7"/>
+      <c r="J48" s="6"/>
+      <c r="K48" s="6"/>
+      <c r="L48" s="6"/>
+      <c r="M48" s="6"/>
+      <c r="N48" s="6"/>
+      <c r="O48" s="7"/>
+      <c r="P48" s="6"/>
+      <c r="Q48" s="6"/>
+      <c r="R48" s="6"/>
+      <c r="S48" s="6"/>
+      <c r="T48" s="6"/>
+    </row>
+    <row r="49" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="7"/>
+      <c r="J49" s="6"/>
+      <c r="K49" s="6"/>
+      <c r="L49" s="6"/>
+      <c r="M49" s="6"/>
+      <c r="N49" s="6"/>
+      <c r="O49" s="7"/>
+      <c r="P49" s="6"/>
+      <c r="Q49" s="6"/>
+      <c r="R49" s="6"/>
+      <c r="S49" s="6"/>
+      <c r="T49" s="6"/>
+    </row>
+    <row r="50" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="7"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
+      <c r="L50" s="6"/>
+      <c r="M50" s="6"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="7"/>
+      <c r="P50" s="6"/>
+      <c r="Q50" s="6"/>
+      <c r="R50" s="6"/>
+      <c r="S50" s="6"/>
+      <c r="T50" s="6"/>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A51" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="6">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="E51" s="6">
+        <v>0.81869999999999998</v>
+      </c>
+      <c r="F51" s="6">
+        <v>0.89700000000000002</v>
+      </c>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6">
+        <v>0.37009999999999998</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="6">
+        <v>0.4677</v>
+      </c>
+      <c r="K51" s="6">
+        <v>0.83730000000000004</v>
+      </c>
+      <c r="L51" s="6">
+        <v>0.90600000000000003</v>
+      </c>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6">
+        <v>0.3614</v>
+      </c>
+      <c r="O51" s="7"/>
+      <c r="P51" s="6">
         <v>0.627</v>
       </c>
-      <c r="Q46" s="6">
+      <c r="Q51" s="6">
         <v>0.878</v>
       </c>
-      <c r="R46" s="6">
+      <c r="R51" s="6">
         <v>0.9647</v>
       </c>
-      <c r="S46" s="3"/>
-      <c r="T46" s="3">
+      <c r="S51" s="3"/>
+      <c r="T51" s="3">
         <v>0.62470000000000003</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A47" s="28"/>
-      <c r="C47" s="8" t="s">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A52" s="28"/>
+      <c r="C52" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D47" s="9">
+      <c r="D52" s="9">
         <v>42.51</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E52" s="9">
         <v>82.97</v>
       </c>
-      <c r="F47" s="9">
+      <c r="F52" s="9">
         <v>90.27</v>
       </c>
-      <c r="G47" s="10"/>
-      <c r="H47" s="11">
+      <c r="G52" s="10"/>
+      <c r="H52" s="11">
         <v>0.37769999999999998</v>
       </c>
-      <c r="I47" s="9"/>
-      <c r="J47" s="9">
+      <c r="I52" s="9"/>
+      <c r="J52" s="9">
         <v>48.62</v>
       </c>
-      <c r="K47" s="9">
+      <c r="K52" s="9">
         <v>87.25</v>
       </c>
-      <c r="L47" s="9">
+      <c r="L52" s="9">
         <v>93.14</v>
       </c>
-      <c r="M47" s="9"/>
-      <c r="N47" s="11">
+      <c r="M52" s="9"/>
+      <c r="N52" s="11">
         <v>0.40760000000000002</v>
       </c>
-      <c r="O47" s="9"/>
-      <c r="P47" s="9">
+      <c r="O52" s="9"/>
+      <c r="P52" s="9">
         <v>63.77</v>
       </c>
-      <c r="Q47" s="9">
+      <c r="Q52" s="9">
         <v>89.79</v>
       </c>
-      <c r="R47" s="9">
+      <c r="R52" s="9">
         <v>97.1</v>
       </c>
-      <c r="S47" s="8"/>
-      <c r="T47" s="11">
+      <c r="S52" s="8"/>
+      <c r="T52" s="11">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A48" s="28"/>
-      <c r="C48" s="12" t="s">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A53" s="28"/>
+      <c r="C53" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D48" s="13">
+      <c r="D53" s="13">
         <v>0.4365</v>
       </c>
-      <c r="E48" s="13">
+      <c r="E53" s="13">
         <v>0.83460000000000001</v>
       </c>
-      <c r="F48" s="13">
+      <c r="F53" s="13">
         <v>0.90629999999999999</v>
       </c>
-      <c r="G48" s="13"/>
-      <c r="H48" s="14">
+      <c r="G53" s="13"/>
+      <c r="H53" s="14">
         <v>0.39729999999999999</v>
       </c>
-      <c r="I48" s="15"/>
-      <c r="J48" s="13">
+      <c r="I53" s="15"/>
+      <c r="J53" s="13">
         <v>0.49740000000000001</v>
       </c>
-      <c r="K48" s="13">
+      <c r="K53" s="13">
         <v>0.87780000000000002</v>
       </c>
-      <c r="L48" s="13">
+      <c r="L53" s="13">
         <v>0.93500000000000005</v>
       </c>
-      <c r="M48" s="13"/>
-      <c r="N48" s="13">
+      <c r="M53" s="13"/>
+      <c r="N53" s="13">
         <v>0.41799999999999998</v>
       </c>
-      <c r="O48" s="15"/>
-      <c r="P48" s="13">
+      <c r="O53" s="15"/>
+      <c r="P53" s="13">
         <v>0.65200000000000002</v>
       </c>
-      <c r="Q48" s="13">
+      <c r="Q53" s="13">
         <v>0.90390000000000004</v>
       </c>
-      <c r="R48" s="13">
+      <c r="R53" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="S48" s="13"/>
-      <c r="T48" s="13">
+      <c r="S53" s="13"/>
+      <c r="T53" s="13">
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="49" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C49" s="6" t="s">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C54" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="6">
+      <c r="D54" s="6">
         <v>0.43480000000000002</v>
       </c>
-      <c r="E49" s="16">
+      <c r="E54" s="16">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F49" s="6">
+      <c r="F54" s="6">
         <v>0.9073</v>
       </c>
-      <c r="G49" s="6"/>
-      <c r="H49" s="6">
+      <c r="G54" s="6"/>
+      <c r="H54" s="6">
         <v>0.39419999999999999</v>
       </c>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6">
+      <c r="I54" s="6"/>
+      <c r="J54" s="6">
         <v>0.502</v>
       </c>
-      <c r="K49" s="6">
+      <c r="K54" s="6">
         <v>0.88019999999999998</v>
       </c>
-      <c r="L49" s="16">
+      <c r="L54" s="16">
         <v>0.93840000000000001</v>
       </c>
-      <c r="M49" s="6"/>
-      <c r="N49" s="16">
+      <c r="M54" s="6"/>
+      <c r="N54" s="16">
         <v>0.43809999999999999</v>
       </c>
-      <c r="O49" s="6"/>
-      <c r="P49" s="6">
+      <c r="O54" s="6"/>
+      <c r="P54" s="6">
         <v>0.65469999999999995</v>
       </c>
-      <c r="Q49" s="6">
+      <c r="Q54" s="6">
         <v>0.90480000000000005</v>
       </c>
-      <c r="R49" s="6">
+      <c r="R54" s="6">
         <v>0.97250000000000003</v>
       </c>
-      <c r="S49" s="6"/>
-      <c r="T49" s="6">
+      <c r="S54" s="6"/>
+      <c r="T54" s="6">
         <v>0.66139999999999999</v>
       </c>
     </row>
-    <row r="50" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C50" s="1" t="s">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C55" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="3">
+      <c r="D55" s="3">
         <v>0.43149999999999999</v>
       </c>
-      <c r="E50" s="3">
+      <c r="E55" s="3">
         <v>0.83409999999999995</v>
       </c>
-      <c r="F50" s="3">
+      <c r="F55" s="3">
         <v>0.90590000000000004</v>
       </c>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3">
+      <c r="G55" s="3"/>
+      <c r="H55" s="3">
         <v>0.39169999999999999</v>
       </c>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3">
+      <c r="I55" s="3"/>
+      <c r="J55" s="3">
         <v>0.49930000000000002</v>
       </c>
-      <c r="K50" s="3">
+      <c r="K55" s="3">
         <v>0.87290000000000001</v>
       </c>
-      <c r="L50" s="3">
+      <c r="L55" s="3">
         <v>0.93389999999999995</v>
       </c>
-      <c r="M50" s="3"/>
-      <c r="N50" s="3">
+      <c r="M55" s="3"/>
+      <c r="N55" s="3">
         <v>0.42930000000000001</v>
       </c>
-      <c r="O50" s="4"/>
-      <c r="P50" s="3">
+      <c r="O55" s="4"/>
+      <c r="P55" s="3">
         <v>0.65239999999999998</v>
       </c>
-      <c r="Q50" s="17">
+      <c r="Q55" s="17">
         <v>0.90569999999999995</v>
       </c>
-      <c r="R50" s="3">
+      <c r="R55" s="3">
         <v>0.97260000000000002</v>
       </c>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3">
+      <c r="S55" s="3"/>
+      <c r="T55" s="3">
         <v>0.65810000000000002</v>
       </c>
     </row>
-    <row r="51" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C51" s="1" t="s">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D56" s="1">
         <v>43.45</v>
       </c>
-      <c r="E51" s="1">
+      <c r="E56" s="1">
         <v>83.11</v>
       </c>
-      <c r="F51" s="1">
+      <c r="F56" s="1">
         <v>90.55</v>
       </c>
-      <c r="G51" s="18"/>
-      <c r="H51" s="3">
+      <c r="G56" s="18"/>
+      <c r="H56" s="3">
         <v>0.3896</v>
       </c>
-      <c r="I51" s="1"/>
-      <c r="J51" s="1">
+      <c r="I56" s="1"/>
+      <c r="J56" s="1">
         <v>49.24</v>
       </c>
-      <c r="K51" s="1">
+      <c r="K56" s="1">
         <v>87.43</v>
       </c>
-      <c r="L51" s="1">
+      <c r="L56" s="1">
         <v>93.52</v>
       </c>
-      <c r="M51" s="1"/>
-      <c r="N51" s="3">
+      <c r="M56" s="1"/>
+      <c r="N56" s="3">
         <v>0.42209999999999998</v>
       </c>
-      <c r="O51" s="1"/>
-      <c r="P51" s="4">
+      <c r="O56" s="1"/>
+      <c r="P56" s="4">
         <v>65.39</v>
       </c>
-      <c r="Q51" s="1">
+      <c r="Q56" s="1">
         <v>90.27</v>
       </c>
-      <c r="R51" s="4">
+      <c r="R56" s="4">
         <v>97.27</v>
       </c>
-      <c r="S51" s="1"/>
-      <c r="T51" s="3">
+      <c r="S56" s="1"/>
+      <c r="T56" s="3">
         <v>0.65659999999999996</v>
       </c>
     </row>
-    <row r="52" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C52" s="1" t="s">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C57" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="3">
+      <c r="D57" s="3">
         <v>0.42909999999999998</v>
       </c>
-      <c r="E52" s="3">
+      <c r="E57" s="3">
         <v>0.83479999999999999</v>
       </c>
-      <c r="F52" s="3">
+      <c r="F57" s="3">
         <v>0.90569999999999995</v>
       </c>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3">
+      <c r="G57" s="3"/>
+      <c r="H57" s="3">
         <v>0.38979999999999998</v>
       </c>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3">
+      <c r="I57" s="3"/>
+      <c r="J57" s="3">
         <v>0.49349999999999999</v>
       </c>
-      <c r="K52" s="17">
+      <c r="K57" s="17">
         <v>0.87919999999999998</v>
       </c>
-      <c r="L52" s="3">
+      <c r="L57" s="3">
         <v>0.93830000000000002</v>
       </c>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3">
+      <c r="M57" s="3"/>
+      <c r="N57" s="3">
         <v>0.43259999999999998</v>
       </c>
-      <c r="O52" s="3"/>
-      <c r="P52" s="3">
+      <c r="O57" s="3"/>
+      <c r="P57" s="3">
         <v>0.6482</v>
       </c>
-      <c r="Q52" s="3">
+      <c r="Q57" s="3">
         <v>0.90500000000000003</v>
       </c>
-      <c r="R52" s="3">
+      <c r="R57" s="3">
         <v>0.97209999999999996</v>
       </c>
-      <c r="S52" s="3"/>
-      <c r="T52" s="3">
+      <c r="S57" s="3"/>
+      <c r="T57" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="53" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C53" s="32" t="s">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C58" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D53" s="33">
+      <c r="D58" s="33">
         <v>0.43919999999999998</v>
       </c>
-      <c r="E53" s="33">
+      <c r="E58" s="33">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F53" s="33">
+      <c r="F58" s="33">
         <v>0.90769999999999995</v>
       </c>
-      <c r="G53" s="34"/>
-      <c r="H53" s="35">
+      <c r="G58" s="34"/>
+      <c r="H58" s="35">
         <v>0.39300000000000002</v>
       </c>
-      <c r="I53" s="32"/>
-      <c r="J53" s="33">
+      <c r="I58" s="32"/>
+      <c r="J58" s="33">
         <v>0.503</v>
       </c>
-      <c r="K53" s="35">
+      <c r="K58" s="35">
         <v>0.87680000000000002</v>
       </c>
-      <c r="L53" s="35">
+      <c r="L58" s="35">
         <v>0.93659999999999999</v>
       </c>
-      <c r="M53" s="35"/>
-      <c r="N53" s="35">
+      <c r="M58" s="35"/>
+      <c r="N58" s="35">
         <v>0.43430000000000002</v>
       </c>
-      <c r="O53" s="32"/>
-      <c r="P53" s="33">
+      <c r="O58" s="32"/>
+      <c r="P58" s="33">
         <v>0.6583</v>
       </c>
-      <c r="Q53" s="35">
+      <c r="Q58" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="R53" s="33">
+      <c r="R58" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="S53" s="1"/>
-      <c r="T53" s="17">
+      <c r="S58" s="1"/>
+      <c r="T58" s="17">
         <v>0.66559999999999997</v>
       </c>
     </row>
-    <row r="54" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C54" s="1" t="s">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D54" s="4">
+      <c r="D59" s="4">
         <v>42.83</v>
       </c>
-      <c r="E54" s="4">
+      <c r="E59" s="4">
         <v>83.36</v>
       </c>
-      <c r="F54" s="4">
+      <c r="F59" s="4">
         <v>90.7</v>
       </c>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4">
+      <c r="G59" s="4"/>
+      <c r="H59" s="4">
         <v>39.229999999999997</v>
       </c>
-      <c r="I54" s="4"/>
-      <c r="J54" s="4">
+      <c r="I59" s="4"/>
+      <c r="J59" s="4">
         <v>49.84</v>
       </c>
-      <c r="K54" s="4">
+      <c r="K59" s="4">
         <v>87.5</v>
       </c>
-      <c r="L54" s="4">
+      <c r="L59" s="4">
         <v>93.41</v>
       </c>
-      <c r="M54" s="4"/>
-      <c r="N54" s="4">
+      <c r="M59" s="4"/>
+      <c r="N59" s="4">
         <v>42.63</v>
       </c>
-      <c r="O54" s="4"/>
-      <c r="P54" s="4">
+      <c r="O59" s="4"/>
+      <c r="P59" s="4">
         <v>65.8</v>
       </c>
-      <c r="Q54" s="4">
+      <c r="Q59" s="4">
         <v>90.5</v>
       </c>
-      <c r="R54" s="4">
+      <c r="R59" s="4">
         <v>97.3</v>
       </c>
-      <c r="S54" s="4"/>
-      <c r="T54" s="4">
+      <c r="S59" s="4"/>
+      <c r="T59" s="4">
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="55" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C55" s="1" t="s">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="C60" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="19">
+      <c r="D60" s="19">
         <v>0.4335</v>
       </c>
-      <c r="E55" s="19">
+      <c r="E60" s="19">
         <v>0.83350000000000002</v>
       </c>
-      <c r="F55" s="19">
+      <c r="F60" s="19">
         <v>0.90259999999999996</v>
       </c>
-      <c r="G55" s="20"/>
-      <c r="H55" s="19">
+      <c r="G60" s="20"/>
+      <c r="H60" s="19">
         <v>0.38850000000000001</v>
       </c>
-      <c r="I55" s="21"/>
-      <c r="J55" s="19">
+      <c r="I60" s="21"/>
+      <c r="J60" s="19">
         <v>0.49130000000000001</v>
       </c>
-      <c r="K55" s="19">
+      <c r="K60" s="19">
         <v>0.87970000000000004</v>
       </c>
-      <c r="L55" s="19">
+      <c r="L60" s="19">
         <v>0.93069999999999997</v>
       </c>
-      <c r="M55" s="19"/>
-      <c r="N55" s="19">
+      <c r="M60" s="19"/>
+      <c r="N60" s="19">
         <v>0.41320000000000001</v>
       </c>
-      <c r="O55" s="21"/>
-      <c r="P55" s="19">
+      <c r="O60" s="21"/>
+      <c r="P60" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="Q55" s="19">
+      <c r="Q60" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="R55" s="19">
+      <c r="R60" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="S55" s="22"/>
-      <c r="T55" s="23">
+      <c r="S60" s="22"/>
+      <c r="T60" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="60" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C60" t="s">
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="61" spans="3:20" x14ac:dyDescent="0.25">
-      <c r="C61" t="s">
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add ways to use prot in 1st layer
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dat\Documents\GitHub\BertGOAnnotation\SeeAttention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\BertGOAnnotation\SeeAttention\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="359" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="109">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -344,15 +344,24 @@
   </si>
   <si>
     <t>2embPpiAnnotE256H1L12I768Set0/BertAve12Ep10e12Drop0.1Lr5e5None</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I512Set0/NoPpiEp10e10Drop0.1</t>
+  </si>
+  <si>
+    <t>no init GO encoder</t>
+  </si>
+  <si>
+    <t>No type emb</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -525,7 +534,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="168" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -809,10 +818,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:T66"/>
+  <dimension ref="A4:U73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,125 +829,129 @@
     <col min="1" max="1" width="25.7109375" customWidth="1"/>
     <col min="2" max="2" width="0" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="9.140625" customWidth="1"/>
-    <col min="7" max="8" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
-    <col min="19" max="20" width="0" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="26.140625" customWidth="1"/>
+    <col min="5" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="0" hidden="1" customWidth="1"/>
+    <col min="20" max="21" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" s="1"/>
+      <c r="E4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="1"/>
+      <c r="K4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="1"/>
       <c r="L4" s="1"/>
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-      <c r="P4" s="1" t="s">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U4" s="1"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
-      <c r="D5" s="1" t="s">
+      <c r="D5" s="1"/>
+      <c r="E5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1" t="s">
+      <c r="G5" s="1"/>
+      <c r="H5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H5" s="1"/>
       <c r="I5" s="1"/>
-      <c r="J5" s="1" t="s">
+      <c r="J5" s="1"/>
+      <c r="K5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K5" s="1" t="s">
+      <c r="L5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="L5" s="2"/>
-      <c r="M5" s="1" t="s">
+      <c r="M5" s="2"/>
+      <c r="N5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="N5" s="2"/>
       <c r="O5" s="2"/>
-      <c r="P5" s="1" t="s">
+      <c r="P5" s="2"/>
+      <c r="Q5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="Q5" s="1" t="s">
+      <c r="R5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="R5" s="1"/>
-      <c r="S5" s="1" t="s">
+      <c r="S5" s="1"/>
+      <c r="T5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T5" s="1"/>
-    </row>
-    <row r="6" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="1"/>
+    </row>
+    <row r="6" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="25"/>
+      <c r="E6" s="26">
         <v>0.34050000000000002</v>
       </c>
-      <c r="E6" s="26">
+      <c r="F6" s="26">
         <v>0.62670000000000003</v>
       </c>
-      <c r="F6" s="26">
+      <c r="G6" s="26">
         <v>0.81889999999999996</v>
       </c>
-      <c r="G6" s="26"/>
-      <c r="H6" s="26">
+      <c r="H6" s="26"/>
+      <c r="I6" s="26">
         <v>0.23710000000000001</v>
       </c>
-      <c r="I6" s="27"/>
-      <c r="J6" s="26">
+      <c r="J6" s="27"/>
+      <c r="K6" s="26">
         <v>0.38629999999999998</v>
       </c>
-      <c r="K6" s="26">
+      <c r="L6" s="26">
         <v>0.72419999999999995</v>
       </c>
-      <c r="L6" s="26">
+      <c r="M6" s="26">
         <v>0.86729999999999996</v>
       </c>
-      <c r="M6" s="26"/>
-      <c r="N6" s="26">
+      <c r="N6" s="26"/>
+      <c r="O6" s="26">
         <v>0.25840000000000002</v>
       </c>
-      <c r="O6" s="27"/>
-      <c r="P6" s="26">
+      <c r="P6" s="27"/>
+      <c r="Q6" s="26">
         <v>0.57199999999999995</v>
       </c>
-      <c r="Q6" s="26">
+      <c r="R6" s="26">
         <v>0.67010000000000003</v>
       </c>
-      <c r="R6" s="26">
+      <c r="S6" s="26">
         <v>0.92390000000000005</v>
       </c>
-      <c r="S6" s="26"/>
-      <c r="T6" s="26">
+      <c r="T6" s="26"/>
+      <c r="U6" s="26">
         <v>0.51829999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>21</v>
       </c>
@@ -946,43 +959,44 @@
         <v>22</v>
       </c>
       <c r="C7" s="25"/>
-      <c r="D7" s="26">
+      <c r="D7" s="25"/>
+      <c r="E7" s="26">
         <v>0.34649999999999997</v>
       </c>
-      <c r="E7" s="26">
+      <c r="F7" s="26">
         <v>0.64170000000000005</v>
       </c>
-      <c r="F7" s="26">
+      <c r="G7" s="26">
         <v>0.83460000000000001</v>
       </c>
-      <c r="G7" s="26"/>
       <c r="H7" s="26"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="26">
+      <c r="I7" s="26"/>
+      <c r="J7" s="27"/>
+      <c r="K7" s="26">
         <v>0.39579999999999999</v>
       </c>
-      <c r="K7" s="26">
+      <c r="L7" s="26">
         <v>0.76959999999999995</v>
       </c>
-      <c r="L7" s="26">
+      <c r="M7" s="26">
         <v>0.89039999999999997</v>
       </c>
-      <c r="M7" s="26"/>
       <c r="N7" s="26"/>
-      <c r="O7" s="27"/>
-      <c r="P7" s="26">
+      <c r="O7" s="26"/>
+      <c r="P7" s="27"/>
+      <c r="Q7" s="26">
         <v>0.57369999999999999</v>
       </c>
-      <c r="Q7" s="26">
+      <c r="R7" s="26">
         <v>0.67589999999999995</v>
       </c>
-      <c r="R7" s="26">
+      <c r="S7" s="26">
         <v>0.92869999999999997</v>
       </c>
-      <c r="S7" s="26"/>
       <c r="T7" s="26"/>
-    </row>
-    <row r="8" spans="1:20" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="26"/>
+    </row>
+    <row r="8" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>25</v>
       </c>
@@ -990,37 +1004,38 @@
         <v>20</v>
       </c>
       <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
+      <c r="D8" s="5"/>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="6">
+      <c r="I8" s="6"/>
+      <c r="J8" s="7"/>
+      <c r="K8" s="6">
         <v>0.38469999999999999</v>
       </c>
-      <c r="K8" s="6">
+      <c r="L8" s="6">
         <v>0.77070000000000005</v>
       </c>
-      <c r="L8" s="6">
+      <c r="M8" s="6">
         <v>0.88870000000000005</v>
       </c>
-      <c r="M8" s="6"/>
       <c r="N8" s="6"/>
-      <c r="O8" s="7"/>
-      <c r="P8" s="6">
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="6">
         <v>0.60209999999999997</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="R8" s="6">
         <v>0.75190000000000001</v>
       </c>
-      <c r="R8" s="6">
+      <c r="S8" s="6">
         <v>0.94389999999999996</v>
       </c>
-      <c r="S8" s="6"/>
       <c r="T8" s="6"/>
-    </row>
-    <row r="9" spans="1:20" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="6"/>
+    </row>
+    <row r="9" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>25</v>
       </c>
@@ -1028,134 +1043,138 @@
         <v>18</v>
       </c>
       <c r="C9" s="5"/>
-      <c r="D9" s="6">
+      <c r="D9" s="5"/>
+      <c r="E9" s="6">
         <v>0.37890000000000001</v>
       </c>
-      <c r="E9" s="6">
+      <c r="F9" s="6">
         <v>0.71919999999999995</v>
       </c>
-      <c r="F9" s="6">
+      <c r="G9" s="6">
         <v>0.8518</v>
       </c>
-      <c r="G9" s="6"/>
       <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="6">
+      <c r="I9" s="6"/>
+      <c r="J9" s="7"/>
+      <c r="K9" s="6">
         <v>0.38790000000000002</v>
       </c>
-      <c r="K9" s="6">
+      <c r="L9" s="6">
         <v>0.77239999999999998</v>
       </c>
-      <c r="L9" s="6">
+      <c r="M9" s="6">
         <v>0.88349999999999995</v>
       </c>
-      <c r="M9" s="6"/>
       <c r="N9" s="6"/>
-      <c r="O9" s="7"/>
-      <c r="P9" s="6">
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="6">
         <v>0.59709999999999996</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="R9" s="6">
         <v>0.74370000000000003</v>
       </c>
-      <c r="R9" s="6">
+      <c r="S9" s="6">
         <v>0.93920000000000003</v>
       </c>
-      <c r="S9" s="6"/>
       <c r="T9" s="6"/>
-    </row>
-    <row r="10" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>27</v>
       </c>
       <c r="B10" s="29"/>
       <c r="C10" s="30"/>
-      <c r="D10" s="26"/>
+      <c r="D10" s="30"/>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
       <c r="G10" s="26"/>
       <c r="H10" s="26"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="26" t="s">
+      <c r="I10" s="26"/>
+      <c r="J10" s="27"/>
+      <c r="K10" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="K10" s="26">
+      <c r="L10" s="26">
         <v>0.77729999999999999</v>
       </c>
-      <c r="L10" s="26">
+      <c r="M10" s="26">
         <v>0.89700000000000002</v>
       </c>
-      <c r="M10" s="26"/>
       <c r="N10" s="26"/>
-      <c r="O10" s="27"/>
-      <c r="P10" s="26" t="s">
+      <c r="O10" s="26"/>
+      <c r="P10" s="27"/>
+      <c r="Q10" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="Q10" s="26">
+      <c r="R10" s="26">
         <v>0.73909999999999998</v>
       </c>
-      <c r="R10" s="26">
+      <c r="S10" s="26">
         <v>0.94120000000000004</v>
       </c>
-      <c r="S10" s="26"/>
       <c r="T10" s="26"/>
-    </row>
-    <row r="11" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="26"/>
+    </row>
+    <row r="11" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>26</v>
       </c>
       <c r="C11" s="25"/>
-      <c r="D11" s="26"/>
+      <c r="D11" s="25"/>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
       <c r="G11" s="26"/>
       <c r="H11" s="26"/>
-      <c r="I11" s="27"/>
-      <c r="J11" s="31">
+      <c r="I11" s="26"/>
+      <c r="J11" s="27"/>
+      <c r="K11" s="31">
         <v>0.46839999999999998</v>
       </c>
-      <c r="K11" s="31">
+      <c r="L11" s="31">
         <v>0.86660000000000004</v>
       </c>
-      <c r="L11" s="31">
+      <c r="M11" s="31">
         <v>0.92869999999999997</v>
       </c>
-      <c r="M11" s="26"/>
       <c r="N11" s="26"/>
-      <c r="O11" s="27"/>
-      <c r="P11" s="26">
+      <c r="O11" s="26"/>
+      <c r="P11" s="27"/>
+      <c r="Q11" s="26">
         <v>0.65210000000000001</v>
       </c>
-      <c r="Q11" s="26">
+      <c r="R11" s="26">
         <v>0.89180000000000004</v>
       </c>
-      <c r="R11" s="26">
+      <c r="S11" s="26">
         <v>0.97009999999999996</v>
       </c>
-      <c r="S11" s="26"/>
       <c r="T11" s="26"/>
-    </row>
-    <row r="12" spans="1:20" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="26"/>
+    </row>
+    <row r="12" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
+      <c r="D12" s="5"/>
       <c r="E12" s="6"/>
       <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="7"/>
       <c r="K12" s="6"/>
       <c r="L12" s="6"/>
       <c r="M12" s="6"/>
       <c r="N12" s="6"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
       <c r="Q12" s="6"/>
       <c r="R12" s="6"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
-    </row>
-    <row r="13" spans="1:20" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="6"/>
+    </row>
+    <row r="13" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
@@ -1163,37 +1182,38 @@
         <v>18</v>
       </c>
       <c r="C13" s="5"/>
-      <c r="D13" s="6"/>
+      <c r="D13" s="5"/>
       <c r="E13" s="6"/>
       <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="6">
+      <c r="I13" s="6"/>
+      <c r="J13" s="7"/>
+      <c r="K13" s="6">
         <v>0.40579999999999999</v>
       </c>
-      <c r="K13" s="6">
+      <c r="L13" s="6">
         <v>0.79730000000000001</v>
       </c>
-      <c r="L13" s="6">
+      <c r="M13" s="6">
         <v>0.89429999999999998</v>
       </c>
-      <c r="M13" s="6"/>
       <c r="N13" s="6"/>
-      <c r="O13" s="7"/>
-      <c r="P13" s="6">
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="6">
         <v>0.60599999999999998</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="R13" s="6">
         <v>0.75949999999999995</v>
       </c>
-      <c r="R13" s="6">
+      <c r="S13" s="6">
         <v>0.94520000000000004</v>
       </c>
-      <c r="S13" s="6"/>
       <c r="T13" s="6"/>
-    </row>
-    <row r="14" spans="1:20" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="6"/>
+    </row>
+    <row r="14" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>19</v>
       </c>
@@ -1201,31 +1221,32 @@
         <v>20</v>
       </c>
       <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
+      <c r="D14" s="5"/>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="6">
+      <c r="I14" s="6"/>
+      <c r="J14" s="7"/>
+      <c r="K14" s="6">
         <v>0.40679999999999999</v>
       </c>
-      <c r="K14" s="6">
+      <c r="L14" s="6">
         <v>0.79210000000000003</v>
       </c>
-      <c r="L14" s="6">
+      <c r="M14" s="6">
         <v>0.8871</v>
       </c>
-      <c r="M14" s="6"/>
       <c r="N14" s="6"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="7"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
-    </row>
-    <row r="15" spans="1:20" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="6"/>
+    </row>
+    <row r="15" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>23</v>
       </c>
@@ -1233,51 +1254,53 @@
         <v>18</v>
       </c>
       <c r="C15" s="5"/>
-      <c r="D15" s="6"/>
+      <c r="D15" s="5"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="6">
+      <c r="I15" s="6"/>
+      <c r="J15" s="7"/>
+      <c r="K15" s="6">
         <v>0.41039999999999999</v>
       </c>
-      <c r="K15" s="6">
+      <c r="L15" s="6">
         <v>0.79279999999999995</v>
       </c>
-      <c r="L15" s="6">
+      <c r="M15" s="6">
         <v>0.88839999999999997</v>
       </c>
-      <c r="M15" s="6"/>
       <c r="N15" s="6"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
       <c r="Q15" s="6"/>
       <c r="R15" s="6"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
-    </row>
-    <row r="16" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="6"/>
+    </row>
+    <row r="16" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
+      <c r="D16" s="5"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="6"/>
       <c r="L16" s="6"/>
       <c r="M16" s="6"/>
       <c r="N16" s="6"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
       <c r="Q16" s="6"/>
       <c r="R16" s="6"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
-    </row>
-    <row r="17" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="6"/>
+    </row>
+    <row r="17" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>28</v>
       </c>
@@ -1285,37 +1308,38 @@
         <v>15</v>
       </c>
       <c r="C17" s="25"/>
-      <c r="D17" s="26"/>
+      <c r="D17" s="25"/>
       <c r="E17" s="26"/>
       <c r="F17" s="26"/>
       <c r="G17" s="26"/>
       <c r="H17" s="26"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="26">
+      <c r="I17" s="26"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="26">
         <v>0.41120000000000001</v>
       </c>
-      <c r="K17" s="26">
+      <c r="L17" s="26">
         <v>0.80179999999999996</v>
       </c>
-      <c r="L17" s="26">
+      <c r="M17" s="26">
         <v>0.89929999999999999</v>
       </c>
-      <c r="M17" s="26"/>
       <c r="N17" s="26"/>
-      <c r="O17" s="27"/>
-      <c r="P17" s="26">
+      <c r="O17" s="26"/>
+      <c r="P17" s="27"/>
+      <c r="Q17" s="26">
         <v>0.58860000000000001</v>
       </c>
-      <c r="Q17" s="26">
+      <c r="R17" s="26">
         <v>0.75490000000000002</v>
       </c>
-      <c r="R17" s="26">
+      <c r="S17" s="26">
         <v>0.94579999999999997</v>
       </c>
-      <c r="S17" s="26"/>
       <c r="T17" s="26"/>
-    </row>
-    <row r="18" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="26"/>
+    </row>
+    <row r="18" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>30</v>
       </c>
@@ -1323,46 +1347,48 @@
         <v>15</v>
       </c>
       <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
+      <c r="D18" s="5"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="7"/>
       <c r="K18" s="6"/>
       <c r="L18" s="6"/>
       <c r="M18" s="6"/>
       <c r="N18" s="6"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="7"/>
       <c r="Q18" s="6"/>
       <c r="R18" s="6"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
-    </row>
-    <row r="19" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U18" s="6"/>
+    </row>
+    <row r="19" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
-      <c r="D19" s="6"/>
+      <c r="D19" s="5"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="7"/>
       <c r="K19" s="6"/>
       <c r="L19" s="6"/>
       <c r="M19" s="6"/>
       <c r="N19" s="6"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
       <c r="Q19" s="6"/>
       <c r="R19" s="6"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
-    </row>
-    <row r="20" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="6"/>
+    </row>
+    <row r="20" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>29</v>
       </c>
@@ -1370,1300 +1396,1508 @@
         <v>15</v>
       </c>
       <c r="C20" s="25"/>
-      <c r="D20" s="26"/>
+      <c r="D20" s="25"/>
       <c r="E20" s="26"/>
       <c r="F20" s="26"/>
       <c r="G20" s="26"/>
       <c r="H20" s="26"/>
-      <c r="I20" s="27"/>
-      <c r="J20" s="26">
+      <c r="I20" s="26"/>
+      <c r="J20" s="27"/>
+      <c r="K20" s="26">
         <v>0.502</v>
       </c>
-      <c r="K20" s="26">
+      <c r="L20" s="26">
         <v>0.88660000000000005</v>
       </c>
-      <c r="L20" s="26">
+      <c r="M20" s="26">
         <v>0.93840000000000001</v>
       </c>
-      <c r="M20" s="26"/>
       <c r="N20" s="26"/>
-      <c r="O20" s="27"/>
-      <c r="P20" s="26">
+      <c r="O20" s="26"/>
+      <c r="P20" s="27"/>
+      <c r="Q20" s="26">
         <v>0.65739999999999998</v>
       </c>
-      <c r="Q20" s="26">
+      <c r="R20" s="26">
         <v>0.90769999999999995</v>
       </c>
-      <c r="R20" s="26">
+      <c r="S20" s="26">
         <v>0.97309999999999997</v>
       </c>
-      <c r="S20" s="26"/>
       <c r="T20" s="26"/>
-    </row>
-    <row r="21" spans="1:20" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U20" s="26"/>
+    </row>
+    <row r="21" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>37</v>
       </c>
       <c r="B21" s="25"/>
       <c r="C21" s="25"/>
-      <c r="D21" s="26"/>
+      <c r="D21" s="25"/>
       <c r="E21" s="26"/>
       <c r="F21" s="26"/>
       <c r="G21" s="26"/>
       <c r="H21" s="26"/>
-      <c r="I21" s="27"/>
-      <c r="J21" s="26">
+      <c r="I21" s="26"/>
+      <c r="J21" s="27"/>
+      <c r="K21" s="26">
         <v>0.50470000000000004</v>
       </c>
-      <c r="K21" s="26">
+      <c r="L21" s="26">
         <v>0.88619999999999999</v>
       </c>
-      <c r="L21" s="26">
+      <c r="M21" s="26">
         <v>0.94006000000000001</v>
       </c>
-      <c r="M21" s="26"/>
       <c r="N21" s="26"/>
-      <c r="O21" s="27"/>
-      <c r="P21" s="26"/>
+      <c r="O21" s="26"/>
+      <c r="P21" s="27"/>
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
-    </row>
-    <row r="22" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="26"/>
+    </row>
+    <row r="22" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
+      <c r="D22" s="5"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
       <c r="G22" s="6"/>
       <c r="H22" s="6"/>
-      <c r="I22" s="7"/>
-      <c r="J22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="7"/>
       <c r="K22" s="6"/>
       <c r="L22" s="6"/>
       <c r="M22" s="6"/>
       <c r="N22" s="6"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="6"/>
+      <c r="O22" s="6"/>
+      <c r="P22" s="7"/>
       <c r="Q22" s="6"/>
       <c r="R22" s="6"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
-    </row>
-    <row r="23" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="6"/>
+    </row>
+    <row r="23" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>32</v>
       </c>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
-      <c r="D23" s="6"/>
+      <c r="D23" s="5"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
       <c r="G23" s="6"/>
       <c r="H23" s="6"/>
-      <c r="I23" s="7"/>
-      <c r="J23" s="6">
+      <c r="I23" s="6"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="6">
         <v>0.50919999999999999</v>
       </c>
-      <c r="K23" s="6">
+      <c r="L23" s="6">
         <v>0.8871</v>
       </c>
-      <c r="L23" s="6">
+      <c r="M23" s="6">
         <v>0.93799999999999994</v>
       </c>
-      <c r="M23" s="6"/>
       <c r="N23" s="6"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="6"/>
+      <c r="O23" s="6"/>
+      <c r="P23" s="7"/>
       <c r="Q23" s="6"/>
       <c r="R23" s="6"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
-    </row>
-    <row r="24" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="6"/>
+    </row>
+    <row r="24" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="6"/>
       <c r="F24" s="6"/>
       <c r="G24" s="6"/>
       <c r="H24" s="6"/>
-      <c r="I24" s="7"/>
-      <c r="J24" s="6"/>
+      <c r="I24" s="6"/>
+      <c r="J24" s="7"/>
       <c r="K24" s="6"/>
       <c r="L24" s="6"/>
       <c r="M24" s="6"/>
       <c r="N24" s="6"/>
-      <c r="O24" s="7"/>
-      <c r="P24" s="6"/>
+      <c r="O24" s="6"/>
+      <c r="P24" s="7"/>
       <c r="Q24" s="6"/>
       <c r="R24" s="6"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
-    </row>
-    <row r="25" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U24" s="6"/>
+    </row>
+    <row r="25" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>36</v>
       </c>
       <c r="B25" s="5"/>
       <c r="C25" s="5"/>
-      <c r="D25" s="6"/>
+      <c r="D25" s="5"/>
       <c r="E25" s="6"/>
       <c r="F25" s="6"/>
       <c r="G25" s="6"/>
       <c r="H25" s="6"/>
-      <c r="I25" s="7"/>
-      <c r="J25" s="6">
+      <c r="I25" s="6"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="6">
         <v>0.49408999999999997</v>
       </c>
-      <c r="K25" s="6">
+      <c r="L25" s="6">
         <v>0.88570000000000004</v>
       </c>
-      <c r="L25" s="6">
+      <c r="M25" s="6">
         <v>0.93967000000000001</v>
       </c>
-      <c r="M25" s="6"/>
       <c r="N25" s="6"/>
-      <c r="O25" s="7"/>
-      <c r="P25" s="6"/>
+      <c r="O25" s="6"/>
+      <c r="P25" s="7"/>
       <c r="Q25" s="6"/>
       <c r="R25" s="6"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
-    </row>
-    <row r="26" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U25" s="6"/>
+    </row>
+    <row r="26" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="5"/>
       <c r="E26" s="6"/>
       <c r="F26" s="6"/>
       <c r="G26" s="6"/>
       <c r="H26" s="6"/>
-      <c r="I26" s="7"/>
-      <c r="J26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="7"/>
       <c r="K26" s="6"/>
       <c r="L26" s="6"/>
       <c r="M26" s="6"/>
       <c r="N26" s="6"/>
-      <c r="O26" s="7"/>
-      <c r="P26" s="6"/>
+      <c r="O26" s="6"/>
+      <c r="P26" s="7"/>
       <c r="Q26" s="6"/>
       <c r="R26" s="6"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
-    </row>
-    <row r="27" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U26" s="6"/>
+    </row>
+    <row r="27" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>38</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
-      <c r="D27" s="6"/>
+      <c r="D27" s="5"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
       <c r="G27" s="6"/>
       <c r="H27" s="6"/>
-      <c r="I27" s="7"/>
-      <c r="J27" s="6">
+      <c r="I27" s="6"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="6">
         <v>0.50070000000000003</v>
       </c>
-      <c r="K27" s="6">
+      <c r="L27" s="6">
         <v>0.88312000000000002</v>
       </c>
-      <c r="L27" s="6">
+      <c r="M27" s="6">
         <v>0.93794</v>
       </c>
-      <c r="M27" s="6"/>
       <c r="N27" s="6"/>
-      <c r="O27" s="7"/>
-      <c r="P27" s="6"/>
+      <c r="O27" s="6"/>
+      <c r="P27" s="7"/>
       <c r="Q27" s="6"/>
       <c r="R27" s="6"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
-    </row>
-    <row r="28" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U27" s="6"/>
+    </row>
+    <row r="28" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
+      <c r="D28" s="5"/>
       <c r="E28" s="6"/>
       <c r="F28" s="6"/>
       <c r="G28" s="6"/>
       <c r="H28" s="6"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="7"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
       <c r="M28" s="6"/>
       <c r="N28" s="6"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="6"/>
+      <c r="O28" s="6"/>
+      <c r="P28" s="7"/>
       <c r="Q28" s="6"/>
       <c r="R28" s="6"/>
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
-    </row>
-    <row r="29" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="28" t="s">
-        <v>99</v>
-      </c>
+      <c r="U28" s="6"/>
+    </row>
+    <row r="29" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
-      <c r="D29" s="6"/>
+      <c r="D29" s="5"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="6"/>
       <c r="H29" s="6"/>
-      <c r="I29" s="7"/>
-      <c r="J29" s="6">
-        <v>0.51929999999999998</v>
-      </c>
-      <c r="K29" s="6">
-        <v>0.89648000000000005</v>
-      </c>
-      <c r="L29" s="6">
-        <v>0.94398000000000004</v>
-      </c>
+      <c r="I29" s="6"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="6"/>
       <c r="M29" s="6"/>
       <c r="N29" s="6"/>
-      <c r="O29" s="7"/>
-      <c r="P29" s="6"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="7"/>
       <c r="Q29" s="6"/>
       <c r="R29" s="6"/>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
-    </row>
-    <row r="30" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U29" s="6"/>
+    </row>
+    <row r="30" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="6">
-        <v>0.43213083677139902</v>
-      </c>
-      <c r="E30" s="6">
-        <v>0.83454316071685597</v>
-      </c>
-      <c r="F30" s="6">
-        <v>0.90633091683560396</v>
-      </c>
+      <c r="D30" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
       <c r="G30" s="6"/>
       <c r="H30" s="6"/>
-      <c r="I30" s="7"/>
-      <c r="J30" s="6">
-        <v>0.52579759999999998</v>
-      </c>
+      <c r="I30" s="6"/>
+      <c r="J30" s="7"/>
       <c r="K30" s="6">
-        <v>0.8861</v>
+        <v>0.43413721381438802</v>
       </c>
       <c r="L30" s="6">
-        <v>0.93849190000000005</v>
-      </c>
-      <c r="M30" s="6"/>
+        <v>0.84059518185658699</v>
+      </c>
+      <c r="M30" s="6">
+        <v>0.92174507542770701</v>
+      </c>
       <c r="N30" s="6"/>
-      <c r="O30" s="7"/>
-      <c r="P30" s="6"/>
+      <c r="O30" s="6"/>
+      <c r="P30" s="7" t="s">
+        <v>107</v>
+      </c>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
       <c r="S30" s="6"/>
       <c r="T30" s="6"/>
-    </row>
-    <row r="31" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="28" t="s">
-        <v>101</v>
-      </c>
+      <c r="U30" s="6"/>
+    </row>
+    <row r="31" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="6"/>
+      <c r="D31" s="5"/>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
-      <c r="I31" s="7"/>
-      <c r="J31" s="6">
-        <v>0.51198109999999997</v>
-      </c>
-      <c r="K31" s="6">
-        <v>0.89452399999999999</v>
-      </c>
-      <c r="L31" s="6">
-        <v>0.94331580000000004</v>
-      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="6"/>
       <c r="M31" s="6"/>
       <c r="N31" s="6"/>
-      <c r="O31" s="7"/>
-      <c r="P31" s="6"/>
+      <c r="O31" s="6"/>
+      <c r="P31" s="7"/>
       <c r="Q31" s="6"/>
       <c r="R31" s="6"/>
       <c r="S31" s="6"/>
       <c r="T31" s="6"/>
-    </row>
-    <row r="32" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U31" s="6"/>
+    </row>
+    <row r="32" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="5"/>
       <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
+      <c r="D32" s="5"/>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
-      <c r="I32" s="7"/>
-      <c r="J32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="7"/>
       <c r="K32" s="6"/>
       <c r="L32" s="6"/>
       <c r="M32" s="6"/>
       <c r="N32" s="6"/>
-      <c r="O32" s="7"/>
-      <c r="P32" s="6"/>
+      <c r="O32" s="6"/>
+      <c r="P32" s="7"/>
       <c r="Q32" s="6"/>
       <c r="R32" s="6"/>
       <c r="S32" s="6"/>
       <c r="T32" s="6"/>
-    </row>
-    <row r="33" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
-        <v>102</v>
-      </c>
+      <c r="U32" s="6"/>
+    </row>
+    <row r="33" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D33" s="6">
-        <v>0.43916617238933098</v>
-      </c>
-      <c r="E33" s="6">
-        <v>0.835605451873769</v>
-      </c>
-      <c r="F33" s="6">
-        <v>0.90752296578104596</v>
-      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
       <c r="G33" s="6"/>
       <c r="H33" s="6"/>
-      <c r="I33" s="7"/>
-      <c r="J33" s="40">
-        <v>0.5309239</v>
-      </c>
-      <c r="K33" s="40">
-        <v>0.892953</v>
-      </c>
-      <c r="L33" s="40">
-        <v>0.94298300000000002</v>
-      </c>
+      <c r="I33" s="6"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="6"/>
       <c r="M33" s="6"/>
       <c r="N33" s="6"/>
-      <c r="O33" s="39">
-        <v>4.1920459275095398E-2</v>
-      </c>
-      <c r="P33" s="6">
-        <v>0.66610357651026797</v>
-      </c>
-      <c r="Q33" s="6">
-        <v>0.90778748640305595</v>
-      </c>
-      <c r="R33" s="6">
-        <v>0.97222662155700101</v>
-      </c>
+      <c r="O33" s="6"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="6"/>
+      <c r="R33" s="6"/>
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
-    </row>
-    <row r="34" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
-        <v>102</v>
-      </c>
+      <c r="U33" s="6"/>
+    </row>
+    <row r="34" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
-      <c r="C34" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="D34" s="6"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
       <c r="E34" s="6"/>
       <c r="F34" s="6"/>
       <c r="G34" s="6"/>
       <c r="H34" s="6"/>
-      <c r="I34" s="7"/>
-      <c r="J34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="7"/>
       <c r="K34" s="6"/>
       <c r="L34" s="6"/>
       <c r="M34" s="6"/>
       <c r="N34" s="6"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="6">
-        <v>0.66219899999999998</v>
-      </c>
-      <c r="Q34" s="6">
-        <v>0.90361093533127401</v>
-      </c>
-      <c r="R34" s="6">
-        <v>0.97134283099715801</v>
-      </c>
+      <c r="O34" s="6"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="6"/>
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
-    </row>
-    <row r="35" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U34" s="6"/>
+    </row>
+    <row r="35" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
-      <c r="D35" s="6"/>
+      <c r="D35" s="5"/>
       <c r="E35" s="6"/>
       <c r="F35" s="6"/>
       <c r="G35" s="6"/>
       <c r="H35" s="6"/>
-      <c r="I35" s="7"/>
-      <c r="J35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="7"/>
       <c r="K35" s="6"/>
       <c r="L35" s="6"/>
       <c r="M35" s="6"/>
       <c r="N35" s="6"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="6"/>
+      <c r="O35" s="6"/>
+      <c r="P35" s="7"/>
       <c r="Q35" s="6"/>
       <c r="R35" s="6"/>
       <c r="S35" s="6"/>
       <c r="T35" s="6"/>
-    </row>
-    <row r="36" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U35" s="6"/>
+    </row>
+    <row r="36" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="B36" s="5"/>
-      <c r="C36" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D36" s="6"/>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
       <c r="G36" s="6"/>
       <c r="H36" s="6"/>
-      <c r="I36" s="7"/>
-      <c r="J36" s="6">
-        <v>0.520983673424954</v>
-      </c>
+      <c r="I36" s="6"/>
+      <c r="J36" s="7"/>
       <c r="K36" s="6">
-        <v>0.89486151979039896</v>
+        <v>0.51929999999999998</v>
       </c>
       <c r="L36" s="6">
-        <v>0.93774798228002598</v>
-      </c>
-      <c r="M36" s="6"/>
+        <v>0.89648000000000005</v>
+      </c>
+      <c r="M36" s="6">
+        <v>0.94398000000000004</v>
+      </c>
       <c r="N36" s="6"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="6"/>
+      <c r="O36" s="6"/>
+      <c r="P36" s="7"/>
       <c r="Q36" s="6"/>
       <c r="R36" s="6"/>
       <c r="S36" s="6"/>
       <c r="T36" s="6"/>
-    </row>
-    <row r="37" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U36" s="6"/>
+    </row>
+    <row r="37" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
+        <v>100</v>
+      </c>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="6">
+        <v>0.43213083677139902</v>
+      </c>
+      <c r="F37" s="6">
+        <v>0.83454316071685597</v>
+      </c>
+      <c r="G37" s="6">
+        <v>0.90633091683560396</v>
+      </c>
       <c r="H37" s="6"/>
-      <c r="I37" s="7"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
-      <c r="L37" s="6"/>
-      <c r="M37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="6">
+        <v>0.52579759999999998</v>
+      </c>
+      <c r="L37" s="6">
+        <v>0.8861</v>
+      </c>
+      <c r="M37" s="6">
+        <v>0.93849190000000005</v>
+      </c>
       <c r="N37" s="6"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="6"/>
+      <c r="O37" s="6"/>
+      <c r="P37" s="7"/>
       <c r="Q37" s="6"/>
       <c r="R37" s="6"/>
       <c r="S37" s="6"/>
       <c r="T37" s="6"/>
-    </row>
-    <row r="38" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U37" s="6"/>
+    </row>
+    <row r="38" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B38" s="5"/>
       <c r="C38" s="5"/>
-      <c r="D38" s="6"/>
+      <c r="D38" s="5"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
       <c r="H38" s="6"/>
-      <c r="I38" s="7"/>
-      <c r="J38" s="6">
-        <v>0.51423909004761503</v>
-      </c>
+      <c r="I38" s="6"/>
+      <c r="J38" s="7"/>
       <c r="K38" s="6">
-        <v>0.88734048870237103</v>
+        <v>0.51198109999999997</v>
       </c>
       <c r="L38" s="6">
-        <v>0.93880771591373202</v>
-      </c>
-      <c r="M38" s="6"/>
+        <v>0.89452399999999999</v>
+      </c>
+      <c r="M38" s="6">
+        <v>0.94331580000000004</v>
+      </c>
       <c r="N38" s="6"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="6"/>
+      <c r="O38" s="6"/>
+      <c r="P38" s="7"/>
       <c r="Q38" s="6"/>
       <c r="R38" s="6"/>
       <c r="S38" s="6"/>
       <c r="T38" s="6"/>
-    </row>
-    <row r="39" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U38" s="6"/>
+    </row>
+    <row r="39" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
-      <c r="D39" s="6"/>
+      <c r="D39" s="5"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
       <c r="H39" s="6"/>
-      <c r="I39" s="7"/>
-      <c r="J39" s="6">
-        <v>0.51169393197777102</v>
-      </c>
-      <c r="K39" s="6">
-        <v>0.89076338804911404</v>
-      </c>
-      <c r="L39" s="6">
-        <v>0.94032778400047801</v>
-      </c>
+      <c r="I39" s="6"/>
+      <c r="J39" s="7"/>
+      <c r="K39" s="6"/>
+      <c r="L39" s="6"/>
       <c r="M39" s="6"/>
       <c r="N39" s="6"/>
-      <c r="O39" s="39">
-        <v>4.2612862119596799E-2</v>
-      </c>
-      <c r="P39" s="6"/>
+      <c r="O39" s="6"/>
+      <c r="P39" s="7"/>
       <c r="Q39" s="6"/>
       <c r="R39" s="6"/>
       <c r="S39" s="6"/>
       <c r="T39" s="6"/>
-    </row>
-    <row r="40" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U39" s="6"/>
+    </row>
+    <row r="40" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="B40" s="5"/>
-      <c r="C40" s="5"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
+      <c r="C40" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D40" s="5"/>
+      <c r="E40" s="6">
+        <v>0.43916617238933098</v>
+      </c>
+      <c r="F40" s="6">
+        <v>0.835605451873769</v>
+      </c>
+      <c r="G40" s="6">
+        <v>0.90752296578104596</v>
+      </c>
       <c r="H40" s="6"/>
-      <c r="I40" s="7"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
-      <c r="L40" s="6"/>
-      <c r="M40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="7"/>
+      <c r="K40" s="40">
+        <v>0.5309239</v>
+      </c>
+      <c r="L40" s="40">
+        <v>0.892953</v>
+      </c>
+      <c r="M40" s="40">
+        <v>0.94298300000000002</v>
+      </c>
       <c r="N40" s="6"/>
-      <c r="O40" s="7"/>
-      <c r="P40" s="6"/>
-      <c r="Q40" s="6"/>
-      <c r="R40" s="6"/>
-      <c r="S40" s="6"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="39">
+        <v>4.1920459275095398E-2</v>
+      </c>
+      <c r="Q40" s="6">
+        <v>0.66610357651026797</v>
+      </c>
+      <c r="R40" s="6">
+        <v>0.90778748640305595</v>
+      </c>
+      <c r="S40" s="6">
+        <v>0.97222662155700101</v>
+      </c>
       <c r="T40" s="6"/>
-    </row>
-    <row r="41" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U40" s="6"/>
+    </row>
+    <row r="41" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="28" t="s">
+        <v>102</v>
+      </c>
       <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="6"/>
+      <c r="C41" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D41" s="5"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
       <c r="G41" s="6"/>
       <c r="H41" s="6"/>
-      <c r="I41" s="7"/>
-      <c r="J41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="7"/>
       <c r="K41" s="6"/>
       <c r="L41" s="6"/>
       <c r="M41" s="6"/>
       <c r="N41" s="6"/>
-      <c r="O41" s="7"/>
-      <c r="P41" s="6"/>
-      <c r="Q41" s="6"/>
-      <c r="R41" s="6"/>
-      <c r="S41" s="6"/>
+      <c r="O41" s="6"/>
+      <c r="P41" s="7"/>
+      <c r="Q41" s="6">
+        <v>0.66219899999999998</v>
+      </c>
+      <c r="R41" s="6">
+        <v>0.90361093533127401</v>
+      </c>
+      <c r="S41" s="6">
+        <v>0.97134283099715801</v>
+      </c>
       <c r="T41" s="6"/>
-    </row>
-    <row r="42" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U41" s="6"/>
+    </row>
+    <row r="42" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
+      <c r="D42" s="5"/>
       <c r="E42" s="6"/>
       <c r="F42" s="6"/>
       <c r="G42" s="6"/>
       <c r="H42" s="6"/>
-      <c r="I42" s="7"/>
-      <c r="J42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="7"/>
       <c r="K42" s="6"/>
       <c r="L42" s="6"/>
       <c r="M42" s="6"/>
       <c r="N42" s="6"/>
-      <c r="O42" s="7"/>
-      <c r="P42" s="6"/>
+      <c r="O42" s="6"/>
+      <c r="P42" s="7"/>
       <c r="Q42" s="6"/>
       <c r="R42" s="6"/>
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
-    </row>
-    <row r="43" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U42" s="6"/>
+    </row>
+    <row r="43" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="28" t="s">
+        <v>103</v>
+      </c>
       <c r="B43" s="5"/>
-      <c r="C43" s="5"/>
-      <c r="D43" s="6"/>
+      <c r="C43" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" s="5"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
       <c r="H43" s="6"/>
-      <c r="I43" s="7"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="7"/>
+      <c r="K43" s="6">
+        <v>0.520983673424954</v>
+      </c>
+      <c r="L43" s="6">
+        <v>0.89486151979039896</v>
+      </c>
+      <c r="M43" s="6">
+        <v>0.93774798228002598</v>
+      </c>
       <c r="N43" s="6"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="6"/>
+      <c r="O43" s="6"/>
+      <c r="P43" s="7"/>
       <c r="Q43" s="6"/>
       <c r="R43" s="6"/>
       <c r="S43" s="6"/>
       <c r="T43" s="6"/>
-    </row>
-    <row r="44" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="28" t="s">
-        <v>96</v>
-      </c>
+      <c r="U43" s="6"/>
+    </row>
+    <row r="44" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
-      <c r="D44" s="6"/>
+      <c r="D44" s="5"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
       <c r="H44" s="6"/>
-      <c r="I44" s="7"/>
-      <c r="J44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="7"/>
       <c r="K44" s="6"/>
       <c r="L44" s="6"/>
       <c r="M44" s="6"/>
       <c r="N44" s="6"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="6">
-        <v>0.66569299999999998</v>
-      </c>
-      <c r="Q44" s="6">
-        <v>0.90422999999999998</v>
-      </c>
-      <c r="R44" s="6">
-        <v>0.97198600000000002</v>
-      </c>
+      <c r="O44" s="6"/>
+      <c r="P44" s="7"/>
+      <c r="Q44" s="6"/>
+      <c r="R44" s="6"/>
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
-    </row>
-    <row r="45" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U44" s="6"/>
+    </row>
+    <row r="45" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="28" t="s">
+        <v>105</v>
+      </c>
       <c r="B45" s="5"/>
       <c r="C45" s="5"/>
-      <c r="D45" s="6"/>
+      <c r="D45" s="5"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
       <c r="H45" s="6"/>
-      <c r="I45" s="7"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
-      <c r="M45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="6">
+        <v>0.51423909004761503</v>
+      </c>
+      <c r="L45" s="6">
+        <v>0.88734048870237103</v>
+      </c>
+      <c r="M45" s="6">
+        <v>0.93880771591373202</v>
+      </c>
       <c r="N45" s="6"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="6"/>
+      <c r="O45" s="6"/>
+      <c r="P45" s="7"/>
       <c r="Q45" s="6"/>
       <c r="R45" s="6"/>
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
-    </row>
-    <row r="46" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="28" t="s">
-        <v>104</v>
-      </c>
+      <c r="U45" s="6"/>
+    </row>
+    <row r="46" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
-      <c r="D46" s="6"/>
+      <c r="D46" s="5"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
       <c r="H46" s="6"/>
-      <c r="I46" s="7"/>
-      <c r="J46" s="6">
-        <v>0.40104148966138098</v>
-      </c>
+      <c r="I46" s="6"/>
+      <c r="J46" s="7"/>
       <c r="K46" s="6">
-        <v>0.78469118831988205</v>
+        <v>0.51169393197777102</v>
       </c>
       <c r="L46" s="6">
-        <v>0.89141190674054405</v>
-      </c>
-      <c r="M46" s="6"/>
+        <v>0.89076338804911404</v>
+      </c>
+      <c r="M46" s="6">
+        <v>0.94032778400047801</v>
+      </c>
       <c r="N46" s="6"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="6">
-        <v>0.59847806990903096</v>
-      </c>
-      <c r="Q46" s="6">
-        <v>0.74540495542180496</v>
-      </c>
-      <c r="R46" s="6">
-        <v>0.94279293529049801</v>
-      </c>
+      <c r="O46" s="6"/>
+      <c r="P46" s="39">
+        <v>4.2612862119596799E-2</v>
+      </c>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
       <c r="S46" s="6"/>
       <c r="T46" s="6"/>
-    </row>
-    <row r="47" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U46" s="6"/>
+    </row>
+    <row r="47" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
-      <c r="D47" s="6"/>
+      <c r="D47" s="5"/>
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
       <c r="H47" s="6"/>
-      <c r="I47" s="7"/>
-      <c r="J47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="7"/>
       <c r="K47" s="6"/>
       <c r="L47" s="6"/>
       <c r="M47" s="6"/>
       <c r="N47" s="6"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="6"/>
+      <c r="O47" s="6"/>
+      <c r="P47" s="7"/>
       <c r="Q47" s="6"/>
       <c r="R47" s="6"/>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
-    </row>
-    <row r="48" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U47" s="6"/>
+    </row>
+    <row r="48" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
+      <c r="D48" s="5"/>
       <c r="E48" s="6"/>
       <c r="F48" s="6"/>
       <c r="G48" s="6"/>
       <c r="H48" s="6"/>
-      <c r="I48" s="7"/>
-      <c r="J48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="7"/>
       <c r="K48" s="6"/>
       <c r="L48" s="6"/>
       <c r="M48" s="6"/>
       <c r="N48" s="6"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="6"/>
+      <c r="O48" s="6"/>
+      <c r="P48" s="7"/>
       <c r="Q48" s="6"/>
       <c r="R48" s="6"/>
       <c r="S48" s="6"/>
       <c r="T48" s="6"/>
-    </row>
-    <row r="49" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="28" t="s">
-        <v>35</v>
-      </c>
+      <c r="U48" s="6"/>
+    </row>
+    <row r="49" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
+      <c r="D49" s="5"/>
       <c r="E49" s="6"/>
       <c r="F49" s="6"/>
       <c r="G49" s="6"/>
       <c r="H49" s="6"/>
-      <c r="I49" s="7"/>
-      <c r="J49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="7"/>
       <c r="K49" s="6"/>
       <c r="L49" s="6"/>
       <c r="M49" s="6"/>
       <c r="N49" s="6"/>
-      <c r="O49" s="7"/>
-      <c r="P49" s="6"/>
+      <c r="O49" s="6"/>
+      <c r="P49" s="7"/>
       <c r="Q49" s="6"/>
       <c r="R49" s="6"/>
       <c r="S49" s="6"/>
       <c r="T49" s="6"/>
-    </row>
-    <row r="50" spans="1:20" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="28" t="s">
-        <v>35</v>
-      </c>
+      <c r="U49" s="6"/>
+    </row>
+    <row r="50" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="5"/>
       <c r="C50" s="5"/>
-      <c r="D50" s="6"/>
+      <c r="D50" s="5"/>
       <c r="E50" s="6"/>
       <c r="F50" s="6"/>
       <c r="G50" s="6"/>
       <c r="H50" s="6"/>
-      <c r="I50" s="7"/>
-      <c r="J50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="7"/>
       <c r="K50" s="6"/>
       <c r="L50" s="6"/>
       <c r="M50" s="6"/>
       <c r="N50" s="6"/>
-      <c r="O50" s="7"/>
-      <c r="P50" s="6"/>
+      <c r="O50" s="6"/>
+      <c r="P50" s="7"/>
       <c r="Q50" s="6"/>
       <c r="R50" s="6"/>
       <c r="S50" s="6"/>
       <c r="T50" s="6"/>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="U50" s="6"/>
+    </row>
+    <row r="51" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="7"/>
+      <c r="Q51" s="6">
+        <v>0.66569299999999998</v>
+      </c>
+      <c r="R51" s="6">
+        <v>0.90422999999999998</v>
+      </c>
+      <c r="S51" s="6">
+        <v>0.97198600000000002</v>
+      </c>
+      <c r="T51" s="6"/>
+      <c r="U51" s="6"/>
+    </row>
+    <row r="52" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="5"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="7"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
+      <c r="O52" s="6"/>
+      <c r="P52" s="7"/>
+      <c r="Q52" s="6"/>
+      <c r="R52" s="6"/>
+      <c r="S52" s="6"/>
+      <c r="T52" s="6"/>
+      <c r="U52" s="6"/>
+    </row>
+    <row r="53" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="28" t="s">
+        <v>104</v>
+      </c>
+      <c r="B53" s="5"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="6">
+        <v>0.40104148966138098</v>
+      </c>
+      <c r="L53" s="6">
+        <v>0.78469118831988205</v>
+      </c>
+      <c r="M53" s="6">
+        <v>0.89141190674054405</v>
+      </c>
+      <c r="N53" s="6"/>
+      <c r="O53" s="6"/>
+      <c r="P53" s="7"/>
+      <c r="Q53" s="6">
+        <v>0.59847806990903096</v>
+      </c>
+      <c r="R53" s="6">
+        <v>0.74540495542180496</v>
+      </c>
+      <c r="S53" s="6">
+        <v>0.94279293529049801</v>
+      </c>
+      <c r="T53" s="6"/>
+      <c r="U53" s="6"/>
+    </row>
+    <row r="54" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="5"/>
+      <c r="C54" s="5"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="7"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
+      <c r="O54" s="6"/>
+      <c r="P54" s="7"/>
+      <c r="Q54" s="6"/>
+      <c r="R54" s="6"/>
+      <c r="S54" s="6"/>
+      <c r="T54" s="6"/>
+      <c r="U54" s="6"/>
+    </row>
+    <row r="55" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="5"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="6"/>
+      <c r="L55" s="6"/>
+      <c r="M55" s="6"/>
+      <c r="N55" s="6"/>
+      <c r="O55" s="6"/>
+      <c r="P55" s="7"/>
+      <c r="Q55" s="6"/>
+      <c r="R55" s="6"/>
+      <c r="S55" s="6"/>
+      <c r="T55" s="6"/>
+      <c r="U55" s="6"/>
+    </row>
+    <row r="56" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="C51" s="5" t="s">
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="7"/>
+      <c r="K56" s="6"/>
+      <c r="L56" s="6"/>
+      <c r="M56" s="6"/>
+      <c r="N56" s="6"/>
+      <c r="O56" s="6"/>
+      <c r="P56" s="7"/>
+      <c r="Q56" s="6"/>
+      <c r="R56" s="6"/>
+      <c r="S56" s="6"/>
+      <c r="T56" s="6"/>
+      <c r="U56" s="6"/>
+    </row>
+    <row r="57" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="6"/>
+      <c r="L57" s="6"/>
+      <c r="M57" s="6"/>
+      <c r="N57" s="6"/>
+      <c r="O57" s="6"/>
+      <c r="P57" s="7"/>
+      <c r="Q57" s="6"/>
+      <c r="R57" s="6"/>
+      <c r="S57" s="6"/>
+      <c r="T57" s="6"/>
+      <c r="U57" s="6"/>
+    </row>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="6">
+      <c r="D58" s="5"/>
+      <c r="E58" s="6">
         <v>0.41799999999999998</v>
       </c>
-      <c r="E51" s="6">
+      <c r="F58" s="6">
         <v>0.81869999999999998</v>
       </c>
-      <c r="F51" s="6">
+      <c r="G58" s="6">
         <v>0.89700000000000002</v>
       </c>
-      <c r="G51" s="6"/>
-      <c r="H51" s="6">
+      <c r="H58" s="6"/>
+      <c r="I58" s="6">
         <v>0.37009999999999998</v>
       </c>
-      <c r="I51" s="7"/>
-      <c r="J51" s="6">
+      <c r="J58" s="7"/>
+      <c r="K58" s="6">
         <v>0.4677</v>
       </c>
-      <c r="K51" s="6">
+      <c r="L58" s="6">
         <v>0.83730000000000004</v>
       </c>
-      <c r="L51" s="6">
+      <c r="M58" s="6">
         <v>0.90600000000000003</v>
       </c>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6">
+      <c r="N58" s="6"/>
+      <c r="O58" s="6">
         <v>0.3614</v>
       </c>
-      <c r="O51" s="7"/>
-      <c r="P51" s="6">
+      <c r="P58" s="7"/>
+      <c r="Q58" s="6">
         <v>0.627</v>
       </c>
-      <c r="Q51" s="6">
+      <c r="R58" s="6">
         <v>0.878</v>
       </c>
-      <c r="R51" s="6">
+      <c r="S58" s="6">
         <v>0.9647</v>
       </c>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3">
+      <c r="T58" s="3"/>
+      <c r="U58" s="3">
         <v>0.62470000000000003</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A52" s="28"/>
-      <c r="C52" s="8" t="s">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A59" s="28"/>
+      <c r="C59" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D52" s="9">
+      <c r="D59" s="8"/>
+      <c r="E59" s="9">
         <v>42.51</v>
       </c>
-      <c r="E52" s="9">
+      <c r="F59" s="9">
         <v>82.97</v>
       </c>
-      <c r="F52" s="9">
+      <c r="G59" s="9">
         <v>90.27</v>
       </c>
-      <c r="G52" s="10"/>
-      <c r="H52" s="11">
+      <c r="H59" s="10"/>
+      <c r="I59" s="11">
         <v>0.37769999999999998</v>
       </c>
-      <c r="I52" s="9"/>
-      <c r="J52" s="9">
+      <c r="J59" s="9"/>
+      <c r="K59" s="9">
         <v>48.62</v>
       </c>
-      <c r="K52" s="9">
+      <c r="L59" s="9">
         <v>87.25</v>
       </c>
-      <c r="L52" s="9">
+      <c r="M59" s="9">
         <v>93.14</v>
       </c>
-      <c r="M52" s="9"/>
-      <c r="N52" s="11">
+      <c r="N59" s="9"/>
+      <c r="O59" s="11">
         <v>0.40760000000000002</v>
       </c>
-      <c r="O52" s="9"/>
-      <c r="P52" s="9">
+      <c r="P59" s="9"/>
+      <c r="Q59" s="9">
         <v>63.77</v>
       </c>
-      <c r="Q52" s="9">
+      <c r="R59" s="9">
         <v>89.79</v>
       </c>
-      <c r="R52" s="9">
+      <c r="S59" s="9">
         <v>97.1</v>
       </c>
-      <c r="S52" s="8"/>
-      <c r="T52" s="11">
+      <c r="T59" s="8"/>
+      <c r="U59" s="11">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A53" s="28"/>
-      <c r="C53" s="12" t="s">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A60" s="28"/>
+      <c r="C60" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D53" s="13">
+      <c r="D60" s="12"/>
+      <c r="E60" s="13">
         <v>0.4365</v>
       </c>
-      <c r="E53" s="13">
+      <c r="F60" s="13">
         <v>0.83460000000000001</v>
       </c>
-      <c r="F53" s="13">
+      <c r="G60" s="13">
         <v>0.90629999999999999</v>
       </c>
-      <c r="G53" s="13"/>
-      <c r="H53" s="14">
+      <c r="H60" s="13"/>
+      <c r="I60" s="14">
         <v>0.39729999999999999</v>
       </c>
-      <c r="I53" s="15"/>
-      <c r="J53" s="13">
+      <c r="J60" s="15"/>
+      <c r="K60" s="13">
         <v>0.49740000000000001</v>
       </c>
-      <c r="K53" s="13">
+      <c r="L60" s="13">
         <v>0.87780000000000002</v>
       </c>
-      <c r="L53" s="13">
+      <c r="M60" s="13">
         <v>0.93500000000000005</v>
       </c>
-      <c r="M53" s="13"/>
-      <c r="N53" s="13">
+      <c r="N60" s="13"/>
+      <c r="O60" s="13">
         <v>0.41799999999999998</v>
       </c>
-      <c r="O53" s="15"/>
-      <c r="P53" s="13">
+      <c r="P60" s="15"/>
+      <c r="Q60" s="13">
         <v>0.65200000000000002</v>
       </c>
-      <c r="Q53" s="13">
+      <c r="R60" s="13">
         <v>0.90390000000000004</v>
       </c>
-      <c r="R53" s="13">
+      <c r="S60" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="S53" s="13"/>
-      <c r="T53" s="13">
+      <c r="T60" s="13"/>
+      <c r="U60" s="13">
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C54" s="6" t="s">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C61" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D54" s="6">
+      <c r="D61" s="6"/>
+      <c r="E61" s="6">
         <v>0.43480000000000002</v>
       </c>
-      <c r="E54" s="16">
+      <c r="F61" s="16">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F54" s="6">
+      <c r="G61" s="6">
         <v>0.9073</v>
       </c>
-      <c r="G54" s="6"/>
-      <c r="H54" s="6">
+      <c r="H61" s="6"/>
+      <c r="I61" s="6">
         <v>0.39419999999999999</v>
       </c>
-      <c r="I54" s="6"/>
-      <c r="J54" s="6">
+      <c r="J61" s="6"/>
+      <c r="K61" s="6">
         <v>0.502</v>
       </c>
-      <c r="K54" s="6">
+      <c r="L61" s="6">
         <v>0.88019999999999998</v>
       </c>
-      <c r="L54" s="16">
+      <c r="M61" s="16">
         <v>0.93840000000000001</v>
       </c>
-      <c r="M54" s="6"/>
-      <c r="N54" s="16">
+      <c r="N61" s="6"/>
+      <c r="O61" s="16">
         <v>0.43809999999999999</v>
       </c>
-      <c r="O54" s="6"/>
-      <c r="P54" s="6">
+      <c r="P61" s="6"/>
+      <c r="Q61" s="6">
         <v>0.65469999999999995</v>
       </c>
-      <c r="Q54" s="6">
+      <c r="R61" s="6">
         <v>0.90480000000000005</v>
       </c>
-      <c r="R54" s="6">
+      <c r="S61" s="6">
         <v>0.97250000000000003</v>
       </c>
-      <c r="S54" s="6"/>
-      <c r="T54" s="6">
+      <c r="T61" s="6"/>
+      <c r="U61" s="6">
         <v>0.66139999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C55" s="1" t="s">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C62" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D55" s="3">
+      <c r="D62" s="1"/>
+      <c r="E62" s="3">
         <v>0.43149999999999999</v>
       </c>
-      <c r="E55" s="3">
+      <c r="F62" s="3">
         <v>0.83409999999999995</v>
       </c>
-      <c r="F55" s="3">
+      <c r="G62" s="3">
         <v>0.90590000000000004</v>
       </c>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3">
+      <c r="H62" s="3"/>
+      <c r="I62" s="3">
         <v>0.39169999999999999</v>
       </c>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3">
+      <c r="J62" s="3"/>
+      <c r="K62" s="3">
         <v>0.49930000000000002</v>
       </c>
-      <c r="K55" s="3">
+      <c r="L62" s="3">
         <v>0.87290000000000001</v>
       </c>
-      <c r="L55" s="3">
+      <c r="M62" s="3">
         <v>0.93389999999999995</v>
       </c>
-      <c r="M55" s="3"/>
-      <c r="N55" s="3">
+      <c r="N62" s="3"/>
+      <c r="O62" s="3">
         <v>0.42930000000000001</v>
       </c>
-      <c r="O55" s="4"/>
-      <c r="P55" s="3">
+      <c r="P62" s="4"/>
+      <c r="Q62" s="3">
         <v>0.65239999999999998</v>
       </c>
-      <c r="Q55" s="17">
+      <c r="R62" s="17">
         <v>0.90569999999999995</v>
       </c>
-      <c r="R55" s="3">
+      <c r="S62" s="3">
         <v>0.97260000000000002</v>
       </c>
-      <c r="S55" s="3"/>
-      <c r="T55" s="3">
+      <c r="T62" s="3"/>
+      <c r="U62" s="3">
         <v>0.65810000000000002</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C56" s="1" t="s">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C63" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D63" s="1"/>
+      <c r="E63" s="1">
         <v>43.45</v>
       </c>
-      <c r="E56" s="1">
+      <c r="F63" s="1">
         <v>83.11</v>
       </c>
-      <c r="F56" s="1">
+      <c r="G63" s="1">
         <v>90.55</v>
       </c>
-      <c r="G56" s="18"/>
-      <c r="H56" s="3">
+      <c r="H63" s="18"/>
+      <c r="I63" s="3">
         <v>0.3896</v>
       </c>
-      <c r="I56" s="1"/>
-      <c r="J56" s="1">
+      <c r="J63" s="1"/>
+      <c r="K63" s="1">
         <v>49.24</v>
       </c>
-      <c r="K56" s="1">
+      <c r="L63" s="1">
         <v>87.43</v>
       </c>
-      <c r="L56" s="1">
+      <c r="M63" s="1">
         <v>93.52</v>
       </c>
-      <c r="M56" s="1"/>
-      <c r="N56" s="3">
+      <c r="N63" s="1"/>
+      <c r="O63" s="3">
         <v>0.42209999999999998</v>
       </c>
-      <c r="O56" s="1"/>
-      <c r="P56" s="4">
+      <c r="P63" s="1"/>
+      <c r="Q63" s="4">
         <v>65.39</v>
       </c>
-      <c r="Q56" s="1">
+      <c r="R63" s="1">
         <v>90.27</v>
       </c>
-      <c r="R56" s="4">
+      <c r="S63" s="4">
         <v>97.27</v>
       </c>
-      <c r="S56" s="1"/>
-      <c r="T56" s="3">
+      <c r="T63" s="1"/>
+      <c r="U63" s="3">
         <v>0.65659999999999996</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C57" s="1" t="s">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D57" s="3">
+      <c r="D64" s="1"/>
+      <c r="E64" s="3">
         <v>0.42909999999999998</v>
       </c>
-      <c r="E57" s="3">
+      <c r="F64" s="3">
         <v>0.83479999999999999</v>
       </c>
-      <c r="F57" s="3">
+      <c r="G64" s="3">
         <v>0.90569999999999995</v>
       </c>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3">
+      <c r="H64" s="3"/>
+      <c r="I64" s="3">
         <v>0.38979999999999998</v>
       </c>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3">
+      <c r="J64" s="3"/>
+      <c r="K64" s="3">
         <v>0.49349999999999999</v>
       </c>
-      <c r="K57" s="17">
+      <c r="L64" s="17">
         <v>0.87919999999999998</v>
       </c>
-      <c r="L57" s="3">
+      <c r="M64" s="3">
         <v>0.93830000000000002</v>
       </c>
-      <c r="M57" s="3"/>
-      <c r="N57" s="3">
+      <c r="N64" s="3"/>
+      <c r="O64" s="3">
         <v>0.43259999999999998</v>
       </c>
-      <c r="O57" s="3"/>
-      <c r="P57" s="3">
+      <c r="P64" s="3"/>
+      <c r="Q64" s="3">
         <v>0.6482</v>
       </c>
-      <c r="Q57" s="3">
+      <c r="R64" s="3">
         <v>0.90500000000000003</v>
       </c>
-      <c r="R57" s="3">
+      <c r="S64" s="3">
         <v>0.97209999999999996</v>
       </c>
-      <c r="S57" s="3"/>
-      <c r="T57" s="3">
+      <c r="T64" s="3"/>
+      <c r="U64" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C58" s="32" t="s">
+    <row r="65" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C65" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D58" s="33">
+      <c r="D65" s="32"/>
+      <c r="E65" s="33">
         <v>0.43919999999999998</v>
       </c>
-      <c r="E58" s="33">
+      <c r="F65" s="33">
         <v>0.83489999999999998</v>
       </c>
-      <c r="F58" s="33">
+      <c r="G65" s="33">
         <v>0.90769999999999995</v>
       </c>
-      <c r="G58" s="34"/>
-      <c r="H58" s="35">
+      <c r="H65" s="34"/>
+      <c r="I65" s="35">
         <v>0.39300000000000002</v>
       </c>
-      <c r="I58" s="32"/>
-      <c r="J58" s="33">
+      <c r="J65" s="32"/>
+      <c r="K65" s="33">
         <v>0.503</v>
       </c>
-      <c r="K58" s="35">
+      <c r="L65" s="35">
         <v>0.87680000000000002</v>
       </c>
-      <c r="L58" s="35">
+      <c r="M65" s="35">
         <v>0.93659999999999999</v>
       </c>
-      <c r="M58" s="35"/>
-      <c r="N58" s="35">
+      <c r="N65" s="35"/>
+      <c r="O65" s="35">
         <v>0.43430000000000002</v>
       </c>
-      <c r="O58" s="32"/>
-      <c r="P58" s="33">
+      <c r="P65" s="32"/>
+      <c r="Q65" s="33">
         <v>0.6583</v>
       </c>
-      <c r="Q58" s="35">
+      <c r="R65" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="R58" s="33">
+      <c r="S65" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="S58" s="1"/>
-      <c r="T58" s="17">
+      <c r="T65" s="1"/>
+      <c r="U65" s="17">
         <v>0.66559999999999997</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C59" s="1" t="s">
+    <row r="66" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C66" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="4">
+      <c r="D66" s="1"/>
+      <c r="E66" s="4">
         <v>42.83</v>
       </c>
-      <c r="E59" s="4">
+      <c r="F66" s="4">
         <v>83.36</v>
       </c>
-      <c r="F59" s="4">
+      <c r="G66" s="4">
         <v>90.7</v>
       </c>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4">
+      <c r="H66" s="4"/>
+      <c r="I66" s="4">
         <v>39.229999999999997</v>
       </c>
-      <c r="I59" s="4"/>
-      <c r="J59" s="4">
+      <c r="J66" s="4"/>
+      <c r="K66" s="4">
         <v>49.84</v>
       </c>
-      <c r="K59" s="4">
+      <c r="L66" s="4">
         <v>87.5</v>
       </c>
-      <c r="L59" s="4">
+      <c r="M66" s="4">
         <v>93.41</v>
       </c>
-      <c r="M59" s="4"/>
-      <c r="N59" s="4">
+      <c r="N66" s="4"/>
+      <c r="O66" s="4">
         <v>42.63</v>
       </c>
-      <c r="O59" s="4"/>
-      <c r="P59" s="4">
+      <c r="P66" s="4"/>
+      <c r="Q66" s="4">
         <v>65.8</v>
       </c>
-      <c r="Q59" s="4">
+      <c r="R66" s="4">
         <v>90.5</v>
       </c>
-      <c r="R59" s="4">
+      <c r="S66" s="4">
         <v>97.3</v>
       </c>
-      <c r="S59" s="4"/>
-      <c r="T59" s="4">
+      <c r="T66" s="4"/>
+      <c r="U66" s="4">
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C60" s="1" t="s">
+    <row r="67" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C67" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D60" s="19">
+      <c r="D67" s="1"/>
+      <c r="E67" s="19">
         <v>0.4335</v>
       </c>
-      <c r="E60" s="19">
+      <c r="F67" s="19">
         <v>0.83350000000000002</v>
       </c>
-      <c r="F60" s="19">
+      <c r="G67" s="19">
         <v>0.90259999999999996</v>
       </c>
-      <c r="G60" s="20"/>
-      <c r="H60" s="19">
+      <c r="H67" s="20"/>
+      <c r="I67" s="19">
         <v>0.38850000000000001</v>
       </c>
-      <c r="I60" s="21"/>
-      <c r="J60" s="19">
+      <c r="J67" s="21"/>
+      <c r="K67" s="19">
         <v>0.49130000000000001</v>
       </c>
-      <c r="K60" s="19">
+      <c r="L67" s="19">
         <v>0.87970000000000004</v>
       </c>
-      <c r="L60" s="19">
+      <c r="M67" s="19">
         <v>0.93069999999999997</v>
       </c>
-      <c r="M60" s="19"/>
-      <c r="N60" s="19">
+      <c r="N67" s="19"/>
+      <c r="O67" s="19">
         <v>0.41320000000000001</v>
       </c>
-      <c r="O60" s="21"/>
-      <c r="P60" s="19">
+      <c r="P67" s="21"/>
+      <c r="Q67" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="Q60" s="19">
+      <c r="R67" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="R60" s="19">
+      <c r="S67" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="S60" s="22"/>
-      <c r="T60" s="23">
+      <c r="T67" s="22"/>
+      <c r="U67" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="72" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
+    <row r="73" spans="3:21" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mode to run ppi to front
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="117">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -346,13 +346,37 @@
     <t>2embPpiAnnotE256H1L12I768Set0/BertAve12Ep10e12Drop0.1Lr5e5None</t>
   </si>
   <si>
-    <t>2embPpiAnnotE256H1L12I512Set0/NoPpiEp10e10Drop0.1</t>
-  </si>
-  <si>
     <t>no init GO encoder</t>
   </si>
   <si>
     <t>No type emb</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I512Set0/NoPpiNoTypeBert12Ep10e10Drop0.1</t>
+  </si>
+  <si>
+    <t>init Bert12</t>
+  </si>
+  <si>
+    <t>test loss</t>
+  </si>
+  <si>
+    <t>dev loss</t>
+  </si>
+  <si>
+    <t>freeze_pretrained_vec": true</t>
+  </si>
+  <si>
+    <t>2embPpiAnnotE256H1L12I512Set0/NoPpiNoTypeEp10e10Drop0.1</t>
+  </si>
+  <si>
+    <t>type emb true</t>
+  </si>
+  <si>
+    <t>input 256 hidden 256 ppi</t>
+  </si>
+  <si>
+    <t>end2end GO label</t>
   </si>
 </sst>
 </file>
@@ -818,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:U73"/>
+  <dimension ref="A4:W73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,11 +856,11 @@
     <col min="4" max="4" width="26.140625" customWidth="1"/>
     <col min="5" max="7" width="9.140625" customWidth="1"/>
     <col min="8" max="9" width="9.140625" hidden="1" customWidth="1"/>
-    <col min="14" max="15" width="0" hidden="1" customWidth="1"/>
-    <col min="20" max="21" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="16" width="0" hidden="1" customWidth="1"/>
+    <col min="22" max="23" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
@@ -857,15 +881,17 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-      <c r="Q4" s="1" t="s">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1" t="s">
@@ -892,19 +918,21 @@
       </c>
       <c r="O5" s="2"/>
       <c r="P5" s="2"/>
-      <c r="Q5" s="1" t="s">
+      <c r="Q5" s="2"/>
+      <c r="R5" s="2"/>
+      <c r="S5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="T5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="S5" s="1"/>
-      <c r="T5" s="1" t="s">
+      <c r="U5" s="1"/>
+      <c r="V5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="W5" s="1"/>
+    </row>
+    <row r="6" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="25" t="s">
         <v>7</v>
       </c>
@@ -937,21 +965,23 @@
         <v>0.25840000000000002</v>
       </c>
       <c r="P6" s="27"/>
-      <c r="Q6" s="26">
+      <c r="Q6" s="27"/>
+      <c r="R6" s="27"/>
+      <c r="S6" s="26">
         <v>0.57199999999999995</v>
       </c>
-      <c r="R6" s="26">
+      <c r="T6" s="26">
         <v>0.67010000000000003</v>
       </c>
-      <c r="S6" s="26">
+      <c r="U6" s="26">
         <v>0.92390000000000005</v>
       </c>
-      <c r="T6" s="26"/>
-      <c r="U6" s="26">
+      <c r="V6" s="26"/>
+      <c r="W6" s="26">
         <v>0.51829999999999998</v>
       </c>
     </row>
-    <row r="7" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>21</v>
       </c>
@@ -984,19 +1014,21 @@
       <c r="N7" s="26"/>
       <c r="O7" s="26"/>
       <c r="P7" s="27"/>
-      <c r="Q7" s="26">
+      <c r="Q7" s="27"/>
+      <c r="R7" s="27"/>
+      <c r="S7" s="26">
         <v>0.57369999999999999</v>
       </c>
-      <c r="R7" s="26">
+      <c r="T7" s="26">
         <v>0.67589999999999995</v>
       </c>
-      <c r="S7" s="26">
+      <c r="U7" s="26">
         <v>0.92869999999999997</v>
       </c>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-    </row>
-    <row r="8" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V7" s="26"/>
+      <c r="W7" s="26"/>
+    </row>
+    <row r="8" spans="1:23" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
         <v>25</v>
       </c>
@@ -1023,19 +1055,21 @@
       <c r="N8" s="6"/>
       <c r="O8" s="6"/>
       <c r="P8" s="7"/>
-      <c r="Q8" s="6">
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="6">
         <v>0.60209999999999997</v>
       </c>
-      <c r="R8" s="6">
+      <c r="T8" s="6">
         <v>0.75190000000000001</v>
       </c>
-      <c r="S8" s="6">
+      <c r="U8" s="6">
         <v>0.94389999999999996</v>
       </c>
-      <c r="T8" s="6"/>
-      <c r="U8" s="6"/>
-    </row>
-    <row r="9" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+    </row>
+    <row r="9" spans="1:23" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="28" t="s">
         <v>25</v>
       </c>
@@ -1068,19 +1102,21 @@
       <c r="N9" s="6"/>
       <c r="O9" s="6"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="6">
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="6">
         <v>0.59709999999999996</v>
       </c>
-      <c r="R9" s="6">
+      <c r="T9" s="6">
         <v>0.74370000000000003</v>
       </c>
-      <c r="S9" s="6">
+      <c r="U9" s="6">
         <v>0.93920000000000003</v>
       </c>
-      <c r="T9" s="6"/>
-      <c r="U9" s="6"/>
-    </row>
-    <row r="10" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+    </row>
+    <row r="10" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="29" t="s">
         <v>27</v>
       </c>
@@ -1105,19 +1141,21 @@
       <c r="N10" s="26"/>
       <c r="O10" s="26"/>
       <c r="P10" s="27"/>
-      <c r="Q10" s="26" t="s">
+      <c r="Q10" s="27"/>
+      <c r="R10" s="27"/>
+      <c r="S10" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="R10" s="26">
+      <c r="T10" s="26">
         <v>0.73909999999999998</v>
       </c>
-      <c r="S10" s="26">
+      <c r="U10" s="26">
         <v>0.94120000000000004</v>
       </c>
-      <c r="T10" s="26"/>
-      <c r="U10" s="26"/>
-    </row>
-    <row r="11" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V10" s="26"/>
+      <c r="W10" s="26"/>
+    </row>
+    <row r="11" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="29" t="s">
         <v>26</v>
       </c>
@@ -1141,19 +1179,21 @@
       <c r="N11" s="26"/>
       <c r="O11" s="26"/>
       <c r="P11" s="27"/>
-      <c r="Q11" s="26">
+      <c r="Q11" s="27"/>
+      <c r="R11" s="27"/>
+      <c r="S11" s="26">
         <v>0.65210000000000001</v>
       </c>
-      <c r="R11" s="26">
+      <c r="T11" s="26">
         <v>0.89180000000000004</v>
       </c>
-      <c r="S11" s="26">
+      <c r="U11" s="26">
         <v>0.97009999999999996</v>
       </c>
-      <c r="T11" s="26"/>
-      <c r="U11" s="26"/>
-    </row>
-    <row r="12" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V11" s="26"/>
+      <c r="W11" s="26"/>
+    </row>
+    <row r="12" spans="1:23" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
       <c r="E12" s="6"/>
@@ -1168,13 +1208,15 @@
       <c r="N12" s="6"/>
       <c r="O12" s="6"/>
       <c r="P12" s="7"/>
-      <c r="Q12" s="6"/>
-      <c r="R12" s="6"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
       <c r="S12" s="6"/>
       <c r="T12" s="6"/>
       <c r="U12" s="6"/>
-    </row>
-    <row r="13" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+    </row>
+    <row r="13" spans="1:23" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="28" t="s">
         <v>19</v>
       </c>
@@ -1201,19 +1243,21 @@
       <c r="N13" s="6"/>
       <c r="O13" s="6"/>
       <c r="P13" s="7"/>
-      <c r="Q13" s="6">
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="6">
         <v>0.60599999999999998</v>
       </c>
-      <c r="R13" s="6">
+      <c r="T13" s="6">
         <v>0.75949999999999995</v>
       </c>
-      <c r="S13" s="6">
+      <c r="U13" s="6">
         <v>0.94520000000000004</v>
       </c>
-      <c r="T13" s="6"/>
-      <c r="U13" s="6"/>
-    </row>
-    <row r="14" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+    </row>
+    <row r="14" spans="1:23" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="28" t="s">
         <v>19</v>
       </c>
@@ -1240,13 +1284,15 @@
       <c r="N14" s="6"/>
       <c r="O14" s="6"/>
       <c r="P14" s="7"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
       <c r="S14" s="6"/>
       <c r="T14" s="6"/>
       <c r="U14" s="6"/>
-    </row>
-    <row r="15" spans="1:21" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+    </row>
+    <row r="15" spans="1:23" s="28" customFormat="1" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="28" t="s">
         <v>23</v>
       </c>
@@ -1273,13 +1319,15 @@
       <c r="N15" s="6"/>
       <c r="O15" s="6"/>
       <c r="P15" s="7"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
       <c r="S15" s="6"/>
       <c r="T15" s="6"/>
       <c r="U15" s="6"/>
-    </row>
-    <row r="16" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+    </row>
+    <row r="16" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
       <c r="E16" s="6"/>
@@ -1294,13 +1342,15 @@
       <c r="N16" s="6"/>
       <c r="O16" s="6"/>
       <c r="P16" s="7"/>
-      <c r="Q16" s="6"/>
-      <c r="R16" s="6"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
       <c r="S16" s="6"/>
       <c r="T16" s="6"/>
       <c r="U16" s="6"/>
-    </row>
-    <row r="17" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+    </row>
+    <row r="17" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>28</v>
       </c>
@@ -1327,19 +1377,21 @@
       <c r="N17" s="26"/>
       <c r="O17" s="26"/>
       <c r="P17" s="27"/>
-      <c r="Q17" s="26">
+      <c r="Q17" s="27"/>
+      <c r="R17" s="27"/>
+      <c r="S17" s="26">
         <v>0.58860000000000001</v>
       </c>
-      <c r="R17" s="26">
+      <c r="T17" s="26">
         <v>0.75490000000000002</v>
       </c>
-      <c r="S17" s="26">
+      <c r="U17" s="26">
         <v>0.94579999999999997</v>
       </c>
-      <c r="T17" s="26"/>
-      <c r="U17" s="26"/>
-    </row>
-    <row r="18" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V17" s="26"/>
+      <c r="W17" s="26"/>
+    </row>
+    <row r="18" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="28" t="s">
         <v>30</v>
       </c>
@@ -1360,13 +1412,15 @@
       <c r="N18" s="6"/>
       <c r="O18" s="6"/>
       <c r="P18" s="7"/>
-      <c r="Q18" s="6"/>
-      <c r="R18" s="6"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
       <c r="S18" s="6"/>
       <c r="T18" s="6"/>
       <c r="U18" s="6"/>
-    </row>
-    <row r="19" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+    </row>
+    <row r="19" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
@@ -1382,13 +1436,15 @@
       <c r="N19" s="6"/>
       <c r="O19" s="6"/>
       <c r="P19" s="7"/>
-      <c r="Q19" s="6"/>
-      <c r="R19" s="6"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
       <c r="S19" s="6"/>
       <c r="T19" s="6"/>
       <c r="U19" s="6"/>
-    </row>
-    <row r="20" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+    </row>
+    <row r="20" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>29</v>
       </c>
@@ -1415,19 +1471,21 @@
       <c r="N20" s="26"/>
       <c r="O20" s="26"/>
       <c r="P20" s="27"/>
-      <c r="Q20" s="26">
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
+      <c r="S20" s="26">
         <v>0.65739999999999998</v>
       </c>
-      <c r="R20" s="26">
+      <c r="T20" s="26">
         <v>0.90769999999999995</v>
       </c>
-      <c r="S20" s="26">
+      <c r="U20" s="26">
         <v>0.97309999999999997</v>
       </c>
-      <c r="T20" s="26"/>
-      <c r="U20" s="26"/>
-    </row>
-    <row r="21" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V20" s="26"/>
+      <c r="W20" s="26"/>
+    </row>
+    <row r="21" spans="1:23" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="24" t="s">
         <v>37</v>
       </c>
@@ -1452,13 +1510,15 @@
       <c r="N21" s="26"/>
       <c r="O21" s="26"/>
       <c r="P21" s="27"/>
-      <c r="Q21" s="26"/>
-      <c r="R21" s="26"/>
+      <c r="Q21" s="27"/>
+      <c r="R21" s="27"/>
       <c r="S21" s="26"/>
       <c r="T21" s="26"/>
       <c r="U21" s="26"/>
-    </row>
-    <row r="22" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V21" s="26"/>
+      <c r="W21" s="26"/>
+    </row>
+    <row r="22" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B22" s="5"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
@@ -1474,13 +1534,15 @@
       <c r="N22" s="6"/>
       <c r="O22" s="6"/>
       <c r="P22" s="7"/>
-      <c r="Q22" s="6"/>
-      <c r="R22" s="6"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
       <c r="S22" s="6"/>
       <c r="T22" s="6"/>
       <c r="U22" s="6"/>
-    </row>
-    <row r="23" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V22" s="6"/>
+      <c r="W22" s="6"/>
+    </row>
+    <row r="23" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="24" t="s">
         <v>32</v>
       </c>
@@ -1505,13 +1567,15 @@
       <c r="N23" s="6"/>
       <c r="O23" s="6"/>
       <c r="P23" s="7"/>
-      <c r="Q23" s="6"/>
-      <c r="R23" s="6"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
       <c r="S23" s="6"/>
       <c r="T23" s="6"/>
       <c r="U23" s="6"/>
-    </row>
-    <row r="24" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V23" s="6"/>
+      <c r="W23" s="6"/>
+    </row>
+    <row r="24" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B24" s="5"/>
       <c r="C24" s="5"/>
       <c r="D24" s="5"/>
@@ -1527,13 +1591,15 @@
       <c r="N24" s="6"/>
       <c r="O24" s="6"/>
       <c r="P24" s="7"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
       <c r="S24" s="6"/>
       <c r="T24" s="6"/>
       <c r="U24" s="6"/>
-    </row>
-    <row r="25" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V24" s="6"/>
+      <c r="W24" s="6"/>
+    </row>
+    <row r="25" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="28" t="s">
         <v>36</v>
       </c>
@@ -1558,13 +1624,15 @@
       <c r="N25" s="6"/>
       <c r="O25" s="6"/>
       <c r="P25" s="7"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
       <c r="S25" s="6"/>
       <c r="T25" s="6"/>
       <c r="U25" s="6"/>
-    </row>
-    <row r="26" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V25" s="6"/>
+      <c r="W25" s="6"/>
+    </row>
+    <row r="26" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
       <c r="D26" s="5"/>
@@ -1580,13 +1648,15 @@
       <c r="N26" s="6"/>
       <c r="O26" s="6"/>
       <c r="P26" s="7"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
       <c r="S26" s="6"/>
       <c r="T26" s="6"/>
       <c r="U26" s="6"/>
-    </row>
-    <row r="27" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V26" s="6"/>
+      <c r="W26" s="6"/>
+    </row>
+    <row r="27" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="28" t="s">
         <v>38</v>
       </c>
@@ -1611,13 +1681,15 @@
       <c r="N27" s="6"/>
       <c r="O27" s="6"/>
       <c r="P27" s="7"/>
-      <c r="Q27" s="6"/>
-      <c r="R27" s="6"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
       <c r="S27" s="6"/>
       <c r="T27" s="6"/>
       <c r="U27" s="6"/>
-    </row>
-    <row r="28" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V27" s="6"/>
+      <c r="W27" s="6"/>
+    </row>
+    <row r="28" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B28" s="5"/>
       <c r="C28" s="5"/>
       <c r="D28" s="5"/>
@@ -1633,13 +1705,15 @@
       <c r="N28" s="6"/>
       <c r="O28" s="6"/>
       <c r="P28" s="7"/>
-      <c r="Q28" s="6"/>
-      <c r="R28" s="6"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
       <c r="S28" s="6"/>
       <c r="T28" s="6"/>
       <c r="U28" s="6"/>
-    </row>
-    <row r="29" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V28" s="6"/>
+      <c r="W28" s="6"/>
+    </row>
+    <row r="29" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="5"/>
       <c r="C29" s="5"/>
       <c r="D29" s="5"/>
@@ -1655,24 +1729,36 @@
       <c r="N29" s="6"/>
       <c r="O29" s="6"/>
       <c r="P29" s="7"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
+      <c r="Q29" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>110</v>
+      </c>
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
       <c r="U29" s="6"/>
-    </row>
-    <row r="30" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V29" s="6"/>
+      <c r="W29" s="6"/>
+    </row>
+    <row r="30" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="28" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
       <c r="D30" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
+        <v>107</v>
+      </c>
+      <c r="E30" s="6">
+        <v>0.35404188032199202</v>
+      </c>
+      <c r="F30" s="6">
+        <v>0.68562932115446795</v>
+      </c>
+      <c r="G30" s="6">
+        <v>0.85097746487881898</v>
+      </c>
       <c r="H30" s="6"/>
       <c r="I30" s="6"/>
       <c r="J30" s="7"/>
@@ -1688,59 +1774,109 @@
       <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="Q30" s="6"/>
-      <c r="R30" s="6"/>
-      <c r="S30" s="6"/>
-      <c r="T30" s="6"/>
-      <c r="U30" s="6"/>
-    </row>
-    <row r="31" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="Q30" s="39">
+        <v>4.7257E-2</v>
+      </c>
+      <c r="R30" s="39">
+        <v>4.7258528256936598E-2</v>
+      </c>
+      <c r="S30" s="6">
+        <v>0.59798275250642696</v>
+      </c>
+      <c r="T30" s="6">
+        <v>0.757679713552465</v>
+      </c>
+      <c r="U30" s="6">
+        <v>0.94589534219438698</v>
+      </c>
+      <c r="V30" s="6"/>
+      <c r="W30" s="6"/>
+    </row>
+    <row r="31" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="28" t="s">
+        <v>108</v>
+      </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="5" t="s">
+        <v>112</v>
+      </c>
       <c r="E31" s="6"/>
       <c r="F31" s="6"/>
       <c r="G31" s="6"/>
       <c r="H31" s="6"/>
       <c r="I31" s="6"/>
       <c r="J31" s="7"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="6"/>
+      <c r="K31" s="6">
+        <v>0.40408129216357502</v>
+      </c>
+      <c r="L31" s="6">
+        <v>0.79076577208003596</v>
+      </c>
+      <c r="M31" s="6">
+        <v>0.89173938877665904</v>
+      </c>
       <c r="N31" s="6"/>
       <c r="O31" s="6"/>
-      <c r="P31" s="7"/>
-      <c r="Q31" s="6"/>
-      <c r="R31" s="6"/>
+      <c r="P31" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q31" s="39">
+        <v>4.7498800000000001E-2</v>
+      </c>
+      <c r="R31" s="39">
+        <v>5.2412652103082498E-2</v>
+      </c>
       <c r="S31" s="6"/>
       <c r="T31" s="6"/>
       <c r="U31" s="6"/>
-    </row>
-    <row r="32" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V31" s="6"/>
+      <c r="W31" s="6"/>
+    </row>
+    <row r="32" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="28" t="s">
+        <v>115</v>
+      </c>
       <c r="B32" s="5"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>116</v>
+      </c>
       <c r="E32" s="6"/>
       <c r="F32" s="6"/>
       <c r="G32" s="6"/>
       <c r="H32" s="6"/>
       <c r="I32" s="6"/>
       <c r="J32" s="7"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="6"/>
-      <c r="M32" s="6"/>
+      <c r="K32" s="6">
+        <v>0.52497242748937301</v>
+      </c>
+      <c r="L32" s="6">
+        <v>0.89571650250248902</v>
+      </c>
+      <c r="M32" s="6">
+        <v>0.94300275811376499</v>
+      </c>
       <c r="N32" s="6"/>
       <c r="O32" s="6"/>
       <c r="P32" s="7"/>
-      <c r="Q32" s="6"/>
-      <c r="R32" s="6"/>
+      <c r="Q32" s="39">
+        <v>3.5161459043737499E-2</v>
+      </c>
+      <c r="R32" s="39">
+        <v>4.1037345544872601E-2</v>
+      </c>
       <c r="S32" s="6"/>
       <c r="T32" s="6"/>
       <c r="U32" s="6"/>
-    </row>
-    <row r="33" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V32" s="6"/>
+      <c r="W32" s="6"/>
+    </row>
+    <row r="33" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B33" s="5"/>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
@@ -1756,13 +1892,15 @@
       <c r="N33" s="6"/>
       <c r="O33" s="6"/>
       <c r="P33" s="7"/>
-      <c r="Q33" s="6"/>
-      <c r="R33" s="6"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
       <c r="S33" s="6"/>
       <c r="T33" s="6"/>
       <c r="U33" s="6"/>
-    </row>
-    <row r="34" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V33" s="6"/>
+      <c r="W33" s="6"/>
+    </row>
+    <row r="34" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1778,13 +1916,15 @@
       <c r="N34" s="6"/>
       <c r="O34" s="6"/>
       <c r="P34" s="7"/>
-      <c r="Q34" s="6"/>
-      <c r="R34" s="6"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
       <c r="S34" s="6"/>
       <c r="T34" s="6"/>
       <c r="U34" s="6"/>
-    </row>
-    <row r="35" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V34" s="6"/>
+      <c r="W34" s="6"/>
+    </row>
+    <row r="35" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
@@ -1800,13 +1940,15 @@
       <c r="N35" s="6"/>
       <c r="O35" s="6"/>
       <c r="P35" s="7"/>
-      <c r="Q35" s="6"/>
-      <c r="R35" s="6"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
       <c r="S35" s="6"/>
       <c r="T35" s="6"/>
       <c r="U35" s="6"/>
-    </row>
-    <row r="36" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V35" s="6"/>
+      <c r="W35" s="6"/>
+    </row>
+    <row r="36" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="28" t="s">
         <v>99</v>
       </c>
@@ -1831,13 +1973,15 @@
       <c r="N36" s="6"/>
       <c r="O36" s="6"/>
       <c r="P36" s="7"/>
-      <c r="Q36" s="6"/>
-      <c r="R36" s="6"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
       <c r="S36" s="6"/>
       <c r="T36" s="6"/>
       <c r="U36" s="6"/>
-    </row>
-    <row r="37" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V36" s="6"/>
+      <c r="W36" s="6"/>
+    </row>
+    <row r="37" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="28" t="s">
         <v>100</v>
       </c>
@@ -1868,13 +2012,15 @@
       <c r="N37" s="6"/>
       <c r="O37" s="6"/>
       <c r="P37" s="7"/>
-      <c r="Q37" s="6"/>
-      <c r="R37" s="6"/>
+      <c r="Q37" s="7"/>
+      <c r="R37" s="7"/>
       <c r="S37" s="6"/>
       <c r="T37" s="6"/>
       <c r="U37" s="6"/>
-    </row>
-    <row r="38" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V37" s="6"/>
+      <c r="W37" s="6"/>
+    </row>
+    <row r="38" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="28" t="s">
         <v>101</v>
       </c>
@@ -1899,13 +2045,15 @@
       <c r="N38" s="6"/>
       <c r="O38" s="6"/>
       <c r="P38" s="7"/>
-      <c r="Q38" s="6"/>
-      <c r="R38" s="6"/>
+      <c r="Q38" s="7"/>
+      <c r="R38" s="7"/>
       <c r="S38" s="6"/>
       <c r="T38" s="6"/>
       <c r="U38" s="6"/>
-    </row>
-    <row r="39" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V38" s="6"/>
+      <c r="W38" s="6"/>
+    </row>
+    <row r="39" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B39" s="5"/>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1921,13 +2069,15 @@
       <c r="N39" s="6"/>
       <c r="O39" s="6"/>
       <c r="P39" s="7"/>
-      <c r="Q39" s="6"/>
-      <c r="R39" s="6"/>
+      <c r="Q39" s="7"/>
+      <c r="R39" s="7"/>
       <c r="S39" s="6"/>
       <c r="T39" s="6"/>
       <c r="U39" s="6"/>
-    </row>
-    <row r="40" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V39" s="6"/>
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="28" t="s">
         <v>102</v>
       </c>
@@ -1962,19 +2112,25 @@
       <c r="P40" s="39">
         <v>4.1920459275095398E-2</v>
       </c>
-      <c r="Q40" s="6">
+      <c r="Q40" s="39">
+        <v>3.5513733944519503E-2</v>
+      </c>
+      <c r="R40" s="39">
+        <v>4.1920459275095398E-2</v>
+      </c>
+      <c r="S40" s="6">
         <v>0.66610357651026797</v>
       </c>
-      <c r="R40" s="6">
+      <c r="T40" s="6">
         <v>0.90778748640305595</v>
       </c>
-      <c r="S40" s="6">
+      <c r="U40" s="6">
         <v>0.97222662155700101</v>
       </c>
-      <c r="T40" s="6"/>
-      <c r="U40" s="6"/>
-    </row>
-    <row r="41" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V40" s="6"/>
+      <c r="W40" s="6"/>
+    </row>
+    <row r="41" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="28" t="s">
         <v>102</v>
       </c>
@@ -1995,19 +2151,21 @@
       <c r="N41" s="6"/>
       <c r="O41" s="6"/>
       <c r="P41" s="7"/>
-      <c r="Q41" s="6">
+      <c r="Q41" s="7"/>
+      <c r="R41" s="7"/>
+      <c r="S41" s="6">
         <v>0.66219899999999998</v>
       </c>
-      <c r="R41" s="6">
+      <c r="T41" s="6">
         <v>0.90361093533127401</v>
       </c>
-      <c r="S41" s="6">
+      <c r="U41" s="6">
         <v>0.97134283099715801</v>
       </c>
-      <c r="T41" s="6"/>
-      <c r="U41" s="6"/>
-    </row>
-    <row r="42" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V41" s="6"/>
+      <c r="W41" s="6"/>
+    </row>
+    <row r="42" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B42" s="5"/>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
@@ -2023,13 +2181,15 @@
       <c r="N42" s="6"/>
       <c r="O42" s="6"/>
       <c r="P42" s="7"/>
-      <c r="Q42" s="6"/>
-      <c r="R42" s="6"/>
+      <c r="Q42" s="7"/>
+      <c r="R42" s="7"/>
       <c r="S42" s="6"/>
       <c r="T42" s="6"/>
       <c r="U42" s="6"/>
-    </row>
-    <row r="43" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V42" s="6"/>
+      <c r="W42" s="6"/>
+    </row>
+    <row r="43" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="28" t="s">
         <v>103</v>
       </c>
@@ -2056,13 +2216,15 @@
       <c r="N43" s="6"/>
       <c r="O43" s="6"/>
       <c r="P43" s="7"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
+      <c r="Q43" s="7"/>
+      <c r="R43" s="7"/>
       <c r="S43" s="6"/>
       <c r="T43" s="6"/>
       <c r="U43" s="6"/>
-    </row>
-    <row r="44" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V43" s="6"/>
+      <c r="W43" s="6"/>
+    </row>
+    <row r="44" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
@@ -2078,13 +2240,15 @@
       <c r="N44" s="6"/>
       <c r="O44" s="6"/>
       <c r="P44" s="7"/>
-      <c r="Q44" s="6"/>
-      <c r="R44" s="6"/>
+      <c r="Q44" s="7"/>
+      <c r="R44" s="7"/>
       <c r="S44" s="6"/>
       <c r="T44" s="6"/>
       <c r="U44" s="6"/>
-    </row>
-    <row r="45" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V44" s="6"/>
+      <c r="W44" s="6"/>
+    </row>
+    <row r="45" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="28" t="s">
         <v>105</v>
       </c>
@@ -2109,13 +2273,15 @@
       <c r="N45" s="6"/>
       <c r="O45" s="6"/>
       <c r="P45" s="7"/>
-      <c r="Q45" s="6"/>
-      <c r="R45" s="6"/>
+      <c r="Q45" s="7"/>
+      <c r="R45" s="7"/>
       <c r="S45" s="6"/>
       <c r="T45" s="6"/>
       <c r="U45" s="6"/>
-    </row>
-    <row r="46" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V45" s="6"/>
+      <c r="W45" s="6"/>
+    </row>
+    <row r="46" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B46" s="5"/>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
@@ -2139,13 +2305,15 @@
       <c r="P46" s="39">
         <v>4.2612862119596799E-2</v>
       </c>
-      <c r="Q46" s="6"/>
-      <c r="R46" s="6"/>
+      <c r="Q46" s="39"/>
+      <c r="R46" s="39"/>
       <c r="S46" s="6"/>
       <c r="T46" s="6"/>
       <c r="U46" s="6"/>
-    </row>
-    <row r="47" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V46" s="6"/>
+      <c r="W46" s="6"/>
+    </row>
+    <row r="47" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
@@ -2161,13 +2329,15 @@
       <c r="N47" s="6"/>
       <c r="O47" s="6"/>
       <c r="P47" s="7"/>
-      <c r="Q47" s="6"/>
-      <c r="R47" s="6"/>
+      <c r="Q47" s="7"/>
+      <c r="R47" s="7"/>
       <c r="S47" s="6"/>
       <c r="T47" s="6"/>
       <c r="U47" s="6"/>
-    </row>
-    <row r="48" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V47" s="6"/>
+      <c r="W47" s="6"/>
+    </row>
+    <row r="48" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B48" s="5"/>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
@@ -2183,13 +2353,15 @@
       <c r="N48" s="6"/>
       <c r="O48" s="6"/>
       <c r="P48" s="7"/>
-      <c r="Q48" s="6"/>
-      <c r="R48" s="6"/>
+      <c r="Q48" s="7"/>
+      <c r="R48" s="7"/>
       <c r="S48" s="6"/>
       <c r="T48" s="6"/>
       <c r="U48" s="6"/>
-    </row>
-    <row r="49" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V48" s="6"/>
+      <c r="W48" s="6"/>
+    </row>
+    <row r="49" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B49" s="5"/>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
@@ -2205,13 +2377,15 @@
       <c r="N49" s="6"/>
       <c r="O49" s="6"/>
       <c r="P49" s="7"/>
-      <c r="Q49" s="6"/>
-      <c r="R49" s="6"/>
+      <c r="Q49" s="7"/>
+      <c r="R49" s="7"/>
       <c r="S49" s="6"/>
       <c r="T49" s="6"/>
       <c r="U49" s="6"/>
-    </row>
-    <row r="50" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V49" s="6"/>
+      <c r="W49" s="6"/>
+    </row>
+    <row r="50" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B50" s="5"/>
       <c r="C50" s="5"/>
       <c r="D50" s="5"/>
@@ -2227,13 +2401,15 @@
       <c r="N50" s="6"/>
       <c r="O50" s="6"/>
       <c r="P50" s="7"/>
-      <c r="Q50" s="6"/>
-      <c r="R50" s="6"/>
+      <c r="Q50" s="7"/>
+      <c r="R50" s="7"/>
       <c r="S50" s="6"/>
       <c r="T50" s="6"/>
       <c r="U50" s="6"/>
-    </row>
-    <row r="51" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V50" s="6"/>
+      <c r="W50" s="6"/>
+    </row>
+    <row r="51" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="28" t="s">
         <v>96</v>
       </c>
@@ -2252,19 +2428,21 @@
       <c r="N51" s="6"/>
       <c r="O51" s="6"/>
       <c r="P51" s="7"/>
-      <c r="Q51" s="6">
+      <c r="Q51" s="7"/>
+      <c r="R51" s="7"/>
+      <c r="S51" s="6">
         <v>0.66569299999999998</v>
       </c>
-      <c r="R51" s="6">
+      <c r="T51" s="6">
         <v>0.90422999999999998</v>
       </c>
-      <c r="S51" s="6">
+      <c r="U51" s="6">
         <v>0.97198600000000002</v>
       </c>
-      <c r="T51" s="6"/>
-      <c r="U51" s="6"/>
-    </row>
-    <row r="52" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V51" s="6"/>
+      <c r="W51" s="6"/>
+    </row>
+    <row r="52" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
@@ -2280,13 +2458,15 @@
       <c r="N52" s="6"/>
       <c r="O52" s="6"/>
       <c r="P52" s="7"/>
-      <c r="Q52" s="6"/>
-      <c r="R52" s="6"/>
+      <c r="Q52" s="7"/>
+      <c r="R52" s="7"/>
       <c r="S52" s="6"/>
       <c r="T52" s="6"/>
       <c r="U52" s="6"/>
-    </row>
-    <row r="53" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V52" s="6"/>
+      <c r="W52" s="6"/>
+    </row>
+    <row r="53" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="28" t="s">
         <v>104</v>
       </c>
@@ -2311,19 +2491,21 @@
       <c r="N53" s="6"/>
       <c r="O53" s="6"/>
       <c r="P53" s="7"/>
-      <c r="Q53" s="6">
+      <c r="Q53" s="7"/>
+      <c r="R53" s="7"/>
+      <c r="S53" s="6">
         <v>0.59847806990903096</v>
       </c>
-      <c r="R53" s="6">
+      <c r="T53" s="6">
         <v>0.74540495542180496</v>
       </c>
-      <c r="S53" s="6">
+      <c r="U53" s="6">
         <v>0.94279293529049801</v>
       </c>
-      <c r="T53" s="6"/>
-      <c r="U53" s="6"/>
-    </row>
-    <row r="54" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V53" s="6"/>
+      <c r="W53" s="6"/>
+    </row>
+    <row r="54" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B54" s="5"/>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
@@ -2339,13 +2521,15 @@
       <c r="N54" s="6"/>
       <c r="O54" s="6"/>
       <c r="P54" s="7"/>
-      <c r="Q54" s="6"/>
-      <c r="R54" s="6"/>
+      <c r="Q54" s="7"/>
+      <c r="R54" s="7"/>
       <c r="S54" s="6"/>
       <c r="T54" s="6"/>
       <c r="U54" s="6"/>
-    </row>
-    <row r="55" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V54" s="6"/>
+      <c r="W54" s="6"/>
+    </row>
+    <row r="55" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B55" s="5"/>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
@@ -2361,13 +2545,15 @@
       <c r="N55" s="6"/>
       <c r="O55" s="6"/>
       <c r="P55" s="7"/>
-      <c r="Q55" s="6"/>
-      <c r="R55" s="6"/>
+      <c r="Q55" s="7"/>
+      <c r="R55" s="7"/>
       <c r="S55" s="6"/>
       <c r="T55" s="6"/>
       <c r="U55" s="6"/>
-    </row>
-    <row r="56" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V55" s="6"/>
+      <c r="W55" s="6"/>
+    </row>
+    <row r="56" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="28" t="s">
         <v>35</v>
       </c>
@@ -2386,13 +2572,15 @@
       <c r="N56" s="6"/>
       <c r="O56" s="6"/>
       <c r="P56" s="7"/>
-      <c r="Q56" s="6"/>
-      <c r="R56" s="6"/>
+      <c r="Q56" s="7"/>
+      <c r="R56" s="7"/>
       <c r="S56" s="6"/>
       <c r="T56" s="6"/>
       <c r="U56" s="6"/>
-    </row>
-    <row r="57" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="V56" s="6"/>
+      <c r="W56" s="6"/>
+    </row>
+    <row r="57" spans="1:23" s="28" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="28" t="s">
         <v>35</v>
       </c>
@@ -2410,13 +2598,15 @@
       <c r="N57" s="6"/>
       <c r="O57" s="6"/>
       <c r="P57" s="7"/>
-      <c r="Q57" s="6"/>
-      <c r="R57" s="6"/>
+      <c r="Q57" s="7"/>
+      <c r="R57" s="7"/>
       <c r="S57" s="6"/>
       <c r="T57" s="6"/>
       <c r="U57" s="6"/>
-    </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="V57" s="6"/>
+      <c r="W57" s="6"/>
+    </row>
+    <row r="58" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A58" s="28" t="s">
         <v>35</v>
       </c>
@@ -2452,21 +2642,23 @@
         <v>0.3614</v>
       </c>
       <c r="P58" s="7"/>
-      <c r="Q58" s="6">
+      <c r="Q58" s="7"/>
+      <c r="R58" s="7"/>
+      <c r="S58" s="6">
         <v>0.627</v>
       </c>
-      <c r="R58" s="6">
+      <c r="T58" s="6">
         <v>0.878</v>
       </c>
-      <c r="S58" s="6">
+      <c r="U58" s="6">
         <v>0.9647</v>
       </c>
-      <c r="T58" s="3"/>
-      <c r="U58" s="3">
+      <c r="V58" s="3"/>
+      <c r="W58" s="3">
         <v>0.62470000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A59" s="28"/>
       <c r="C59" s="8" t="s">
         <v>9</v>
@@ -2500,21 +2692,23 @@
         <v>0.40760000000000002</v>
       </c>
       <c r="P59" s="9"/>
-      <c r="Q59" s="9">
+      <c r="Q59" s="9"/>
+      <c r="R59" s="9"/>
+      <c r="S59" s="9">
         <v>63.77</v>
       </c>
-      <c r="R59" s="9">
+      <c r="T59" s="9">
         <v>89.79</v>
       </c>
-      <c r="S59" s="9">
+      <c r="U59" s="9">
         <v>97.1</v>
       </c>
-      <c r="T59" s="8"/>
-      <c r="U59" s="11">
+      <c r="V59" s="8"/>
+      <c r="W59" s="11">
         <v>0.64100000000000001</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A60" s="28"/>
       <c r="C60" s="12" t="s">
         <v>10</v>
@@ -2548,21 +2742,23 @@
         <v>0.41799999999999998</v>
       </c>
       <c r="P60" s="15"/>
-      <c r="Q60" s="13">
+      <c r="Q60" s="15"/>
+      <c r="R60" s="15"/>
+      <c r="S60" s="13">
         <v>0.65200000000000002</v>
       </c>
-      <c r="R60" s="13">
+      <c r="T60" s="13">
         <v>0.90390000000000004</v>
       </c>
-      <c r="S60" s="13">
+      <c r="U60" s="13">
         <v>0.97199999999999998</v>
       </c>
-      <c r="T60" s="13"/>
-      <c r="U60" s="13">
+      <c r="V60" s="13"/>
+      <c r="W60" s="13">
         <v>0.65949999999999998</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C61" s="6" t="s">
         <v>11</v>
       </c>
@@ -2595,21 +2791,23 @@
         <v>0.43809999999999999</v>
       </c>
       <c r="P61" s="6"/>
-      <c r="Q61" s="6">
+      <c r="Q61" s="6"/>
+      <c r="R61" s="6"/>
+      <c r="S61" s="6">
         <v>0.65469999999999995</v>
       </c>
-      <c r="R61" s="6">
+      <c r="T61" s="6">
         <v>0.90480000000000005</v>
       </c>
-      <c r="S61" s="6">
+      <c r="U61" s="6">
         <v>0.97250000000000003</v>
       </c>
-      <c r="T61" s="6"/>
-      <c r="U61" s="6">
+      <c r="V61" s="6"/>
+      <c r="W61" s="6">
         <v>0.66139999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C62" s="1" t="s">
         <v>12</v>
       </c>
@@ -2642,21 +2840,23 @@
         <v>0.42930000000000001</v>
       </c>
       <c r="P62" s="4"/>
-      <c r="Q62" s="3">
+      <c r="Q62" s="4"/>
+      <c r="R62" s="4"/>
+      <c r="S62" s="3">
         <v>0.65239999999999998</v>
       </c>
-      <c r="R62" s="17">
+      <c r="T62" s="17">
         <v>0.90569999999999995</v>
       </c>
-      <c r="S62" s="3">
+      <c r="U62" s="3">
         <v>0.97260000000000002</v>
       </c>
-      <c r="T62" s="3"/>
-      <c r="U62" s="3">
+      <c r="V62" s="3"/>
+      <c r="W62" s="3">
         <v>0.65810000000000002</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C63" s="1" t="s">
         <v>13</v>
       </c>
@@ -2689,21 +2889,23 @@
         <v>0.42209999999999998</v>
       </c>
       <c r="P63" s="1"/>
-      <c r="Q63" s="4">
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+      <c r="S63" s="4">
         <v>65.39</v>
       </c>
-      <c r="R63" s="1">
+      <c r="T63" s="1">
         <v>90.27</v>
       </c>
-      <c r="S63" s="4">
+      <c r="U63" s="4">
         <v>97.27</v>
       </c>
-      <c r="T63" s="1"/>
-      <c r="U63" s="3">
+      <c r="V63" s="1"/>
+      <c r="W63" s="3">
         <v>0.65659999999999996</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.25">
       <c r="C64" s="1" t="s">
         <v>14</v>
       </c>
@@ -2736,21 +2938,23 @@
         <v>0.43259999999999998</v>
       </c>
       <c r="P64" s="3"/>
-      <c r="Q64" s="3">
+      <c r="Q64" s="3"/>
+      <c r="R64" s="3"/>
+      <c r="S64" s="3">
         <v>0.6482</v>
       </c>
-      <c r="R64" s="3">
+      <c r="T64" s="3">
         <v>0.90500000000000003</v>
       </c>
-      <c r="S64" s="3">
+      <c r="U64" s="3">
         <v>0.97209999999999996</v>
       </c>
-      <c r="T64" s="3"/>
-      <c r="U64" s="3">
+      <c r="V64" s="3"/>
+      <c r="W64" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="65" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="65" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C65" s="32" t="s">
         <v>15</v>
       </c>
@@ -2783,21 +2987,23 @@
         <v>0.43430000000000002</v>
       </c>
       <c r="P65" s="32"/>
-      <c r="Q65" s="33">
+      <c r="Q65" s="32"/>
+      <c r="R65" s="32"/>
+      <c r="S65" s="33">
         <v>0.6583</v>
       </c>
-      <c r="R65" s="35">
+      <c r="T65" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="S65" s="33">
+      <c r="U65" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="T65" s="1"/>
-      <c r="U65" s="17">
+      <c r="V65" s="1"/>
+      <c r="W65" s="17">
         <v>0.66559999999999997</v>
       </c>
     </row>
-    <row r="66" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="66" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C66" s="1" t="s">
         <v>16</v>
       </c>
@@ -2830,21 +3036,23 @@
         <v>42.63</v>
       </c>
       <c r="P66" s="4"/>
-      <c r="Q66" s="4">
+      <c r="Q66" s="4"/>
+      <c r="R66" s="4"/>
+      <c r="S66" s="4">
         <v>65.8</v>
       </c>
-      <c r="R66" s="4">
+      <c r="T66" s="4">
         <v>90.5</v>
       </c>
-      <c r="S66" s="4">
+      <c r="U66" s="4">
         <v>97.3</v>
       </c>
-      <c r="T66" s="4"/>
-      <c r="U66" s="4">
+      <c r="V66" s="4"/>
+      <c r="W66" s="4">
         <v>66.290000000000006</v>
       </c>
     </row>
-    <row r="67" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="67" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C67" s="1" t="s">
         <v>17</v>
       </c>
@@ -2877,26 +3085,28 @@
         <v>0.41320000000000001</v>
       </c>
       <c r="P67" s="21"/>
-      <c r="Q67" s="19">
+      <c r="Q67" s="21"/>
+      <c r="R67" s="21"/>
+      <c r="S67" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="R67" s="19">
+      <c r="T67" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="S67" s="19">
+      <c r="U67" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="T67" s="22"/>
-      <c r="U67" s="23">
+      <c r="V67" s="22"/>
+      <c r="W67" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="72" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="72" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C72" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="73" spans="3:21" x14ac:dyDescent="0.25">
+    <row r="73" spans="3:23" x14ac:dyDescent="0.25">
       <c r="C73" t="s">
         <v>31</v>
       </c>

</xml_diff>

<commit_message>
add go vec output
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\BertGOAnnotation\SeeAttention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dat\Documents\GitHub\BertGOAnnotation\SeeAttention\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="146">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -462,17 +462,20 @@
   </si>
   <si>
     <t xml:space="preserve">add bert12 dim768 </t>
+  </si>
+  <si>
+    <t>bert12-&gt;unfreeze-&gt;layernorm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -606,7 +609,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
@@ -649,7 +652,9 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="10" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="9" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3495,11 +3500,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:U26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:J20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="15" width="10.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -3796,19 +3805,19 @@
       <c r="C17" t="s">
         <v>137</v>
       </c>
-      <c r="K17" s="41">
+      <c r="K17" s="43">
         <v>0.40326794737190902</v>
       </c>
-      <c r="L17" s="41">
+      <c r="L17" s="43">
         <v>0.77992288244587304</v>
       </c>
-      <c r="M17" s="41">
+      <c r="M17" s="43">
         <v>0.89643268200654302</v>
       </c>
-      <c r="N17" s="42">
+      <c r="N17" s="44">
         <v>4.4325446345408998E-2</v>
       </c>
-      <c r="O17" s="42">
+      <c r="O17" s="44">
         <v>5.0013094739035202E-2</v>
       </c>
       <c r="Q17" s="41">
@@ -3819,6 +3828,9 @@
       </c>
       <c r="S17" s="41">
         <v>0.94572578270612895</v>
+      </c>
+      <c r="T17">
+        <v>5.4420958964907298E-2</v>
       </c>
       <c r="U17">
         <v>5.5321342714533601E-2</v>
@@ -3957,11 +3969,21 @@
       <c r="C23" t="s">
         <v>140</v>
       </c>
-      <c r="K23" s="41"/>
-      <c r="L23" s="41"/>
-      <c r="M23" s="41"/>
-      <c r="N23" s="41"/>
-      <c r="O23" s="41"/>
+      <c r="K23" s="43">
+        <v>0.39728044509084198</v>
+      </c>
+      <c r="L23" s="43">
+        <v>0.76987304761827202</v>
+      </c>
+      <c r="M23" s="43">
+        <v>0.88266797860906099</v>
+      </c>
+      <c r="N23" s="44">
+        <v>4.0290715267610099E-2</v>
+      </c>
+      <c r="O23" s="44">
+        <v>5.2531731185968301E-2</v>
+      </c>
     </row>
     <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="K24" s="41"/>
@@ -3974,21 +3996,60 @@
       <c r="S24" s="6"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
+      <c r="A25" t="s">
+        <v>139</v>
+      </c>
+      <c r="B25" t="s">
+        <v>138</v>
+      </c>
+      <c r="C25" t="s">
+        <v>145</v>
+      </c>
+      <c r="K25" s="41">
+        <v>0.52798739219405399</v>
+      </c>
+      <c r="L25" s="41">
+        <v>0.88908131752518804</v>
+      </c>
+      <c r="M25" s="41">
+        <v>0.93999240479022494</v>
+      </c>
+      <c r="N25" s="42">
+        <v>2.3933667898394601E-2</v>
+      </c>
+      <c r="O25" s="42">
+        <v>4.2602221911121202E-2</v>
+      </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
+      <c r="A26" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" t="s">
+        <v>136</v>
+      </c>
+      <c r="C26" t="s">
+        <v>145</v>
+      </c>
+      <c r="K26" s="43">
+        <v>0.40407461052249199</v>
+      </c>
+      <c r="L26" s="43">
+        <v>0.78409109272143296</v>
+      </c>
+      <c r="M26" s="43">
+        <v>0.88931404963882599</v>
+      </c>
+      <c r="N26" s="44">
+        <v>4.0847215751155602E-2</v>
+      </c>
+      <c r="O26" s="44">
+        <v>5.2182795027841303E-2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
change script add posthoc?
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="434" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="151">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -465,6 +465,21 @@
   </si>
   <si>
     <t>bert12-&gt;unfreeze-&gt;layernorm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">running </t>
+  </si>
+  <si>
+    <t>running</t>
+  </si>
+  <si>
+    <t>running nlp7</t>
+  </si>
+  <si>
+    <t>running nlp8</t>
+  </si>
+  <si>
+    <t>need redo</t>
   </si>
 </sst>
 </file>
@@ -609,7 +624,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
@@ -658,6 +673,9 @@
     <xf numFmtId="10" fontId="9" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="9" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="2" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -943,8 +961,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:X79"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T64" sqref="T64:V65"/>
+    <sheetView topLeftCell="A42" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66:E73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3503,8 +3521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:V26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3688,9 +3706,15 @@
         <v>142</v>
       </c>
       <c r="F12" s="24"/>
-      <c r="G12" s="26"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="26"/>
+      <c r="G12" s="26">
+        <v>0.41799999999999998</v>
+      </c>
+      <c r="H12" s="26">
+        <v>0.81869999999999998</v>
+      </c>
+      <c r="I12" s="26">
+        <v>0.89700000000000002</v>
+      </c>
       <c r="J12" s="26"/>
       <c r="K12" s="24"/>
       <c r="L12" s="26">
@@ -3720,9 +3744,15 @@
         <v>143</v>
       </c>
       <c r="F13" s="24"/>
-      <c r="G13" s="26"/>
-      <c r="H13" s="26"/>
-      <c r="I13" s="26"/>
+      <c r="G13" s="27">
+        <v>42.51</v>
+      </c>
+      <c r="H13" s="27">
+        <v>82.97</v>
+      </c>
+      <c r="I13" s="27">
+        <v>90.27</v>
+      </c>
       <c r="J13" s="26"/>
       <c r="K13" s="24"/>
       <c r="L13" s="27">
@@ -3819,7 +3849,9 @@
       <c r="C17" t="s">
         <v>137</v>
       </c>
-      <c r="G17" s="41"/>
+      <c r="G17" s="41" t="s">
+        <v>150</v>
+      </c>
       <c r="H17" s="41"/>
       <c r="I17" s="41"/>
       <c r="L17" s="43">
@@ -3885,69 +3917,97 @@
       <c r="S18" s="41"/>
       <c r="T18" s="41"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="36" t="s">
         <v>138</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="G19" s="41"/>
-      <c r="H19" s="41"/>
-      <c r="I19" s="41"/>
-      <c r="L19" s="41">
+      <c r="G19" s="47" t="s">
+        <v>149</v>
+      </c>
+      <c r="H19" s="47"/>
+      <c r="I19" s="47"/>
+      <c r="L19" s="47">
         <v>0.47566398921654102</v>
       </c>
-      <c r="M19" s="41">
+      <c r="M19" s="47">
         <v>0.84405080649754105</v>
       </c>
-      <c r="N19" s="41">
+      <c r="N19" s="47">
         <v>0.92051855478715705</v>
       </c>
-      <c r="O19" s="42">
+      <c r="O19" s="48">
         <v>3.2037597043465003E-2</v>
       </c>
-      <c r="P19" s="42">
+      <c r="P19" s="48">
         <v>4.6118542378074397E-2</v>
       </c>
-      <c r="R19" s="41"/>
-      <c r="S19" s="41"/>
-      <c r="T19" s="41"/>
-    </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="R19" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="S19" s="47"/>
+      <c r="T19" s="47"/>
+    </row>
+    <row r="20" spans="1:22" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B20" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="G20" s="41"/>
-      <c r="H20" s="41"/>
-      <c r="I20" s="41"/>
-      <c r="L20" s="6">
+      <c r="G20" s="47">
+        <v>0.43734748978439902</v>
+      </c>
+      <c r="H20" s="47">
+        <v>0.83582195309103802</v>
+      </c>
+      <c r="I20" s="47">
+        <v>0.90654547633930604</v>
+      </c>
+      <c r="J20" s="36">
+        <v>7.6435628227395802E-2</v>
+      </c>
+      <c r="K20" s="36">
+        <v>9.4105249121416296E-2</v>
+      </c>
+      <c r="L20" s="11">
         <v>0.52719019632316599</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M20" s="11">
         <v>0.89044415843526803</v>
       </c>
-      <c r="N20" s="6">
+      <c r="N20" s="11">
         <v>0.94233414227701595</v>
       </c>
-      <c r="O20" s="42">
+      <c r="O20" s="48">
         <v>2.5079185192247801E-2</v>
       </c>
-      <c r="P20" s="42">
+      <c r="P20" s="48">
         <v>4.2406372327575999E-2</v>
       </c>
-      <c r="R20" s="41"/>
-      <c r="S20" s="41"/>
-      <c r="T20" s="41"/>
+      <c r="R20" s="47">
+        <v>0.66063238169757499</v>
+      </c>
+      <c r="S20" s="47">
+        <v>0.90979241274186395</v>
+      </c>
+      <c r="T20" s="47">
+        <v>0.97291791160275398</v>
+      </c>
+      <c r="U20" s="36">
+        <v>3.6398513055700001E-2</v>
+      </c>
+      <c r="V20" s="36">
+        <v>4.5410556638999199E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="G21" s="41"/>
@@ -3959,37 +4019,41 @@
       <c r="S21" s="41"/>
       <c r="T21" s="41"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:22" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="24" t="s">
         <v>140</v>
       </c>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="41"/>
-      <c r="L22" s="41">
+      <c r="G22" s="49" t="s">
+        <v>146</v>
+      </c>
+      <c r="H22" s="49"/>
+      <c r="I22" s="49"/>
+      <c r="L22" s="49">
         <v>0.52181982596156395</v>
       </c>
-      <c r="M22" s="41">
+      <c r="M22" s="49">
         <v>0.89093869573544204</v>
       </c>
-      <c r="N22" s="41">
+      <c r="N22" s="49">
         <v>0.94258284186542496</v>
       </c>
-      <c r="O22" s="42">
+      <c r="O22" s="50">
         <v>2.8461095022346401E-2</v>
       </c>
-      <c r="P22" s="42">
+      <c r="P22" s="50">
         <v>4.1900366180971801E-2</v>
       </c>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
-      <c r="T22" s="41"/>
+      <c r="R22" s="49" t="s">
+        <v>148</v>
+      </c>
+      <c r="S22" s="49"/>
+      <c r="T22" s="49"/>
     </row>
     <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
@@ -4086,6 +4150,9 @@
       </c>
       <c r="I26" s="47">
         <v>0.84248623447175797</v>
+      </c>
+      <c r="J26" s="36">
+        <v>0.103582492198157</v>
       </c>
       <c r="K26" s="36">
         <v>0.110216817388472</v>

</xml_diff>

<commit_message>
change to run on large data
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="148">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -462,6 +462,15 @@
   </si>
   <si>
     <t>bert12-&gt;unfreeze-&gt;layernorm</t>
+  </si>
+  <si>
+    <t>add 20 topology</t>
+  </si>
+  <si>
+    <t>BertAveWordClsSepLayer11+12</t>
+  </si>
+  <si>
+    <t>ELMO</t>
   </si>
 </sst>
 </file>
@@ -474,7 +483,7 @@
     <numFmt numFmtId="165" formatCode="0.000000"/>
     <numFmt numFmtId="166" formatCode="_(* #,##0.00000_);_(* \(#,##0.00000\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -558,8 +567,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +630,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -630,7 +652,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
@@ -676,8 +698,6 @@
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="3" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="3" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="12" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="166" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
@@ -690,6 +710,13 @@
     <xf numFmtId="10" fontId="0" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="12" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="166" fontId="12" fillId="8" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="13" fillId="9" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="13" fillId="9" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="2" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="2" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -973,10 +1000,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:X79"/>
+  <dimension ref="A4:X81"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F79" sqref="F79"/>
+    <sheetView topLeftCell="A46" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3216,312 +3243,400 @@
       </c>
     </row>
     <row r="68" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C68" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D68" s="1"/>
-      <c r="E68" s="3">
-        <v>0.43149999999999999</v>
-      </c>
-      <c r="F68" s="3">
-        <v>0.83409999999999995</v>
-      </c>
-      <c r="G68" s="3">
-        <v>0.90590000000000004</v>
-      </c>
-      <c r="H68" s="3"/>
-      <c r="I68" s="3">
-        <v>0.39169999999999999</v>
-      </c>
-      <c r="J68" s="3"/>
-      <c r="K68" s="3">
-        <v>0.49930000000000002</v>
-      </c>
-      <c r="L68" s="3">
-        <v>0.87290000000000001</v>
-      </c>
-      <c r="M68" s="3">
-        <v>0.93389999999999995</v>
-      </c>
-      <c r="N68" s="3"/>
-      <c r="O68" s="3">
-        <v>0.42930000000000001</v>
-      </c>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="3">
-        <v>0.65239999999999998</v>
-      </c>
-      <c r="U68" s="17">
-        <v>0.90569999999999995</v>
-      </c>
-      <c r="V68" s="3">
-        <v>0.97260000000000002</v>
-      </c>
-      <c r="W68" s="3"/>
-      <c r="X68" s="3">
-        <v>0.65810000000000002</v>
-      </c>
+      <c r="C68" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="6"/>
+      <c r="E68" s="61">
+        <v>0.43940000000000001</v>
+      </c>
+      <c r="F68" s="61">
+        <v>0.8347</v>
+      </c>
+      <c r="G68" s="61">
+        <v>0.9052</v>
+      </c>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="61">
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="L68" s="61">
+        <v>0.87409999999999999</v>
+      </c>
+      <c r="M68" s="61">
+        <v>0.93269999999999997</v>
+      </c>
+      <c r="N68" s="6"/>
+      <c r="O68" s="16"/>
+      <c r="P68" s="6"/>
+      <c r="Q68" s="6"/>
+      <c r="R68" s="6"/>
+      <c r="S68" s="6"/>
+      <c r="T68" s="61">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="U68" s="61">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="V68" s="61">
+        <v>0.97289999999999999</v>
+      </c>
+      <c r="W68" s="6"/>
+      <c r="X68" s="6"/>
     </row>
     <row r="69" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C69" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D69" s="1"/>
-      <c r="E69" s="1">
-        <v>43.45</v>
-      </c>
-      <c r="F69" s="1">
-        <v>83.11</v>
-      </c>
-      <c r="G69" s="1">
-        <v>90.55</v>
-      </c>
-      <c r="H69" s="18"/>
+      <c r="E69" s="3">
+        <v>0.43149999999999999</v>
+      </c>
+      <c r="F69" s="3">
+        <v>0.83409999999999995</v>
+      </c>
+      <c r="G69" s="3">
+        <v>0.90590000000000004</v>
+      </c>
+      <c r="H69" s="3"/>
       <c r="I69" s="3">
-        <v>0.3896</v>
-      </c>
-      <c r="J69" s="1"/>
-      <c r="K69" s="1">
-        <v>49.24</v>
-      </c>
-      <c r="L69" s="1">
-        <v>87.43</v>
-      </c>
-      <c r="M69" s="1">
-        <v>93.52</v>
-      </c>
-      <c r="N69" s="1"/>
+        <v>0.39169999999999999</v>
+      </c>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3">
+        <v>0.49930000000000002</v>
+      </c>
+      <c r="L69" s="3">
+        <v>0.87290000000000001</v>
+      </c>
+      <c r="M69" s="3">
+        <v>0.93389999999999995</v>
+      </c>
+      <c r="N69" s="3"/>
       <c r="O69" s="3">
-        <v>0.42209999999999998</v>
-      </c>
-      <c r="P69" s="1"/>
-      <c r="Q69" s="1"/>
-      <c r="R69" s="1"/>
-      <c r="S69" s="1"/>
-      <c r="T69" s="4">
-        <v>65.39</v>
-      </c>
-      <c r="U69" s="1">
-        <v>90.27</v>
-      </c>
-      <c r="V69" s="4">
-        <v>97.27</v>
-      </c>
-      <c r="W69" s="1"/>
+        <v>0.42930000000000001</v>
+      </c>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="3">
+        <v>0.65239999999999998</v>
+      </c>
+      <c r="U69" s="17">
+        <v>0.90569999999999995</v>
+      </c>
+      <c r="V69" s="3">
+        <v>0.97260000000000002</v>
+      </c>
+      <c r="W69" s="3"/>
       <c r="X69" s="3">
-        <v>0.65659999999999996</v>
+        <v>0.65810000000000002</v>
       </c>
     </row>
     <row r="70" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1">
+        <v>43.45</v>
+      </c>
+      <c r="F70" s="1">
+        <v>83.11</v>
+      </c>
+      <c r="G70" s="1">
+        <v>90.55</v>
+      </c>
+      <c r="H70" s="18"/>
+      <c r="I70" s="3">
+        <v>0.3896</v>
+      </c>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1">
+        <v>49.24</v>
+      </c>
+      <c r="L70" s="1">
+        <v>87.43</v>
+      </c>
+      <c r="M70" s="1">
+        <v>93.52</v>
+      </c>
+      <c r="N70" s="1"/>
+      <c r="O70" s="3">
+        <v>0.42209999999999998</v>
+      </c>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+      <c r="S70" s="1"/>
+      <c r="T70" s="4">
+        <v>65.39</v>
+      </c>
+      <c r="U70" s="1">
+        <v>90.27</v>
+      </c>
+      <c r="V70" s="4">
+        <v>97.27</v>
+      </c>
+      <c r="W70" s="1"/>
+      <c r="X70" s="3">
+        <v>0.65659999999999996</v>
+      </c>
+    </row>
+    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C71" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D70" s="1"/>
-      <c r="E70" s="3">
+      <c r="D71" s="1"/>
+      <c r="E71" s="3">
         <v>0.42909999999999998</v>
       </c>
-      <c r="F70" s="3">
+      <c r="F71" s="3">
         <v>0.83479999999999999</v>
       </c>
-      <c r="G70" s="3">
+      <c r="G71" s="3">
         <v>0.90569999999999995</v>
       </c>
-      <c r="H70" s="3"/>
-      <c r="I70" s="3">
+      <c r="H71" s="3"/>
+      <c r="I71" s="3">
         <v>0.38979999999999998</v>
       </c>
-      <c r="J70" s="3"/>
-      <c r="K70" s="3">
+      <c r="J71" s="3"/>
+      <c r="K71" s="3">
         <v>0.49349999999999999</v>
       </c>
-      <c r="L70" s="17">
+      <c r="L71" s="17">
         <v>0.87919999999999998</v>
       </c>
-      <c r="M70" s="3">
+      <c r="M71" s="3">
         <v>0.93830000000000002</v>
       </c>
-      <c r="N70" s="3"/>
-      <c r="O70" s="3">
+      <c r="N71" s="3"/>
+      <c r="O71" s="3">
         <v>0.43259999999999998</v>
       </c>
-      <c r="P70" s="3"/>
-      <c r="Q70" s="3"/>
-      <c r="R70" s="3"/>
-      <c r="S70" s="3"/>
-      <c r="T70" s="3">
+      <c r="P71" s="3"/>
+      <c r="Q71" s="3"/>
+      <c r="R71" s="3"/>
+      <c r="S71" s="3"/>
+      <c r="T71" s="3">
         <v>0.6482</v>
       </c>
-      <c r="U70" s="3">
+      <c r="U71" s="3">
         <v>0.90500000000000003</v>
       </c>
-      <c r="V70" s="3">
+      <c r="V71" s="3">
         <v>0.97209999999999996</v>
       </c>
-      <c r="W70" s="3"/>
-      <c r="X70" s="3">
+      <c r="W71" s="3"/>
+      <c r="X71" s="3">
         <v>0.65500000000000003</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C71" s="32" t="s">
+    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C72" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="D71" s="32"/>
-      <c r="E71" s="33">
+      <c r="D72" s="32"/>
+      <c r="E72" s="33">
         <v>0.43919999999999998</v>
       </c>
-      <c r="F71" s="33">
+      <c r="F72" s="33">
         <v>0.83489999999999998</v>
       </c>
-      <c r="G71" s="33">
+      <c r="G72" s="33">
         <v>0.90769999999999995</v>
       </c>
-      <c r="H71" s="34"/>
-      <c r="I71" s="35">
+      <c r="H72" s="34"/>
+      <c r="I72" s="35">
         <v>0.39300000000000002</v>
       </c>
-      <c r="J71" s="32"/>
-      <c r="K71" s="33">
+      <c r="J72" s="32"/>
+      <c r="K72" s="33">
         <v>0.503</v>
       </c>
-      <c r="L71" s="35">
+      <c r="L72" s="35">
         <v>0.87680000000000002</v>
       </c>
-      <c r="M71" s="35">
+      <c r="M72" s="35">
         <v>0.93659999999999999</v>
       </c>
-      <c r="N71" s="35"/>
-      <c r="O71" s="35">
+      <c r="N72" s="35"/>
+      <c r="O72" s="35">
         <v>0.43430000000000002</v>
       </c>
-      <c r="P71" s="32"/>
-      <c r="Q71" s="32"/>
-      <c r="R71" s="32"/>
-      <c r="S71" s="32"/>
-      <c r="T71" s="33">
+      <c r="P72" s="32"/>
+      <c r="Q72" s="32"/>
+      <c r="R72" s="32"/>
+      <c r="S72" s="32"/>
+      <c r="T72" s="33">
         <v>0.6583</v>
       </c>
-      <c r="U71" s="35">
+      <c r="U72" s="35">
         <v>0.90510000000000002</v>
       </c>
-      <c r="V71" s="33">
+      <c r="V72" s="33">
         <v>0.97299999999999998</v>
       </c>
-      <c r="W71" s="1"/>
-      <c r="X71" s="17">
+      <c r="W72" s="1"/>
+      <c r="X72" s="17">
         <v>0.66559999999999997</v>
-      </c>
-    </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C72" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D72" s="1"/>
-      <c r="E72" s="4">
-        <v>42.83</v>
-      </c>
-      <c r="F72" s="4">
-        <v>83.36</v>
-      </c>
-      <c r="G72" s="4">
-        <v>90.7</v>
-      </c>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4">
-        <v>39.229999999999997</v>
-      </c>
-      <c r="J72" s="4"/>
-      <c r="K72" s="4">
-        <v>49.84</v>
-      </c>
-      <c r="L72" s="4">
-        <v>87.5</v>
-      </c>
-      <c r="M72" s="4">
-        <v>93.41</v>
-      </c>
-      <c r="N72" s="4"/>
-      <c r="O72" s="4">
-        <v>42.63</v>
-      </c>
-      <c r="P72" s="4"/>
-      <c r="Q72" s="4"/>
-      <c r="R72" s="4"/>
-      <c r="S72" s="4"/>
-      <c r="T72" s="4">
-        <v>65.8</v>
-      </c>
-      <c r="U72" s="4">
-        <v>90.5</v>
-      </c>
-      <c r="V72" s="4">
-        <v>97.3</v>
-      </c>
-      <c r="W72" s="4"/>
-      <c r="X72" s="4">
-        <v>66.290000000000006</v>
       </c>
     </row>
     <row r="73" spans="1:24" x14ac:dyDescent="0.25">
       <c r="C73" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D73" s="1"/>
+      <c r="E73" s="4">
+        <v>42.83</v>
+      </c>
+      <c r="F73" s="4">
+        <v>83.36</v>
+      </c>
+      <c r="G73" s="4">
+        <v>90.7</v>
+      </c>
+      <c r="H73" s="4"/>
+      <c r="I73" s="4">
+        <v>39.229999999999997</v>
+      </c>
+      <c r="J73" s="4"/>
+      <c r="K73" s="4">
+        <v>49.84</v>
+      </c>
+      <c r="L73" s="4">
+        <v>87.5</v>
+      </c>
+      <c r="M73" s="4">
+        <v>93.41</v>
+      </c>
+      <c r="N73" s="4"/>
+      <c r="O73" s="4">
+        <v>42.63</v>
+      </c>
+      <c r="P73" s="4"/>
+      <c r="Q73" s="4"/>
+      <c r="R73" s="4"/>
+      <c r="S73" s="4"/>
+      <c r="T73" s="4">
+        <v>65.8</v>
+      </c>
+      <c r="U73" s="4">
+        <v>90.5</v>
+      </c>
+      <c r="V73" s="4">
+        <v>97.3</v>
+      </c>
+      <c r="W73" s="4"/>
+      <c r="X73" s="4">
+        <v>66.290000000000006</v>
+      </c>
+    </row>
+    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C74" s="60" t="s">
+        <v>146</v>
+      </c>
+      <c r="D74" s="1"/>
+      <c r="E74" s="61">
+        <v>0.44109999999999999</v>
+      </c>
+      <c r="F74" s="61">
+        <v>0.83840000000000003</v>
+      </c>
+      <c r="G74" s="61">
+        <v>0.90900000000000003</v>
+      </c>
+      <c r="H74" s="4"/>
+      <c r="I74" s="4"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="61">
+        <v>0.50419999999999998</v>
+      </c>
+      <c r="L74" s="61">
+        <v>0.88060000000000005</v>
+      </c>
+      <c r="M74" s="61">
+        <v>0.93830000000000002</v>
+      </c>
+      <c r="N74" s="4"/>
+      <c r="O74" s="4"/>
+      <c r="P74" s="4"/>
+      <c r="Q74" s="4"/>
+      <c r="R74" s="4"/>
+      <c r="S74" s="4"/>
+      <c r="T74" s="61">
+        <v>0.66110000000000002</v>
+      </c>
+      <c r="U74" s="61">
+        <v>0.9052</v>
+      </c>
+      <c r="V74" s="61">
+        <v>0.97289999999999999</v>
+      </c>
+      <c r="W74" s="4"/>
+      <c r="X74" s="4"/>
+    </row>
+    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C75" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D73" s="1"/>
-      <c r="E73" s="19">
+      <c r="D75" s="1"/>
+      <c r="E75" s="19">
         <v>0.4335</v>
       </c>
-      <c r="F73" s="19">
+      <c r="F75" s="19">
         <v>0.83350000000000002</v>
       </c>
-      <c r="G73" s="19">
+      <c r="G75" s="19">
         <v>0.90259999999999996</v>
       </c>
-      <c r="H73" s="20"/>
-      <c r="I73" s="19">
+      <c r="H75" s="20"/>
+      <c r="I75" s="19">
         <v>0.38850000000000001</v>
       </c>
-      <c r="J73" s="21"/>
-      <c r="K73" s="19">
+      <c r="J75" s="21"/>
+      <c r="K75" s="19">
         <v>0.49130000000000001</v>
       </c>
-      <c r="L73" s="19">
+      <c r="L75" s="19">
         <v>0.87970000000000004</v>
       </c>
-      <c r="M73" s="19">
+      <c r="M75" s="19">
         <v>0.93069999999999997</v>
       </c>
-      <c r="N73" s="19"/>
-      <c r="O73" s="19">
+      <c r="N75" s="19"/>
+      <c r="O75" s="19">
         <v>0.41320000000000001</v>
       </c>
-      <c r="P73" s="21"/>
-      <c r="Q73" s="21"/>
-      <c r="R73" s="21"/>
-      <c r="S73" s="21"/>
-      <c r="T73" s="19">
+      <c r="P75" s="21"/>
+      <c r="Q75" s="21"/>
+      <c r="R75" s="21"/>
+      <c r="S75" s="21"/>
+      <c r="T75" s="19">
         <v>0.65659999999999996</v>
       </c>
-      <c r="U73" s="19">
+      <c r="U75" s="19">
         <v>0.90269999999999995</v>
       </c>
-      <c r="V73" s="19">
+      <c r="V75" s="19">
         <v>0.97240000000000004</v>
       </c>
-      <c r="W73" s="22"/>
-      <c r="X73" s="23">
+      <c r="W75" s="22"/>
+      <c r="X75" s="23">
         <v>0.66069999999999995</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
+    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3533,10 +3648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U26"/>
+  <dimension ref="A2:U27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3789,42 +3904,82 @@
       </c>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D14" s="28"/>
+      <c r="D14" s="60" t="s">
+        <v>146</v>
+      </c>
       <c r="E14" s="28"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="F14" s="61">
+        <v>0.44109999999999999</v>
+      </c>
+      <c r="G14" s="61">
+        <v>0.83840000000000003</v>
+      </c>
+      <c r="H14" s="61">
+        <v>0.90900000000000003</v>
+      </c>
       <c r="I14" s="6"/>
       <c r="J14" s="28"/>
-      <c r="K14" s="6"/>
-      <c r="L14" s="6"/>
-      <c r="M14" s="6"/>
+      <c r="K14" s="61">
+        <v>0.50419999999999998</v>
+      </c>
+      <c r="L14" s="61">
+        <v>0.88060000000000005</v>
+      </c>
+      <c r="M14" s="61">
+        <v>0.93830000000000002</v>
+      </c>
       <c r="N14" s="6"/>
       <c r="O14" s="28"/>
       <c r="P14" s="28"/>
-      <c r="Q14" s="6"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
+      <c r="Q14" s="61">
+        <v>0.66110000000000002</v>
+      </c>
+      <c r="R14" s="61">
+        <v>0.9052</v>
+      </c>
+      <c r="S14" s="61">
+        <v>0.97289999999999999</v>
+      </c>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="D15" s="28"/>
+      <c r="D15" s="61" t="s">
+        <v>147</v>
+      </c>
       <c r="E15" s="28"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="F15" s="61">
+        <v>0.43940000000000001</v>
+      </c>
+      <c r="G15" s="61">
+        <v>0.8347</v>
+      </c>
+      <c r="H15" s="61">
+        <v>0.9052</v>
+      </c>
       <c r="I15" s="6"/>
       <c r="J15" s="28"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
+      <c r="K15" s="61">
+        <v>0.50229999999999997</v>
+      </c>
+      <c r="L15" s="61">
+        <v>0.87409999999999999</v>
+      </c>
+      <c r="M15" s="61">
+        <v>0.93269999999999997</v>
+      </c>
       <c r="N15" s="6"/>
       <c r="O15" s="28"/>
       <c r="P15" s="28"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="Q15" s="61">
+        <v>0.66449999999999998</v>
+      </c>
+      <c r="R15" s="61">
+        <v>0.90780000000000005</v>
+      </c>
+      <c r="S15" s="61">
+        <v>0.97289999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="36" t="s">
         <v>140</v>
       </c>
@@ -3834,19 +3989,25 @@
       <c r="C16" s="36" t="s">
         <v>133</v>
       </c>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="N16" t="s">
+      <c r="F16" s="62"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="O16" t="s">
+      <c r="J16" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="T16" t="s">
+      <c r="N16" s="36" t="s">
         <v>120</v>
       </c>
-      <c r="U16" t="s">
+      <c r="O16" s="36" t="s">
+        <v>109</v>
+      </c>
+      <c r="T16" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="U16" s="36" t="s">
         <v>109</v>
       </c>
     </row>
@@ -3875,19 +4036,19 @@
       <c r="J17">
         <v>0.10941309332454401</v>
       </c>
-      <c r="K17" s="47">
+      <c r="K17" s="45">
         <v>0.40326794737190902</v>
       </c>
-      <c r="L17" s="47">
+      <c r="L17" s="45">
         <v>0.77992288244587304</v>
       </c>
-      <c r="M17" s="47">
+      <c r="M17" s="45">
         <v>0.89643268200654302</v>
       </c>
-      <c r="N17" s="48">
+      <c r="N17" s="46">
         <v>4.4325446345408998E-2</v>
       </c>
-      <c r="O17" s="48">
+      <c r="O17" s="46">
         <v>5.0013094739035202E-2</v>
       </c>
       <c r="Q17" s="41">
@@ -3906,376 +4067,423 @@
         <v>5.5321342714533601E-2</v>
       </c>
     </row>
-    <row r="18" spans="1:21" s="49" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="49" t="s">
+    <row r="18" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="47" t="s">
         <v>137</v>
       </c>
-      <c r="B18" s="49" t="s">
+      <c r="B18" s="47" t="s">
         <v>135</v>
       </c>
-      <c r="C18" s="49" t="s">
+      <c r="C18" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="F18" s="50">
+      <c r="F18" s="48">
         <v>0.435953328415844</v>
       </c>
-      <c r="G18" s="50">
+      <c r="G18" s="48">
         <v>0.84098678518822201</v>
       </c>
-      <c r="H18" s="50">
+      <c r="H18" s="48">
         <v>0.909752681877249</v>
       </c>
-      <c r="I18" s="49">
+      <c r="I18" s="47">
         <v>8.06950336631517E-2</v>
       </c>
-      <c r="J18" s="49">
+      <c r="J18" s="47">
         <v>9.2957143526118502E-2</v>
       </c>
-      <c r="K18" s="50">
+      <c r="K18" s="48">
         <v>0.485681593218527</v>
       </c>
-      <c r="L18" s="50">
+      <c r="L18" s="48">
         <v>0.87586599959642397</v>
       </c>
-      <c r="M18" s="50">
+      <c r="M18" s="48">
         <v>0.93627788500424103</v>
       </c>
-      <c r="N18" s="51">
+      <c r="N18" s="49">
         <v>2.8760288764905599E-2</v>
       </c>
-      <c r="O18" s="51">
+      <c r="O18" s="49">
         <v>4.4049561360450601E-2</v>
       </c>
-      <c r="Q18" s="50">
+      <c r="Q18" s="48">
         <v>0.66452553949577498</v>
       </c>
-      <c r="R18" s="50">
+      <c r="R18" s="48">
         <v>0.912509538326713</v>
       </c>
-      <c r="S18" s="50">
+      <c r="S18" s="48">
         <v>0.97378513227352603</v>
       </c>
-      <c r="T18" s="49">
+      <c r="T18" s="47">
         <v>3.7570015463531101E-2</v>
       </c>
-      <c r="U18" s="49">
+      <c r="U18" s="47">
         <v>4.4823117068284901E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:21" s="52" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="52" t="s">
+    <row r="19" spans="1:21" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="50" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="50" t="s">
         <v>137</v>
       </c>
-      <c r="C19" s="52" t="s">
+      <c r="C19" s="50" t="s">
         <v>136</v>
       </c>
-      <c r="F19" s="53">
+      <c r="F19" s="51">
         <v>0.37528022552289197</v>
       </c>
-      <c r="G19" s="53">
+      <c r="G19" s="51">
         <v>0.70898888205050303</v>
       </c>
-      <c r="H19" s="53">
+      <c r="H19" s="51">
         <v>0.859816502371338</v>
       </c>
-      <c r="I19" s="52">
+      <c r="I19" s="50">
         <v>9.6331666316721604E-2</v>
       </c>
-      <c r="J19" s="52">
+      <c r="J19" s="50">
         <v>0.105713729081702</v>
       </c>
-      <c r="K19" s="53">
+      <c r="K19" s="51">
         <v>0.47566398921654102</v>
       </c>
-      <c r="L19" s="53">
+      <c r="L19" s="51">
         <v>0.84405080649754105</v>
       </c>
-      <c r="M19" s="53">
+      <c r="M19" s="51">
         <v>0.92051855478715705</v>
       </c>
-      <c r="N19" s="54">
+      <c r="N19" s="52">
         <v>3.2037597043465003E-2</v>
       </c>
-      <c r="O19" s="54">
+      <c r="O19" s="52">
         <v>4.6118542378074397E-2</v>
       </c>
-      <c r="Q19" s="53">
+      <c r="Q19" s="51">
         <v>0.59955926502497103</v>
       </c>
-      <c r="R19" s="53">
+      <c r="R19" s="51">
         <v>0.78933125988883501</v>
       </c>
-      <c r="S19" s="53">
+      <c r="S19" s="51">
         <v>0.94869662089206597</v>
       </c>
-      <c r="T19" s="52">
+      <c r="T19" s="50">
         <v>5.0057571149238499E-2</v>
       </c>
-      <c r="U19" s="52">
+      <c r="U19" s="50">
         <v>5.4877029770464998E-2</v>
       </c>
     </row>
-    <row r="20" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="28" t="s">
+    <row r="20" spans="1:21" s="57" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="57" t="s">
+        <v>134</v>
+      </c>
+      <c r="B20" s="57" t="s">
+        <v>137</v>
+      </c>
+      <c r="C20" s="57" t="s">
+        <v>136</v>
+      </c>
+      <c r="D20" s="57" t="s">
+        <v>145</v>
+      </c>
+      <c r="F20" s="58">
+        <v>0.38279141526039001</v>
+      </c>
+      <c r="G20" s="58">
+        <v>0.72872930902799604</v>
+      </c>
+      <c r="H20" s="58">
+        <v>0.86052761948635903</v>
+      </c>
+      <c r="I20" s="57">
+        <v>9.2658910977718695E-2</v>
+      </c>
+      <c r="J20" s="57">
+        <v>0.106904722470687</v>
+      </c>
+      <c r="K20" s="58">
+        <v>0.49033099802018498</v>
+      </c>
+      <c r="L20" s="58">
+        <v>0.84597499629899997</v>
+      </c>
+      <c r="M20" s="58">
+        <v>0.91922881446351901</v>
+      </c>
+      <c r="N20" s="59">
+        <v>3.1466688934283102E-2</v>
+      </c>
+      <c r="O20" s="59">
+        <v>4.5968399905775399E-2</v>
+      </c>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="58"/>
+      <c r="S20" s="58"/>
+    </row>
+    <row r="21" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B21" s="47" t="s">
         <v>138</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C21" s="47" t="s">
         <v>136</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F21" s="48">
         <v>0.43734748978439902</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G21" s="48">
         <v>0.83582195309103802</v>
       </c>
-      <c r="H20" s="45">
+      <c r="H21" s="48">
         <v>0.90654547633930604</v>
       </c>
-      <c r="I20" s="28">
+      <c r="I21" s="47">
         <v>7.6435628227395802E-2</v>
       </c>
-      <c r="J20" s="28">
+      <c r="J21" s="47">
         <v>9.4105249121416296E-2</v>
       </c>
-      <c r="K20" s="6">
+      <c r="K21" s="63">
         <v>0.52719019632316599</v>
       </c>
-      <c r="L20" s="6">
+      <c r="L21" s="63">
         <v>0.89044415843526803</v>
       </c>
-      <c r="M20" s="6">
+      <c r="M21" s="63">
         <v>0.94233414227701595</v>
       </c>
-      <c r="N20" s="46">
+      <c r="N21" s="49">
         <v>2.5079185192247801E-2</v>
       </c>
-      <c r="O20" s="46">
+      <c r="O21" s="49">
         <v>4.2406372327575999E-2</v>
       </c>
-      <c r="Q20" s="45">
+      <c r="Q21" s="48">
         <v>0.66063238169757499</v>
       </c>
-      <c r="R20" s="45">
+      <c r="R21" s="48">
         <v>0.90979241274186395</v>
       </c>
-      <c r="S20" s="45">
+      <c r="S21" s="48">
         <v>0.97291791160275398</v>
       </c>
-      <c r="T20" s="28">
+      <c r="T21" s="47">
         <v>3.6398513055700001E-2</v>
       </c>
-      <c r="U20" s="28">
+      <c r="U21" s="47">
         <v>4.5410556638999199E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="N21" s="42"/>
-      <c r="O21" s="42"/>
-      <c r="Q21" s="41"/>
-      <c r="R21" s="41"/>
-      <c r="S21" s="41"/>
-    </row>
-    <row r="22" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="N22" s="42"/>
+      <c r="O22" s="42"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+    </row>
+    <row r="23" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B22" s="24" t="s">
+      <c r="B23" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C23" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F22" s="43">
+      <c r="F23" s="43">
         <v>0.44214474328229503</v>
       </c>
-      <c r="G22" s="43">
+      <c r="G23" s="43">
         <v>0.84107673950456596</v>
       </c>
-      <c r="H22" s="43">
+      <c r="H23" s="43">
         <v>0.907716085449224</v>
       </c>
-      <c r="I22" s="24">
+      <c r="I23" s="24">
         <v>7.3904807642565407E-2</v>
       </c>
-      <c r="J22" s="24">
+      <c r="J23" s="24">
         <v>9.3746807413714606E-2</v>
       </c>
-      <c r="K22" s="43">
+      <c r="K23" s="43">
         <v>0.52181982596156395</v>
       </c>
-      <c r="L22" s="43">
+      <c r="L23" s="43">
         <v>0.89093869573544204</v>
       </c>
-      <c r="M22" s="43">
+      <c r="M23" s="43">
         <v>0.94258284186542496</v>
       </c>
-      <c r="N22" s="44">
+      <c r="N23" s="44">
         <v>2.8461095022346401E-2</v>
       </c>
-      <c r="O22" s="44">
+      <c r="O23" s="44">
         <v>4.1900366180971801E-2</v>
       </c>
-      <c r="Q22" s="43">
+      <c r="Q23" s="43">
         <v>0.664197295226434</v>
       </c>
-      <c r="R22" s="43">
+      <c r="R23" s="43">
         <v>0.90936678856998998</v>
       </c>
-      <c r="S22" s="43">
+      <c r="S23" s="43">
         <v>0.97201489595589596</v>
       </c>
-      <c r="T22" s="24">
+      <c r="T23" s="24">
         <v>3.5743781660970003E-2</v>
       </c>
-      <c r="U22" s="24">
+      <c r="U23" s="24">
         <v>4.5720232950223497E-2</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>134</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>135</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C24" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="41"/>
-      <c r="G23" s="41"/>
-      <c r="H23" s="41"/>
-      <c r="K23" s="47">
-        <v>0.39728044509084198</v>
-      </c>
-      <c r="L23" s="47">
-        <v>0.76987304761827202</v>
-      </c>
-      <c r="M23" s="47">
-        <v>0.88266797860906099</v>
-      </c>
-      <c r="N23" s="48">
-        <v>4.0290715267610099E-2</v>
-      </c>
-      <c r="O23" s="48">
-        <v>5.2531731185968301E-2</v>
-      </c>
-      <c r="Q23" s="41"/>
-      <c r="R23" s="41"/>
-      <c r="S23" s="41"/>
-    </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F24" s="41"/>
       <c r="G24" s="41"/>
       <c r="H24" s="41"/>
-      <c r="K24" s="41"/>
-      <c r="L24" s="41"/>
-      <c r="M24" s="41"/>
-      <c r="N24" s="41"/>
-      <c r="O24" s="41"/>
-      <c r="Q24" s="6"/>
-      <c r="R24" s="6"/>
-      <c r="S24" s="6"/>
+      <c r="K24" s="45">
+        <v>0.39728044509084198</v>
+      </c>
+      <c r="L24" s="45">
+        <v>0.76987304761827202</v>
+      </c>
+      <c r="M24" s="45">
+        <v>0.88266797860906099</v>
+      </c>
+      <c r="N24" s="46">
+        <v>4.0290715267610099E-2</v>
+      </c>
+      <c r="O24" s="46">
+        <v>5.2531731185968301E-2</v>
+      </c>
+      <c r="Q24" s="41"/>
+      <c r="R24" s="41"/>
+      <c r="S24" s="41"/>
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>138</v>
-      </c>
-      <c r="B25" t="s">
-        <v>137</v>
-      </c>
-      <c r="C25" t="s">
-        <v>144</v>
-      </c>
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
-      <c r="K25" s="41">
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
+      <c r="M25" s="41"/>
+      <c r="N25" s="41"/>
+      <c r="O25" s="41"/>
+      <c r="Q25" s="6"/>
+      <c r="R25" s="6"/>
+      <c r="S25" s="6"/>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>138</v>
+      </c>
+      <c r="B26" t="s">
+        <v>137</v>
+      </c>
+      <c r="C26" t="s">
+        <v>144</v>
+      </c>
+      <c r="F26" s="41"/>
+      <c r="G26" s="41"/>
+      <c r="H26" s="41"/>
+      <c r="K26" s="41">
         <v>0.52798739219405399</v>
       </c>
-      <c r="L25" s="41">
+      <c r="L26" s="41">
         <v>0.88908131752518804</v>
       </c>
-      <c r="M25" s="41">
+      <c r="M26" s="41">
         <v>0.93999240479022494</v>
       </c>
-      <c r="N25" s="42">
+      <c r="N26" s="42">
         <v>2.3933667898394601E-2</v>
       </c>
-      <c r="O25" s="42">
+      <c r="O26" s="42">
         <v>4.2602221911121202E-2</v>
       </c>
-      <c r="Q25" s="41"/>
-      <c r="R25" s="41"/>
-      <c r="S25" s="41"/>
-    </row>
-    <row r="26" spans="1:21" s="55" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="55" t="s">
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
+    </row>
+    <row r="27" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="55" t="s">
+      <c r="B27" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="C26" s="55" t="s">
+      <c r="C27" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="F26" s="56">
+      <c r="F27" s="54">
         <v>0.34893247055384802</v>
       </c>
-      <c r="G26" s="56">
+      <c r="G27" s="54">
         <v>0.67317502542262897</v>
       </c>
-      <c r="H26" s="56">
+      <c r="H27" s="54">
         <v>0.84248623447175797</v>
       </c>
-      <c r="I26" s="55">
+      <c r="I27" s="53">
         <v>0.103582492198157</v>
       </c>
-      <c r="J26" s="55">
+      <c r="J27" s="53">
         <v>0.110216817388472</v>
       </c>
-      <c r="K26" s="57">
+      <c r="K27" s="55">
         <v>0.40407461052249199</v>
       </c>
-      <c r="L26" s="57">
+      <c r="L27" s="55">
         <v>0.78409109272143296</v>
       </c>
-      <c r="M26" s="57">
+      <c r="M27" s="55">
         <v>0.88931404963882599</v>
       </c>
-      <c r="N26" s="58">
+      <c r="N27" s="56">
         <v>4.0847215751155602E-2</v>
       </c>
-      <c r="O26" s="58">
+      <c r="O27" s="56">
         <v>5.2182795027841303E-2</v>
       </c>
-      <c r="Q26" s="56">
+      <c r="Q27" s="54">
         <v>0.60047364223300004</v>
       </c>
-      <c r="R26" s="56">
+      <c r="R27" s="54">
         <v>0.74598242392985104</v>
       </c>
-      <c r="S26" s="56">
+      <c r="S27" s="54">
         <v>0.94286147483809202</v>
       </c>
-      <c r="T26" s="55">
+      <c r="T27" s="53">
         <v>4.9549475900016203E-2</v>
       </c>
-      <c r="U26" s="55">
+      <c r="U27" s="53">
         <v>5.6839456085560298E-2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
testing the 0 shot
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Github\BertGOAnnotation\SeeAttention\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dat\Documents\GitHub\BertGOAnnotation\SeeAttention\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="443" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="148">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -476,7 +476,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="4">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0000"/>
@@ -575,7 +575,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -636,6 +636,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -652,7 +658,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="69">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1"/>
@@ -717,6 +723,11 @@
     <xf numFmtId="10" fontId="2" fillId="10" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="10" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="2" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="3" builtinId="3"/>
@@ -3648,10 +3659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U27"/>
+  <dimension ref="A2:U28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="U22" sqref="U22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4222,9 +4233,21 @@
       <c r="O20" s="59">
         <v>4.5968399905775399E-2</v>
       </c>
-      <c r="Q20" s="58"/>
-      <c r="R20" s="58"/>
-      <c r="S20" s="58"/>
+      <c r="Q20" s="58">
+        <v>0.61519720109939702</v>
+      </c>
+      <c r="R20" s="58">
+        <v>0.80117443786838605</v>
+      </c>
+      <c r="S20" s="58">
+        <v>0.95193928700906905</v>
+      </c>
+      <c r="T20" s="57">
+        <v>4.8338237030663297E-2</v>
+      </c>
+      <c r="U20" s="57">
+        <v>5.3086872495026999E-2</v>
+      </c>
     </row>
     <row r="21" spans="1:21" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47" t="s">
@@ -4282,202 +4305,233 @@
         <v>4.5410556638999199E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="N22" s="42"/>
-      <c r="O22" s="42"/>
-      <c r="Q22" s="41"/>
-      <c r="R22" s="41"/>
-      <c r="S22" s="41"/>
-    </row>
-    <row r="23" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
+    <row r="22" spans="1:21" s="64" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="B22" s="64" t="s">
+        <v>137</v>
+      </c>
+      <c r="C22" s="64" t="s">
+        <v>136</v>
+      </c>
+      <c r="D22" s="64" t="s">
+        <v>145</v>
+      </c>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
+      <c r="H22" s="65"/>
+      <c r="N22" s="66"/>
+      <c r="O22" s="66"/>
+      <c r="Q22" s="65">
+        <v>0.67126424790124095</v>
+      </c>
+      <c r="R22" s="65">
+        <v>0.90641066109189905</v>
+      </c>
+      <c r="S22" s="65">
+        <v>0.97211803796346896</v>
+      </c>
+      <c r="U22" s="64">
+        <v>4.5328427185508897E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="N23" s="68"/>
+      <c r="O23" s="68"/>
+      <c r="Q23" s="67"/>
+      <c r="R23" s="67"/>
+      <c r="S23" s="67"/>
+    </row>
+    <row r="24" spans="1:21" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B24" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C23" s="24" t="s">
+      <c r="C24" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="F23" s="43">
+      <c r="F24" s="43">
         <v>0.44214474328229503</v>
       </c>
-      <c r="G23" s="43">
+      <c r="G24" s="43">
         <v>0.84107673950456596</v>
       </c>
-      <c r="H23" s="43">
+      <c r="H24" s="43">
         <v>0.907716085449224</v>
       </c>
-      <c r="I23" s="24">
+      <c r="I24" s="24">
         <v>7.3904807642565407E-2</v>
       </c>
-      <c r="J23" s="24">
+      <c r="J24" s="24">
         <v>9.3746807413714606E-2</v>
       </c>
-      <c r="K23" s="43">
+      <c r="K24" s="43">
         <v>0.52181982596156395</v>
       </c>
-      <c r="L23" s="43">
+      <c r="L24" s="43">
         <v>0.89093869573544204</v>
       </c>
-      <c r="M23" s="43">
+      <c r="M24" s="43">
         <v>0.94258284186542496</v>
       </c>
-      <c r="N23" s="44">
+      <c r="N24" s="44">
         <v>2.8461095022346401E-2</v>
       </c>
-      <c r="O23" s="44">
+      <c r="O24" s="44">
         <v>4.1900366180971801E-2</v>
       </c>
-      <c r="Q23" s="43">
+      <c r="Q24" s="43">
         <v>0.664197295226434</v>
       </c>
-      <c r="R23" s="43">
+      <c r="R24" s="43">
         <v>0.90936678856998998</v>
       </c>
-      <c r="S23" s="43">
+      <c r="S24" s="43">
         <v>0.97201489595589596</v>
       </c>
-      <c r="T23" s="24">
+      <c r="T24" s="24">
         <v>3.5743781660970003E-2</v>
       </c>
-      <c r="U23" s="24">
+      <c r="U24" s="24">
         <v>4.5720232950223497E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>134</v>
       </c>
-      <c r="B24" t="s">
+      <c r="B25" t="s">
         <v>135</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C25" t="s">
         <v>139</v>
       </c>
-      <c r="F24" s="41"/>
-      <c r="G24" s="41"/>
-      <c r="H24" s="41"/>
-      <c r="K24" s="45">
-        <v>0.39728044509084198</v>
-      </c>
-      <c r="L24" s="45">
-        <v>0.76987304761827202</v>
-      </c>
-      <c r="M24" s="45">
-        <v>0.88266797860906099</v>
-      </c>
-      <c r="N24" s="46">
-        <v>4.0290715267610099E-2</v>
-      </c>
-      <c r="O24" s="46">
-        <v>5.2531731185968301E-2</v>
-      </c>
-      <c r="Q24" s="41"/>
-      <c r="R24" s="41"/>
-      <c r="S24" s="41"/>
-    </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="F25" s="41"/>
       <c r="G25" s="41"/>
       <c r="H25" s="41"/>
-      <c r="K25" s="41"/>
-      <c r="L25" s="41"/>
-      <c r="M25" s="41"/>
-      <c r="N25" s="41"/>
-      <c r="O25" s="41"/>
-      <c r="Q25" s="6"/>
-      <c r="R25" s="6"/>
-      <c r="S25" s="6"/>
+      <c r="K25" s="45">
+        <v>0.39728044509084198</v>
+      </c>
+      <c r="L25" s="45">
+        <v>0.76987304761827202</v>
+      </c>
+      <c r="M25" s="45">
+        <v>0.88266797860906099</v>
+      </c>
+      <c r="N25" s="46">
+        <v>4.0290715267610099E-2</v>
+      </c>
+      <c r="O25" s="46">
+        <v>5.2531731185968301E-2</v>
+      </c>
+      <c r="Q25" s="41"/>
+      <c r="R25" s="41"/>
+      <c r="S25" s="41"/>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>138</v>
-      </c>
-      <c r="B26" t="s">
-        <v>137</v>
-      </c>
-      <c r="C26" t="s">
-        <v>144</v>
-      </c>
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
-      <c r="K26" s="41">
+      <c r="K26" s="41"/>
+      <c r="L26" s="41"/>
+      <c r="M26" s="41"/>
+      <c r="N26" s="41"/>
+      <c r="O26" s="41"/>
+      <c r="Q26" s="6"/>
+      <c r="R26" s="6"/>
+      <c r="S26" s="6"/>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>138</v>
+      </c>
+      <c r="B27" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" t="s">
+        <v>144</v>
+      </c>
+      <c r="F27" s="41"/>
+      <c r="G27" s="41"/>
+      <c r="H27" s="41"/>
+      <c r="K27" s="41">
         <v>0.52798739219405399</v>
       </c>
-      <c r="L26" s="41">
+      <c r="L27" s="41">
         <v>0.88908131752518804</v>
       </c>
-      <c r="M26" s="41">
+      <c r="M27" s="41">
         <v>0.93999240479022494</v>
       </c>
-      <c r="N26" s="42">
+      <c r="N27" s="42">
         <v>2.3933667898394601E-2</v>
       </c>
-      <c r="O26" s="42">
+      <c r="O27" s="42">
         <v>4.2602221911121202E-2</v>
       </c>
-      <c r="Q26" s="41"/>
-      <c r="R26" s="41"/>
-      <c r="S26" s="41"/>
-    </row>
-    <row r="27" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="53" t="s">
+      <c r="Q27" s="41"/>
+      <c r="R27" s="41"/>
+      <c r="S27" s="41"/>
+    </row>
+    <row r="28" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="B27" s="53" t="s">
+      <c r="B28" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="C27" s="53" t="s">
+      <c r="C28" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="F27" s="54">
+      <c r="F28" s="54">
         <v>0.34893247055384802</v>
       </c>
-      <c r="G27" s="54">
+      <c r="G28" s="54">
         <v>0.67317502542262897</v>
       </c>
-      <c r="H27" s="54">
+      <c r="H28" s="54">
         <v>0.84248623447175797</v>
       </c>
-      <c r="I27" s="53">
+      <c r="I28" s="53">
         <v>0.103582492198157</v>
       </c>
-      <c r="J27" s="53">
+      <c r="J28" s="53">
         <v>0.110216817388472</v>
       </c>
-      <c r="K27" s="55">
+      <c r="K28" s="55">
         <v>0.40407461052249199</v>
       </c>
-      <c r="L27" s="55">
+      <c r="L28" s="55">
         <v>0.78409109272143296</v>
       </c>
-      <c r="M27" s="55">
+      <c r="M28" s="55">
         <v>0.88931404963882599</v>
       </c>
-      <c r="N27" s="56">
+      <c r="N28" s="56">
         <v>4.0847215751155602E-2</v>
       </c>
-      <c r="O27" s="56">
+      <c r="O28" s="56">
         <v>5.2182795027841303E-2</v>
       </c>
-      <c r="Q27" s="54">
+      <c r="Q28" s="54">
         <v>0.60047364223300004</v>
       </c>
-      <c r="R27" s="54">
+      <c r="R28" s="54">
         <v>0.74598242392985104</v>
       </c>
-      <c r="S27" s="54">
+      <c r="S28" s="54">
         <v>0.94286147483809202</v>
       </c>
-      <c r="T27" s="53">
+      <c r="T28" s="53">
         <v>4.9549475900016203E-2</v>
       </c>
-      <c r="U27" s="53">
+      <c r="U28" s="53">
         <v>5.6839456085560298E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add option to save prediction as pickle
</commit_message>
<xml_diff>
--- a/SeeAttention/PrelimResult.xlsx
+++ b/SeeAttention/PrelimResult.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="460" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="153">
   <si>
     <t xml:space="preserve">Method </t>
   </si>
@@ -483,6 +483,9 @@
   </si>
   <si>
     <t>baseline on larger deepo data</t>
+  </si>
+  <si>
+    <t>`</t>
   </si>
 </sst>
 </file>
@@ -3674,10 +3677,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:U40"/>
+  <dimension ref="A2:U43"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M36" sqref="M36"/>
+      <selection activeCell="F24" sqref="F24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4481,350 +4484,404 @@
       <c r="F26" s="41"/>
       <c r="G26" s="41"/>
       <c r="H26" s="41"/>
-      <c r="K26" s="41"/>
-      <c r="L26" s="41"/>
-      <c r="M26" s="41"/>
-      <c r="N26" s="41"/>
-      <c r="O26" s="41"/>
-      <c r="Q26" s="6"/>
-      <c r="R26" s="6"/>
-      <c r="S26" s="6"/>
+      <c r="K26" s="45"/>
+      <c r="L26" s="45"/>
+      <c r="M26" s="45"/>
+      <c r="N26" s="46"/>
+      <c r="O26" s="46"/>
+      <c r="Q26" s="41"/>
+      <c r="R26" s="41"/>
+      <c r="S26" s="41"/>
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="A27" s="24" t="s">
         <v>138</v>
       </c>
-      <c r="B27" t="s">
+      <c r="B27" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C27" t="s">
-        <v>144</v>
+      <c r="C27" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="D27" s="57" t="s">
+        <v>145</v>
       </c>
       <c r="F27" s="41"/>
       <c r="G27" s="41"/>
       <c r="H27" s="41"/>
-      <c r="K27" s="41">
-        <v>0.52798739219405399</v>
-      </c>
-      <c r="L27" s="41">
-        <v>0.88908131752518804</v>
-      </c>
-      <c r="M27" s="41">
-        <v>0.93999240479022494</v>
-      </c>
-      <c r="N27" s="42">
-        <v>2.3933667898394601E-2</v>
-      </c>
-      <c r="O27" s="42">
-        <v>4.2602221911121202E-2</v>
-      </c>
+      <c r="K27" s="45"/>
+      <c r="L27" s="45"/>
+      <c r="M27" s="45"/>
+      <c r="N27" s="46"/>
+      <c r="O27" s="46"/>
       <c r="Q27" s="41"/>
       <c r="R27" s="41"/>
       <c r="S27" s="41"/>
     </row>
-    <row r="28" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="53" t="s">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F28" s="41"/>
+      <c r="G28" s="41"/>
+      <c r="H28" s="41"/>
+      <c r="K28" s="45"/>
+      <c r="L28" s="45"/>
+      <c r="M28" s="45"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="46"/>
+      <c r="Q28" s="41"/>
+      <c r="R28" s="41"/>
+      <c r="S28" s="41"/>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F29" s="41"/>
+      <c r="G29" s="41"/>
+      <c r="H29" s="41"/>
+      <c r="K29" s="41"/>
+      <c r="L29" s="41"/>
+      <c r="M29" s="41"/>
+      <c r="N29" s="41"/>
+      <c r="O29" s="41"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="6"/>
+      <c r="S29" s="6"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" t="s">
+        <v>137</v>
+      </c>
+      <c r="C30" t="s">
+        <v>144</v>
+      </c>
+      <c r="F30" s="41"/>
+      <c r="G30" s="41"/>
+      <c r="H30" s="41"/>
+      <c r="K30" s="41">
+        <v>0.52798739219405399</v>
+      </c>
+      <c r="L30" s="41">
+        <v>0.88908131752518804</v>
+      </c>
+      <c r="M30" s="41">
+        <v>0.93999240479022494</v>
+      </c>
+      <c r="N30" s="42">
+        <v>2.3933667898394601E-2</v>
+      </c>
+      <c r="O30" s="42">
+        <v>4.2602221911121202E-2</v>
+      </c>
+      <c r="Q30" s="41"/>
+      <c r="R30" s="41"/>
+      <c r="S30" s="41"/>
+    </row>
+    <row r="31" spans="1:21" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="53" t="s">
         <v>134</v>
       </c>
-      <c r="B28" s="53" t="s">
+      <c r="B31" s="53" t="s">
         <v>135</v>
       </c>
-      <c r="C28" s="53" t="s">
+      <c r="C31" s="53" t="s">
         <v>144</v>
       </c>
-      <c r="F28" s="54">
+      <c r="F31" s="54">
         <v>0.34893247055384802</v>
       </c>
-      <c r="G28" s="54">
+      <c r="G31" s="54">
         <v>0.67317502542262897</v>
       </c>
-      <c r="H28" s="54">
+      <c r="H31" s="54">
         <v>0.84248623447175797</v>
       </c>
-      <c r="I28" s="53">
+      <c r="I31" s="53">
         <v>0.103582492198157</v>
       </c>
-      <c r="J28" s="53">
+      <c r="J31" s="53">
         <v>0.110216817388472</v>
       </c>
-      <c r="K28" s="55">
+      <c r="K31" s="55">
         <v>0.40407461052249199</v>
       </c>
-      <c r="L28" s="55">
+      <c r="L31" s="55">
         <v>0.78409109272143296</v>
       </c>
-      <c r="M28" s="55">
+      <c r="M31" s="55">
         <v>0.88931404963882599</v>
       </c>
-      <c r="N28" s="56">
+      <c r="N31" s="56">
         <v>4.0847215751155602E-2</v>
       </c>
-      <c r="O28" s="56">
+      <c r="O31" s="56">
         <v>5.2182795027841303E-2</v>
       </c>
-      <c r="Q28" s="54">
+      <c r="Q31" s="54">
         <v>0.60047364223300004</v>
       </c>
-      <c r="R28" s="54">
+      <c r="R31" s="54">
         <v>0.74598242392985104</v>
       </c>
-      <c r="S28" s="54">
+      <c r="S31" s="54">
         <v>0.94286147483809202</v>
       </c>
-      <c r="T28" s="53">
+      <c r="T31" s="53">
         <v>4.9549475900016203E-2</v>
       </c>
-      <c r="U28" s="53">
+      <c r="U31" s="53">
         <v>5.6839456085560298E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F29" s="67"/>
-      <c r="G29" s="67"/>
-      <c r="H29" s="67"/>
-      <c r="K29" s="69"/>
-      <c r="L29" s="69"/>
-      <c r="M29" s="69"/>
-      <c r="N29" s="70"/>
-      <c r="O29" s="70"/>
-      <c r="Q29" s="67"/>
-      <c r="R29" s="67"/>
-      <c r="S29" s="67"/>
-    </row>
-    <row r="30" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F30" s="67"/>
-      <c r="G30" s="67"/>
-      <c r="H30" s="67"/>
-      <c r="K30" s="69"/>
-      <c r="L30" s="69"/>
-      <c r="M30" s="69"/>
-      <c r="N30" s="70"/>
-      <c r="O30" s="70"/>
-      <c r="Q30" s="67"/>
-      <c r="R30" s="67"/>
-      <c r="S30" s="67"/>
-    </row>
-    <row r="31" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="67"/>
-      <c r="G31" s="67"/>
-      <c r="H31" s="67"/>
-      <c r="K31" s="1" t="s">
+    <row r="32" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="67"/>
+      <c r="G32" s="67"/>
+      <c r="H32" s="67"/>
+      <c r="K32" s="69"/>
+      <c r="L32" s="69"/>
+      <c r="M32" s="69"/>
+      <c r="N32" s="70"/>
+      <c r="O32" s="70"/>
+      <c r="Q32" s="67"/>
+      <c r="R32" s="67"/>
+      <c r="S32" s="67"/>
+    </row>
+    <row r="33" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F33" s="67"/>
+      <c r="G33" s="67"/>
+      <c r="H33" s="67"/>
+      <c r="K33" s="69"/>
+      <c r="L33" s="69"/>
+      <c r="M33" s="69"/>
+      <c r="N33" s="70"/>
+      <c r="O33" s="70"/>
+      <c r="Q33" s="67"/>
+      <c r="R33" s="67"/>
+      <c r="S33" s="67"/>
+    </row>
+    <row r="34" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="28" t="s">
+        <v>152</v>
+      </c>
+      <c r="F34" s="67"/>
+      <c r="G34" s="67"/>
+      <c r="H34" s="67"/>
+      <c r="K34" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="70"/>
-      <c r="O31" s="70"/>
-      <c r="Q31" s="67"/>
-      <c r="R31" s="67"/>
-      <c r="S31" s="67"/>
-    </row>
-    <row r="32" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="36" t="s">
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="70"/>
+      <c r="O34" s="70"/>
+      <c r="Q34" s="67"/>
+      <c r="R34" s="67"/>
+      <c r="S34" s="67"/>
+    </row>
+    <row r="35" spans="1:21" s="36" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="36" t="s">
         <v>148</v>
       </c>
-      <c r="K32" s="8" t="s">
+      <c r="K35" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L32" s="8" t="s">
+      <c r="L35" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="M32" s="71"/>
-    </row>
-    <row r="33" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="28" t="s">
+      <c r="M35" s="71"/>
+    </row>
+    <row r="36" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B36" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C36" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E36" s="28" t="s">
         <v>149</v>
       </c>
-      <c r="K33" s="28">
+      <c r="K36" s="28">
         <v>0.49995137507486298</v>
       </c>
-      <c r="L33" s="28">
+      <c r="L36" s="28">
         <v>0.88200590665096601</v>
       </c>
-      <c r="M33" s="28">
+      <c r="M36" s="28">
         <v>0.95620694227470504</v>
       </c>
-      <c r="O33" s="28">
+      <c r="O36" s="28">
         <v>1.7895665044541001E-2</v>
       </c>
     </row>
-    <row r="34" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="28" t="s">
+    <row r="37" spans="1:21" s="28" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="28" t="s">
         <v>138</v>
       </c>
-      <c r="B34" s="28" t="s">
+      <c r="B37" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C37" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E34" s="28" t="s">
+      <c r="E37" s="28" t="s">
         <v>150</v>
       </c>
-      <c r="F34" s="28">
+      <c r="F37" s="28">
         <v>0.35273594851526402</v>
       </c>
-      <c r="G34" s="28">
+      <c r="G37" s="28">
         <v>0.78617779613900696</v>
       </c>
-      <c r="H34" s="28">
+      <c r="H37" s="28">
         <v>0.89320226496106903</v>
       </c>
-      <c r="J34" s="28">
+      <c r="J37" s="28">
         <v>5.1299052617878399E-2</v>
       </c>
-      <c r="K34" s="28">
+      <c r="K37" s="28">
         <v>0.42935275192161299</v>
       </c>
-      <c r="L34" s="28">
+      <c r="L37" s="28">
         <v>0.82282910372960305</v>
       </c>
-      <c r="M34" s="28">
+      <c r="M37" s="28">
         <v>0.92870785302355496</v>
       </c>
-      <c r="O34" s="28">
+      <c r="O37" s="28">
         <v>2.2637682752899499E-2</v>
       </c>
-      <c r="Q34" s="28">
+      <c r="Q37" s="28">
         <v>0.62031515141027105</v>
       </c>
-      <c r="R34" s="28">
+      <c r="R37" s="28">
         <v>0.86300522966999405</v>
       </c>
-      <c r="S34" s="28">
+      <c r="S37" s="28">
         <v>0.97016478340557599</v>
       </c>
-      <c r="U34" s="28">
+      <c r="U37" s="28">
         <v>2.65183782934416E-2</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F37" s="11">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F40" s="11">
         <v>0.40029999999999999</v>
       </c>
-      <c r="G37" s="11">
+      <c r="G40" s="11">
         <v>0.86060000000000003</v>
       </c>
-      <c r="H37" s="11">
+      <c r="H40" s="11">
         <v>0.93940000000000001</v>
       </c>
-      <c r="K37" s="11">
+      <c r="K40" s="11">
         <v>0.46189999999999998</v>
       </c>
-      <c r="L37" s="11">
+      <c r="L40" s="11">
         <v>0.87009999999999998</v>
       </c>
-      <c r="M37" s="11">
+      <c r="M40" s="11">
         <v>0.95009999999999994</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="Q40" s="11">
         <v>0.63870000000000005</v>
       </c>
-      <c r="R37" s="11">
+      <c r="R40" s="11">
         <v>0.9052</v>
       </c>
-      <c r="S37" s="11">
+      <c r="S40" s="11">
         <v>0.98019999999999996</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F38" s="13">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F41" s="13">
         <v>0.41099999999999998</v>
       </c>
-      <c r="G38" s="13">
+      <c r="G41" s="13">
         <v>0.86070000000000002</v>
       </c>
-      <c r="H38" s="13">
+      <c r="H41" s="13">
         <v>0.93859999999999999</v>
       </c>
-      <c r="K38" s="13">
+      <c r="K41" s="13">
         <v>0.48020000000000002</v>
       </c>
-      <c r="L38" s="13">
+      <c r="L41" s="13">
         <v>0.8649</v>
       </c>
-      <c r="M38" s="13">
+      <c r="M41" s="13">
         <v>0.95309999999999995</v>
       </c>
-      <c r="Q38" s="13">
+      <c r="Q41" s="13">
         <v>0.64639999999999997</v>
       </c>
-      <c r="R38" s="13">
+      <c r="R41" s="13">
         <v>0.90239999999999998</v>
       </c>
-      <c r="S38" s="13">
+      <c r="S41" s="13">
         <v>0.97989999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F39" s="6">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F42" s="6">
         <v>0.40579999999999999</v>
       </c>
-      <c r="G39" s="6">
+      <c r="G42" s="6">
         <v>0.85680000000000001</v>
       </c>
-      <c r="H39" s="6">
+      <c r="H42" s="6">
         <v>0.9385</v>
       </c>
-      <c r="K39" s="6">
+      <c r="K42" s="6">
         <v>0.47460000000000002</v>
       </c>
-      <c r="L39" s="6">
+      <c r="L42" s="6">
         <v>0.85680000000000001</v>
       </c>
-      <c r="M39" s="6">
+      <c r="M42" s="6">
         <v>0.95009999999999994</v>
       </c>
-      <c r="Q39" s="6">
+      <c r="Q42" s="6">
         <v>0.64170000000000005</v>
       </c>
-      <c r="R39" s="6">
+      <c r="R42" s="6">
         <v>0.90990000000000004</v>
       </c>
-      <c r="S39" s="6">
+      <c r="S42" s="6">
         <v>0.98119999999999996</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="F40" s="3">
+    <row r="43" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="F43" s="3">
         <v>0.40339999999999998</v>
       </c>
-      <c r="G40" s="3">
+      <c r="G43" s="3">
         <v>0.86080000000000001</v>
       </c>
-      <c r="H40" s="3">
+      <c r="H43" s="3">
         <v>0.93899999999999995</v>
       </c>
-      <c r="K40" s="3">
+      <c r="K43" s="3">
         <v>0.48170000000000002</v>
       </c>
-      <c r="L40" s="3">
+      <c r="L43" s="3">
         <v>0.88090000000000002</v>
       </c>
-      <c r="M40" s="3">
+      <c r="M43" s="3">
         <v>0.95499999999999996</v>
       </c>
-      <c r="Q40" s="3">
+      <c r="Q43" s="3">
         <v>0.64019999999999999</v>
       </c>
-      <c r="R40" s="3">
+      <c r="R43" s="3">
         <v>0.90200000000000002</v>
       </c>
-      <c r="S40" s="3">
+      <c r="S43" s="3">
         <v>0.98050000000000004</v>
       </c>
     </row>

</xml_diff>